<commit_message>
Justering protokoll - tog bort senio i namnet eftersom young vaulter också anv det.
</commit_message>
<xml_diff>
--- a/mallar/Protokoll/Protokoll 2019 individuell klass_(mall).xlsx
+++ b/mallar/Protokoll/Protokoll 2019 individuell klass_(mall).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\episerver\voltige\VoltigeClosedXML\mallar\Protokoll\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F36A6316-7967-4152-BD71-22C76821E564}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6783E5B1-67EC-4B99-B4AA-7EDBD2056315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" tabRatio="966" firstSheet="10" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43080" yWindow="8820" windowWidth="29040" windowHeight="17640" tabRatio="966" firstSheet="6" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="37" r:id="rId1"/>
@@ -163,7 +163,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="779" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="779" uniqueCount="185">
   <si>
     <t>Nation:</t>
   </si>
@@ -710,9 +710,6 @@
   </si>
   <si>
     <t>Individuell kür junior</t>
-  </si>
-  <si>
-    <t>Individuell kür senior</t>
   </si>
   <si>
     <t>Individuell kür minior</t>
@@ -2957,6 +2954,179 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="14" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="61" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="45" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="55" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="56" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="58" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="59" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="60" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="62" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="58" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="172" fontId="2" fillId="3" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="172" fontId="2" fillId="3" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="57" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="59" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="45" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="58" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="59" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="40" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="28" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="40" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="41" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="53" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="50" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="45" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="55" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="56" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="58" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="59" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="23" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="43" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="46" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
@@ -2965,173 +3135,6 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="40" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="28" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="40" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="41" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="53" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="50" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="45" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="55" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="56" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="58" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="59" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="23" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="43" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="57" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="46" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="14" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="61" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="45" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="55" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="56" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="58" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="59" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="60" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="62" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="58" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="172" fontId="2" fillId="3" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="172" fontId="2" fillId="3" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="59" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="45" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="58" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="59" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3298,12 +3301,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3719,12 +3716,12 @@
     </row>
     <row r="4" spans="1:6" s="242" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="242" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="279" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="279" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="242" customFormat="1" x14ac:dyDescent="0.35"/>
@@ -3792,10 +3789,10 @@
         <v>83</v>
       </c>
       <c r="C18" s="209" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D18" s="209" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E18" s="216"/>
       <c r="F18" s="209" t="s">
@@ -3836,7 +3833,7 @@
         <v>83</v>
       </c>
       <c r="G20" s="209" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H20" s="209" t="s">
         <v>84</v>
@@ -3870,7 +3867,7 @@
         <v>83</v>
       </c>
       <c r="G22" s="209" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H22" s="209" t="s">
         <v>84</v>
@@ -3918,7 +3915,7 @@
         <v>83</v>
       </c>
       <c r="C25" s="209" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D25" s="209" t="s">
         <v>84</v>
@@ -3950,7 +3947,7 @@
         <v>83</v>
       </c>
       <c r="G27" s="209" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H27" s="209" t="s">
         <v>84</v>
@@ -4019,13 +4016,13 @@
         <v>83</v>
       </c>
       <c r="C33" s="209" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D33" s="209" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E33" s="209" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F33" s="209" t="s">
         <v>83</v>
@@ -4071,13 +4068,13 @@
         <v>83</v>
       </c>
       <c r="G35" s="209" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H35" s="209" t="s">
         <v>84</v>
       </c>
       <c r="I35" s="209" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -4111,13 +4108,13 @@
         <v>83</v>
       </c>
       <c r="G37" s="209" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H37" s="209" t="s">
         <v>84</v>
       </c>
       <c r="I37" s="209" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="38" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -4168,13 +4165,13 @@
         <v>83</v>
       </c>
       <c r="C40" s="209" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D40" s="209" t="s">
         <v>84</v>
       </c>
       <c r="E40" s="209" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.35">
@@ -4203,13 +4200,13 @@
         <v>83</v>
       </c>
       <c r="G42" s="209" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H42" s="209" t="s">
         <v>84</v>
       </c>
       <c r="I42" s="209" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="43" spans="1:14" ht="25.5" x14ac:dyDescent="0.35">
@@ -4310,10 +4307,10 @@
         <v>83</v>
       </c>
       <c r="C50" s="209" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D50" s="209" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E50" s="216"/>
       <c r="F50" s="209" t="s">
@@ -4329,10 +4326,10 @@
         <v>83</v>
       </c>
       <c r="K50" s="209" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L50" s="209" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="M50" s="216"/>
       <c r="N50" s="209" t="s">
@@ -4380,7 +4377,7 @@
         <v>83</v>
       </c>
       <c r="G52" s="209" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H52" s="209" t="s">
         <v>84</v>
@@ -4399,7 +4396,7 @@
         <v>83</v>
       </c>
       <c r="O52" s="209" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="P52" s="209" t="s">
         <v>84</v>
@@ -4440,7 +4437,7 @@
         <v>83</v>
       </c>
       <c r="G54" s="209" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H54" s="209" t="s">
         <v>84</v>
@@ -4459,7 +4456,7 @@
         <v>83</v>
       </c>
       <c r="O54" s="209" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="P54" s="209" t="s">
         <v>84</v>
@@ -4500,7 +4497,7 @@
         <v>83</v>
       </c>
       <c r="G56" s="209" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H56" s="209" t="s">
         <v>84</v>
@@ -4519,7 +4516,7 @@
         <v>83</v>
       </c>
       <c r="O56" s="209" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="P56" s="209" t="s">
         <v>84</v>
@@ -4611,13 +4608,13 @@
         <v>83</v>
       </c>
       <c r="C63" s="209" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D63" s="209" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E63" s="209" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F63" s="209" t="s">
         <v>83</v>
@@ -4635,13 +4632,13 @@
         <v>83</v>
       </c>
       <c r="K63" s="209" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="L63" s="209" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="M63" s="209" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="N63" s="209" t="s">
         <v>83</v>
@@ -4695,13 +4692,13 @@
         <v>83</v>
       </c>
       <c r="G65" s="209" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H65" s="209" t="s">
         <v>84</v>
       </c>
       <c r="I65" s="209" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J65" s="209" t="s">
         <v>83</v>
@@ -4719,13 +4716,13 @@
         <v>83</v>
       </c>
       <c r="O65" s="209" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="P65" s="209" t="s">
         <v>84</v>
       </c>
       <c r="Q65" s="209" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="66" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -4767,13 +4764,13 @@
         <v>83</v>
       </c>
       <c r="G67" s="209" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H67" s="209" t="s">
         <v>84</v>
       </c>
       <c r="I67" s="209" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J67" s="209" t="s">
         <v>83</v>
@@ -4791,13 +4788,13 @@
         <v>83</v>
       </c>
       <c r="O67" s="209" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="P67" s="209" t="s">
         <v>84</v>
       </c>
       <c r="Q67" s="209" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="68" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
@@ -4839,13 +4836,13 @@
         <v>83</v>
       </c>
       <c r="G69" s="209" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H69" s="209" t="s">
         <v>84</v>
       </c>
       <c r="I69" s="209" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J69" s="209" t="s">
         <v>83</v>
@@ -4863,13 +4860,13 @@
         <v>83</v>
       </c>
       <c r="O69" s="209" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="P69" s="209" t="s">
         <v>84</v>
       </c>
       <c r="Q69" s="209" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="73" spans="1:17" s="242" customFormat="1" ht="17.25" x14ac:dyDescent="0.45">
@@ -4928,7 +4925,7 @@
         <v>103</v>
       </c>
       <c r="D76" s="249" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E76" s="243" t="s">
         <v>105</v>
@@ -4948,7 +4945,7 @@
         <v>103</v>
       </c>
       <c r="D77" s="249" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E77" s="243" t="s">
         <v>105</v>
@@ -5061,7 +5058,7 @@
   </sheetPr>
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView showZeros="0" view="pageLayout" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showZeros="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B15" sqref="B15:I15"/>
     </sheetView>
   </sheetViews>
@@ -5696,10 +5693,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="11"/>
-      <c r="C5" s="367"/>
-      <c r="D5" s="367"/>
-      <c r="E5" s="367"/>
-      <c r="F5" s="367"/>
+      <c r="C5" s="369"/>
+      <c r="D5" s="369"/>
+      <c r="E5" s="369"/>
+      <c r="F5" s="369"/>
       <c r="H5" s="13"/>
       <c r="I5" s="14" t="s">
         <v>11</v>
@@ -5713,10 +5710,10 @@
         <v>8</v>
       </c>
       <c r="B6" s="11"/>
-      <c r="C6" s="367"/>
-      <c r="D6" s="367"/>
-      <c r="E6" s="367"/>
-      <c r="F6" s="367"/>
+      <c r="C6" s="369"/>
+      <c r="D6" s="369"/>
+      <c r="E6" s="369"/>
+      <c r="F6" s="369"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -5745,30 +5742,30 @@
         <v>0</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="368"/>
-      <c r="D8" s="368"/>
-      <c r="E8" s="368"/>
-      <c r="F8" s="368"/>
+      <c r="C8" s="370"/>
+      <c r="D8" s="370"/>
+      <c r="E8" s="370"/>
+      <c r="F8" s="370"/>
     </row>
     <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="11"/>
-      <c r="C9" s="367"/>
-      <c r="D9" s="367"/>
-      <c r="E9" s="367"/>
-      <c r="F9" s="367"/>
+      <c r="C9" s="369"/>
+      <c r="D9" s="369"/>
+      <c r="E9" s="369"/>
+      <c r="F9" s="369"/>
     </row>
     <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="11"/>
-      <c r="C10" s="367"/>
-      <c r="D10" s="367"/>
-      <c r="E10" s="367"/>
-      <c r="F10" s="367"/>
+      <c r="C10" s="369"/>
+      <c r="D10" s="369"/>
+      <c r="E10" s="369"/>
+      <c r="F10" s="369"/>
     </row>
     <row r="11" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -5781,19 +5778,19 @@
       </c>
     </row>
     <row r="14" spans="1:12" ht="59.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="376" t="s">
-        <v>164</v>
-      </c>
-      <c r="B14" s="378" t="s">
+      <c r="A14" s="378" t="s">
+        <v>163</v>
+      </c>
+      <c r="B14" s="380" t="s">
         <v>114</v>
       </c>
-      <c r="C14" s="379"/>
-      <c r="D14" s="379"/>
-      <c r="E14" s="379"/>
-      <c r="F14" s="379"/>
-      <c r="G14" s="379"/>
-      <c r="H14" s="379"/>
-      <c r="I14" s="380"/>
+      <c r="C14" s="381"/>
+      <c r="D14" s="381"/>
+      <c r="E14" s="381"/>
+      <c r="F14" s="381"/>
+      <c r="G14" s="381"/>
+      <c r="H14" s="381"/>
+      <c r="I14" s="382"/>
       <c r="J14" s="18" t="s">
         <v>122</v>
       </c>
@@ -5806,17 +5803,17 @@
       </c>
     </row>
     <row r="15" spans="1:12" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="389"/>
-      <c r="B15" s="381" t="s">
-        <v>182</v>
-      </c>
-      <c r="C15" s="382"/>
-      <c r="D15" s="382"/>
-      <c r="E15" s="382"/>
-      <c r="F15" s="382"/>
-      <c r="G15" s="382"/>
-      <c r="H15" s="382"/>
-      <c r="I15" s="382"/>
+      <c r="A15" s="391"/>
+      <c r="B15" s="383" t="s">
+        <v>181</v>
+      </c>
+      <c r="C15" s="384"/>
+      <c r="D15" s="384"/>
+      <c r="E15" s="384"/>
+      <c r="F15" s="384"/>
+      <c r="G15" s="384"/>
+      <c r="H15" s="384"/>
+      <c r="I15" s="384"/>
       <c r="J15" s="20" t="s">
         <v>123</v>
       </c>
@@ -5829,21 +5826,21 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="85.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="376" t="s">
-        <v>165</v>
-      </c>
-      <c r="B16" s="385" t="s">
-        <v>155</v>
-      </c>
-      <c r="C16" s="386"/>
-      <c r="D16" s="386"/>
-      <c r="E16" s="386"/>
-      <c r="F16" s="386"/>
-      <c r="G16" s="386"/>
-      <c r="H16" s="386"/>
-      <c r="I16" s="386"/>
+      <c r="A16" s="378" t="s">
+        <v>164</v>
+      </c>
+      <c r="B16" s="387" t="s">
+        <v>154</v>
+      </c>
+      <c r="C16" s="388"/>
+      <c r="D16" s="388"/>
+      <c r="E16" s="388"/>
+      <c r="F16" s="388"/>
+      <c r="G16" s="388"/>
+      <c r="H16" s="388"/>
+      <c r="I16" s="388"/>
       <c r="J16" s="18" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K16" s="270">
         <v>0</v>
@@ -5854,19 +5851,19 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="377"/>
-      <c r="B17" s="387" t="s">
-        <v>156</v>
-      </c>
-      <c r="C17" s="388"/>
-      <c r="D17" s="388"/>
-      <c r="E17" s="388"/>
-      <c r="F17" s="388"/>
-      <c r="G17" s="388"/>
-      <c r="H17" s="388"/>
-      <c r="I17" s="388"/>
+      <c r="A17" s="379"/>
+      <c r="B17" s="389" t="s">
+        <v>155</v>
+      </c>
+      <c r="C17" s="390"/>
+      <c r="D17" s="390"/>
+      <c r="E17" s="390"/>
+      <c r="F17" s="390"/>
+      <c r="G17" s="390"/>
+      <c r="H17" s="390"/>
+      <c r="I17" s="390"/>
       <c r="J17" s="19" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K17" s="271">
         <v>0</v>
@@ -6595,7 +6592,7 @@
     <row r="1" spans="1:12" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="50" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H2" s="13"/>
       <c r="I2" s="14" t="s">
@@ -6639,10 +6636,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="11"/>
-      <c r="C5" s="367"/>
-      <c r="D5" s="367"/>
-      <c r="E5" s="367"/>
-      <c r="F5" s="367"/>
+      <c r="C5" s="369"/>
+      <c r="D5" s="369"/>
+      <c r="E5" s="369"/>
+      <c r="F5" s="369"/>
       <c r="H5" s="13"/>
       <c r="I5" s="14" t="s">
         <v>11</v>
@@ -6656,10 +6653,10 @@
         <v>8</v>
       </c>
       <c r="B6" s="11"/>
-      <c r="C6" s="367"/>
-      <c r="D6" s="367"/>
-      <c r="E6" s="367"/>
-      <c r="F6" s="367"/>
+      <c r="C6" s="369"/>
+      <c r="D6" s="369"/>
+      <c r="E6" s="369"/>
+      <c r="F6" s="369"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -6688,30 +6685,30 @@
         <v>0</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="368"/>
-      <c r="D8" s="368"/>
-      <c r="E8" s="368"/>
-      <c r="F8" s="368"/>
+      <c r="C8" s="370"/>
+      <c r="D8" s="370"/>
+      <c r="E8" s="370"/>
+      <c r="F8" s="370"/>
     </row>
     <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="11"/>
-      <c r="C9" s="367"/>
-      <c r="D9" s="367"/>
-      <c r="E9" s="367"/>
-      <c r="F9" s="367"/>
+      <c r="C9" s="369"/>
+      <c r="D9" s="369"/>
+      <c r="E9" s="369"/>
+      <c r="F9" s="369"/>
     </row>
     <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="11"/>
-      <c r="C10" s="367"/>
-      <c r="D10" s="367"/>
-      <c r="E10" s="367"/>
-      <c r="F10" s="367"/>
+      <c r="C10" s="369"/>
+      <c r="D10" s="369"/>
+      <c r="E10" s="369"/>
+      <c r="F10" s="369"/>
     </row>
     <row r="11" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -6724,19 +6721,19 @@
       </c>
     </row>
     <row r="14" spans="1:12" ht="59.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="376" t="s">
-        <v>164</v>
-      </c>
-      <c r="B14" s="378" t="s">
+      <c r="A14" s="378" t="s">
+        <v>163</v>
+      </c>
+      <c r="B14" s="380" t="s">
         <v>114</v>
       </c>
-      <c r="C14" s="379"/>
-      <c r="D14" s="379"/>
-      <c r="E14" s="379"/>
-      <c r="F14" s="379"/>
-      <c r="G14" s="379"/>
-      <c r="H14" s="379"/>
-      <c r="I14" s="380"/>
+      <c r="C14" s="381"/>
+      <c r="D14" s="381"/>
+      <c r="E14" s="381"/>
+      <c r="F14" s="381"/>
+      <c r="G14" s="381"/>
+      <c r="H14" s="381"/>
+      <c r="I14" s="382"/>
       <c r="J14" s="18" t="s">
         <v>122</v>
       </c>
@@ -6749,17 +6746,17 @@
       </c>
     </row>
     <row r="15" spans="1:12" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="389"/>
-      <c r="B15" s="381" t="s">
-        <v>182</v>
-      </c>
-      <c r="C15" s="382"/>
-      <c r="D15" s="382"/>
-      <c r="E15" s="382"/>
-      <c r="F15" s="382"/>
-      <c r="G15" s="382"/>
-      <c r="H15" s="382"/>
-      <c r="I15" s="382"/>
+      <c r="A15" s="391"/>
+      <c r="B15" s="383" t="s">
+        <v>181</v>
+      </c>
+      <c r="C15" s="384"/>
+      <c r="D15" s="384"/>
+      <c r="E15" s="384"/>
+      <c r="F15" s="384"/>
+      <c r="G15" s="384"/>
+      <c r="H15" s="384"/>
+      <c r="I15" s="384"/>
       <c r="J15" s="20" t="s">
         <v>123</v>
       </c>
@@ -6772,21 +6769,21 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="85.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="376" t="s">
-        <v>165</v>
-      </c>
-      <c r="B16" s="385" t="s">
-        <v>155</v>
-      </c>
-      <c r="C16" s="386"/>
-      <c r="D16" s="386"/>
-      <c r="E16" s="386"/>
-      <c r="F16" s="386"/>
-      <c r="G16" s="386"/>
-      <c r="H16" s="386"/>
-      <c r="I16" s="386"/>
+      <c r="A16" s="378" t="s">
+        <v>164</v>
+      </c>
+      <c r="B16" s="387" t="s">
+        <v>154</v>
+      </c>
+      <c r="C16" s="388"/>
+      <c r="D16" s="388"/>
+      <c r="E16" s="388"/>
+      <c r="F16" s="388"/>
+      <c r="G16" s="388"/>
+      <c r="H16" s="388"/>
+      <c r="I16" s="388"/>
       <c r="J16" s="18" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K16" s="270">
         <v>0</v>
@@ -6797,19 +6794,19 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="377"/>
-      <c r="B17" s="387" t="s">
-        <v>156</v>
-      </c>
-      <c r="C17" s="388"/>
-      <c r="D17" s="388"/>
-      <c r="E17" s="388"/>
-      <c r="F17" s="388"/>
-      <c r="G17" s="388"/>
-      <c r="H17" s="388"/>
-      <c r="I17" s="388"/>
+      <c r="A17" s="379"/>
+      <c r="B17" s="389" t="s">
+        <v>155</v>
+      </c>
+      <c r="C17" s="390"/>
+      <c r="D17" s="390"/>
+      <c r="E17" s="390"/>
+      <c r="F17" s="390"/>
+      <c r="G17" s="390"/>
+      <c r="H17" s="390"/>
+      <c r="I17" s="390"/>
       <c r="J17" s="19" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K17" s="271">
         <v>0</v>
@@ -6920,17 +6917,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="C10:F10"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="B14:I14"/>
     <mergeCell ref="B15:I15"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="B16:I16"/>
     <mergeCell ref="B17:I17"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C10:F10"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7014,10 +7011,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="11"/>
-      <c r="C5" s="367"/>
-      <c r="D5" s="367"/>
-      <c r="E5" s="367"/>
-      <c r="F5" s="367"/>
+      <c r="C5" s="369"/>
+      <c r="D5" s="369"/>
+      <c r="E5" s="369"/>
+      <c r="F5" s="369"/>
       <c r="H5" s="13"/>
       <c r="I5" s="14" t="s">
         <v>11</v>
@@ -7031,10 +7028,10 @@
         <v>8</v>
       </c>
       <c r="B6" s="11"/>
-      <c r="C6" s="367"/>
-      <c r="D6" s="367"/>
-      <c r="E6" s="367"/>
-      <c r="F6" s="367"/>
+      <c r="C6" s="369"/>
+      <c r="D6" s="369"/>
+      <c r="E6" s="369"/>
+      <c r="F6" s="369"/>
       <c r="K6" s="30"/>
     </row>
     <row r="7" spans="1:12" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -7057,30 +7054,30 @@
         <v>0</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="368"/>
-      <c r="D8" s="368"/>
-      <c r="E8" s="368"/>
-      <c r="F8" s="368"/>
+      <c r="C8" s="370"/>
+      <c r="D8" s="370"/>
+      <c r="E8" s="370"/>
+      <c r="F8" s="370"/>
     </row>
     <row r="9" spans="1:12" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="11"/>
-      <c r="C9" s="367"/>
-      <c r="D9" s="367"/>
-      <c r="E9" s="367"/>
-      <c r="F9" s="367"/>
+      <c r="C9" s="369"/>
+      <c r="D9" s="369"/>
+      <c r="E9" s="369"/>
+      <c r="F9" s="369"/>
     </row>
     <row r="10" spans="1:12" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="11"/>
-      <c r="C10" s="367"/>
-      <c r="D10" s="367"/>
-      <c r="E10" s="367"/>
-      <c r="F10" s="367"/>
+      <c r="C10" s="369"/>
+      <c r="D10" s="369"/>
+      <c r="E10" s="369"/>
+      <c r="F10" s="369"/>
     </row>
     <row r="11" spans="1:12" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:12" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -7106,14 +7103,14 @@
       </c>
     </row>
     <row r="15" spans="1:12" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="390" t="s">
-        <v>150</v>
-      </c>
-      <c r="B15" s="391"/>
-      <c r="C15" s="391"/>
-      <c r="D15" s="391"/>
-      <c r="E15" s="391"/>
-      <c r="F15" s="392"/>
+      <c r="A15" s="392" t="s">
+        <v>149</v>
+      </c>
+      <c r="B15" s="393"/>
+      <c r="C15" s="393"/>
+      <c r="D15" s="393"/>
+      <c r="E15" s="393"/>
+      <c r="F15" s="394"/>
       <c r="G15" s="33"/>
       <c r="H15" s="33"/>
       <c r="I15" s="11"/>
@@ -7122,14 +7119,14 @@
       <c r="L15" s="263"/>
     </row>
     <row r="16" spans="1:12" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="390" t="s">
-        <v>183</v>
-      </c>
-      <c r="B16" s="391"/>
-      <c r="C16" s="391"/>
-      <c r="D16" s="391"/>
-      <c r="E16" s="391"/>
-      <c r="F16" s="392"/>
+      <c r="A16" s="392" t="s">
+        <v>182</v>
+      </c>
+      <c r="B16" s="393"/>
+      <c r="C16" s="393"/>
+      <c r="D16" s="393"/>
+      <c r="E16" s="393"/>
+      <c r="F16" s="394"/>
       <c r="G16" s="33"/>
       <c r="H16" s="33"/>
       <c r="I16" s="11"/>
@@ -7139,7 +7136,7 @@
     </row>
     <row r="17" spans="1:18" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="225" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B17" s="88"/>
       <c r="C17" s="88"/>
@@ -7190,27 +7187,27 @@
       <c r="L20" s="140"/>
     </row>
     <row r="21" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="396" t="s">
+      <c r="A21" s="398" t="s">
         <v>72</v>
       </c>
-      <c r="B21" s="397"/>
-      <c r="C21" s="397"/>
-      <c r="D21" s="397"/>
-      <c r="E21" s="397"/>
-      <c r="F21" s="397"/>
-      <c r="G21" s="397"/>
-      <c r="H21" s="397"/>
-      <c r="I21" s="397"/>
+      <c r="B21" s="399"/>
+      <c r="C21" s="399"/>
+      <c r="D21" s="399"/>
+      <c r="E21" s="399"/>
+      <c r="F21" s="399"/>
+      <c r="G21" s="399"/>
+      <c r="H21" s="399"/>
+      <c r="I21" s="399"/>
       <c r="J21" s="139"/>
       <c r="K21" s="138"/>
       <c r="L21" s="8"/>
       <c r="R21" s="133"/>
     </row>
     <row r="22" spans="1:18" ht="66" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="404" t="s">
+      <c r="A22" s="406" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="405"/>
+      <c r="B22" s="407"/>
       <c r="C22" s="137"/>
       <c r="D22" s="137"/>
       <c r="E22" s="137"/>
@@ -7224,15 +7221,15 @@
       <c r="R22" s="133"/>
     </row>
     <row r="23" spans="1:18" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="400" t="s">
+      <c r="A23" s="402" t="s">
         <v>60</v>
       </c>
-      <c r="B23" s="401"/>
+      <c r="B23" s="403"/>
       <c r="C23" s="272"/>
-      <c r="D23" s="398" t="s">
+      <c r="D23" s="400" t="s">
         <v>52</v>
       </c>
-      <c r="E23" s="399"/>
+      <c r="E23" s="401"/>
       <c r="F23" s="273"/>
       <c r="G23" s="232" t="s">
         <v>71</v>
@@ -7255,11 +7252,11 @@
       <c r="R23" s="133"/>
     </row>
     <row r="24" spans="1:18" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="402" t="s">
+      <c r="A24" s="404" t="s">
         <v>14</v>
       </c>
-      <c r="B24" s="403"/>
-      <c r="C24" s="403"/>
+      <c r="B24" s="405"/>
+      <c r="C24" s="405"/>
       <c r="D24" s="236"/>
       <c r="E24" s="236"/>
       <c r="F24" s="236"/>
@@ -7271,19 +7268,19 @@
       <c r="R24" s="133"/>
     </row>
     <row r="25" spans="1:18" ht="16.350000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="393" t="s">
+      <c r="A25" s="395" t="s">
         <v>62</v>
       </c>
-      <c r="B25" s="394"/>
-      <c r="C25" s="394"/>
-      <c r="D25" s="394"/>
-      <c r="E25" s="394"/>
-      <c r="F25" s="394"/>
-      <c r="G25" s="394"/>
-      <c r="H25" s="394"/>
-      <c r="I25" s="394"/>
-      <c r="J25" s="394"/>
-      <c r="K25" s="395"/>
+      <c r="B25" s="396"/>
+      <c r="C25" s="396"/>
+      <c r="D25" s="396"/>
+      <c r="E25" s="396"/>
+      <c r="F25" s="396"/>
+      <c r="G25" s="396"/>
+      <c r="H25" s="396"/>
+      <c r="I25" s="396"/>
+      <c r="J25" s="396"/>
+      <c r="K25" s="397"/>
       <c r="L25" s="9">
         <f>IFERROR(K23-K24,0)</f>
         <v>0</v>
@@ -7497,10 +7494,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="11"/>
-      <c r="C5" s="367"/>
-      <c r="D5" s="367"/>
-      <c r="E5" s="367"/>
-      <c r="F5" s="367"/>
+      <c r="C5" s="369"/>
+      <c r="D5" s="369"/>
+      <c r="E5" s="369"/>
+      <c r="F5" s="369"/>
       <c r="H5" s="13"/>
       <c r="I5" s="14" t="s">
         <v>11</v>
@@ -7514,10 +7511,10 @@
         <v>8</v>
       </c>
       <c r="B6" s="11"/>
-      <c r="C6" s="367"/>
-      <c r="D6" s="367"/>
-      <c r="E6" s="367"/>
-      <c r="F6" s="367"/>
+      <c r="C6" s="369"/>
+      <c r="D6" s="369"/>
+      <c r="E6" s="369"/>
+      <c r="F6" s="369"/>
       <c r="K6" s="30"/>
     </row>
     <row r="7" spans="1:12" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -7540,30 +7537,30 @@
         <v>0</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="368"/>
-      <c r="D8" s="368"/>
-      <c r="E8" s="368"/>
-      <c r="F8" s="368"/>
+      <c r="C8" s="370"/>
+      <c r="D8" s="370"/>
+      <c r="E8" s="370"/>
+      <c r="F8" s="370"/>
     </row>
     <row r="9" spans="1:12" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="11"/>
-      <c r="C9" s="367"/>
-      <c r="D9" s="367"/>
-      <c r="E9" s="367"/>
-      <c r="F9" s="367"/>
+      <c r="C9" s="369"/>
+      <c r="D9" s="369"/>
+      <c r="E9" s="369"/>
+      <c r="F9" s="369"/>
     </row>
     <row r="10" spans="1:12" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="11"/>
-      <c r="C10" s="367"/>
-      <c r="D10" s="367"/>
-      <c r="E10" s="367"/>
-      <c r="F10" s="367"/>
+      <c r="C10" s="369"/>
+      <c r="D10" s="369"/>
+      <c r="E10" s="369"/>
+      <c r="F10" s="369"/>
     </row>
     <row r="11" spans="1:12" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:12" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -7589,14 +7586,14 @@
       </c>
     </row>
     <row r="15" spans="1:12" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="390" t="s">
-        <v>150</v>
-      </c>
-      <c r="B15" s="391"/>
-      <c r="C15" s="391"/>
-      <c r="D15" s="391"/>
-      <c r="E15" s="391"/>
-      <c r="F15" s="392"/>
+      <c r="A15" s="392" t="s">
+        <v>149</v>
+      </c>
+      <c r="B15" s="393"/>
+      <c r="C15" s="393"/>
+      <c r="D15" s="393"/>
+      <c r="E15" s="393"/>
+      <c r="F15" s="394"/>
       <c r="G15" s="33"/>
       <c r="H15" s="33"/>
       <c r="I15" s="11"/>
@@ -7605,14 +7602,14 @@
       <c r="L15" s="263"/>
     </row>
     <row r="16" spans="1:12" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="390" t="s">
-        <v>183</v>
-      </c>
-      <c r="B16" s="391"/>
-      <c r="C16" s="391"/>
-      <c r="D16" s="391"/>
-      <c r="E16" s="391"/>
-      <c r="F16" s="392"/>
+      <c r="A16" s="392" t="s">
+        <v>182</v>
+      </c>
+      <c r="B16" s="393"/>
+      <c r="C16" s="393"/>
+      <c r="D16" s="393"/>
+      <c r="E16" s="393"/>
+      <c r="F16" s="394"/>
       <c r="G16" s="33"/>
       <c r="H16" s="33"/>
       <c r="I16" s="11"/>
@@ -7622,7 +7619,7 @@
     </row>
     <row r="17" spans="1:18" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="301" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B17" s="302"/>
       <c r="C17" s="302"/>
@@ -7673,27 +7670,27 @@
       <c r="L20" s="140"/>
     </row>
     <row r="21" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="396" t="s">
+      <c r="A21" s="398" t="s">
         <v>72</v>
       </c>
-      <c r="B21" s="397"/>
-      <c r="C21" s="397"/>
-      <c r="D21" s="397"/>
-      <c r="E21" s="397"/>
-      <c r="F21" s="397"/>
-      <c r="G21" s="397"/>
-      <c r="H21" s="397"/>
-      <c r="I21" s="397"/>
+      <c r="B21" s="399"/>
+      <c r="C21" s="399"/>
+      <c r="D21" s="399"/>
+      <c r="E21" s="399"/>
+      <c r="F21" s="399"/>
+      <c r="G21" s="399"/>
+      <c r="H21" s="399"/>
+      <c r="I21" s="399"/>
       <c r="J21" s="139"/>
       <c r="K21" s="138"/>
       <c r="L21" s="8"/>
       <c r="R21" s="133"/>
     </row>
     <row r="22" spans="1:18" ht="66" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="404" t="s">
+      <c r="A22" s="406" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="405"/>
+      <c r="B22" s="407"/>
       <c r="C22" s="137"/>
       <c r="D22" s="137"/>
       <c r="E22" s="137"/>
@@ -7707,15 +7704,15 @@
       <c r="R22" s="133"/>
     </row>
     <row r="23" spans="1:18" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="400" t="s">
+      <c r="A23" s="402" t="s">
         <v>60</v>
       </c>
-      <c r="B23" s="401"/>
+      <c r="B23" s="403"/>
       <c r="C23" s="272"/>
-      <c r="D23" s="398" t="s">
+      <c r="D23" s="400" t="s">
         <v>52</v>
       </c>
-      <c r="E23" s="399"/>
+      <c r="E23" s="401"/>
       <c r="F23" s="273"/>
       <c r="G23" s="232" t="s">
         <v>71</v>
@@ -7738,11 +7735,11 @@
       <c r="R23" s="133"/>
     </row>
     <row r="24" spans="1:18" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="402" t="s">
+      <c r="A24" s="404" t="s">
         <v>14</v>
       </c>
-      <c r="B24" s="403"/>
-      <c r="C24" s="403"/>
+      <c r="B24" s="405"/>
+      <c r="C24" s="405"/>
       <c r="D24" s="236"/>
       <c r="E24" s="236"/>
       <c r="F24" s="236"/>
@@ -7754,19 +7751,19 @@
       <c r="R24" s="133"/>
     </row>
     <row r="25" spans="1:18" ht="16.350000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="393" t="s">
+      <c r="A25" s="395" t="s">
         <v>62</v>
       </c>
-      <c r="B25" s="394"/>
-      <c r="C25" s="394"/>
-      <c r="D25" s="394"/>
-      <c r="E25" s="394"/>
-      <c r="F25" s="394"/>
-      <c r="G25" s="394"/>
-      <c r="H25" s="394"/>
-      <c r="I25" s="394"/>
-      <c r="J25" s="394"/>
-      <c r="K25" s="395"/>
+      <c r="B25" s="396"/>
+      <c r="C25" s="396"/>
+      <c r="D25" s="396"/>
+      <c r="E25" s="396"/>
+      <c r="F25" s="396"/>
+      <c r="G25" s="396"/>
+      <c r="H25" s="396"/>
+      <c r="I25" s="396"/>
+      <c r="J25" s="396"/>
+      <c r="K25" s="397"/>
       <c r="L25" s="9">
         <f>IFERROR(K23-K24,0)</f>
         <v>0</v>
@@ -7813,7 +7810,7 @@
     </row>
     <row r="28" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="L28" s="127" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="29" spans="1:18" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -7884,6 +7881,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A15:F15"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C10:F10"/>
     <mergeCell ref="A25:K25"/>
     <mergeCell ref="A16:F16"/>
     <mergeCell ref="A21:I21"/>
@@ -7891,12 +7894,6 @@
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="D23:E23"/>
     <mergeCell ref="A24:C24"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="A15:F15"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8506,17 +8503,17 @@
   <sheetData>
     <row r="1" spans="1:12" s="113" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="410" t="s">
+      <c r="A2" s="412" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="410"/>
-      <c r="C2" s="410"/>
-      <c r="D2" s="410"/>
-      <c r="E2" s="410"/>
-      <c r="F2" s="410"/>
-      <c r="G2" s="410"/>
-      <c r="H2" s="410"/>
-      <c r="I2" s="410"/>
+      <c r="B2" s="412"/>
+      <c r="C2" s="412"/>
+      <c r="D2" s="412"/>
+      <c r="E2" s="412"/>
+      <c r="F2" s="412"/>
+      <c r="G2" s="412"/>
+      <c r="H2" s="412"/>
+      <c r="I2" s="412"/>
       <c r="J2" s="143"/>
       <c r="K2" s="143"/>
       <c r="L2" s="143"/>
@@ -8561,10 +8558,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="11"/>
-      <c r="C5" s="367"/>
-      <c r="D5" s="367"/>
-      <c r="E5" s="367"/>
-      <c r="F5" s="367"/>
+      <c r="C5" s="369"/>
+      <c r="D5" s="369"/>
+      <c r="E5" s="369"/>
+      <c r="F5" s="369"/>
       <c r="G5" s="142"/>
       <c r="H5" s="13"/>
       <c r="I5" s="14" t="s">
@@ -8579,10 +8576,10 @@
         <v>8</v>
       </c>
       <c r="B6" s="11"/>
-      <c r="C6" s="367"/>
-      <c r="D6" s="367"/>
-      <c r="E6" s="367"/>
-      <c r="F6" s="367"/>
+      <c r="C6" s="369"/>
+      <c r="D6" s="369"/>
+      <c r="E6" s="369"/>
+      <c r="F6" s="369"/>
       <c r="G6" s="141"/>
       <c r="H6" s="13"/>
       <c r="I6" s="14" t="s">
@@ -8613,10 +8610,10 @@
         <v>0</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="368"/>
-      <c r="D8" s="368"/>
-      <c r="E8" s="368"/>
-      <c r="F8" s="368"/>
+      <c r="C8" s="370"/>
+      <c r="D8" s="370"/>
+      <c r="E8" s="370"/>
+      <c r="F8" s="370"/>
       <c r="G8" s="151"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -8631,10 +8628,10 @@
         <v>6</v>
       </c>
       <c r="B9" s="11"/>
-      <c r="C9" s="367"/>
-      <c r="D9" s="367"/>
-      <c r="E9" s="367"/>
-      <c r="F9" s="367"/>
+      <c r="C9" s="369"/>
+      <c r="D9" s="369"/>
+      <c r="E9" s="369"/>
+      <c r="F9" s="369"/>
       <c r="G9" s="151"/>
       <c r="H9" s="141"/>
       <c r="I9" s="141"/>
@@ -8647,15 +8644,15 @@
         <v>7</v>
       </c>
       <c r="B10" s="11"/>
-      <c r="C10" s="367"/>
-      <c r="D10" s="367"/>
-      <c r="E10" s="367"/>
-      <c r="F10" s="367"/>
+      <c r="C10" s="369"/>
+      <c r="D10" s="369"/>
+      <c r="E10" s="369"/>
+      <c r="F10" s="369"/>
       <c r="G10" s="151"/>
       <c r="H10" s="141"/>
       <c r="I10" s="141"/>
-      <c r="J10" s="406"/>
-      <c r="K10" s="406"/>
+      <c r="J10" s="408"/>
+      <c r="K10" s="408"/>
       <c r="L10" s="152"/>
     </row>
     <row r="11" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -8682,10 +8679,10 @@
       <c r="C13" s="255" t="s">
         <v>125</v>
       </c>
-      <c r="D13" s="411" t="s">
+      <c r="D13" s="413" t="s">
         <v>126</v>
       </c>
-      <c r="E13" s="412"/>
+      <c r="E13" s="414"/>
       <c r="F13" s="255" t="s">
         <v>127</v>
       </c>
@@ -8698,17 +8695,17 @@
       <c r="I13" s="257" t="s">
         <v>97</v>
       </c>
-      <c r="J13" s="415" t="s">
+      <c r="J13" s="417" t="s">
         <v>134</v>
       </c>
-      <c r="K13" s="416"/>
+      <c r="K13" s="418"/>
       <c r="L13" s="150"/>
     </row>
     <row r="14" spans="1:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="274"/>
       <c r="C14" s="275"/>
-      <c r="D14" s="413"/>
-      <c r="E14" s="414"/>
+      <c r="D14" s="415"/>
+      <c r="E14" s="416"/>
       <c r="F14" s="275"/>
       <c r="G14" s="275"/>
       <c r="H14" s="276"/>
@@ -8716,11 +8713,11 @@
         <f>SUM(B14:H14)</f>
         <v>0</v>
       </c>
-      <c r="J14" s="417">
+      <c r="J14" s="419">
         <f>I14/6</f>
         <v>0</v>
       </c>
-      <c r="K14" s="418"/>
+      <c r="K14" s="420"/>
       <c r="L14" s="150"/>
     </row>
     <row r="15" spans="1:12" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -8736,16 +8733,16 @@
       <c r="A17" s="250" t="s">
         <v>133</v>
       </c>
-      <c r="B17" s="407" t="s">
+      <c r="B17" s="409" t="s">
         <v>130</v>
       </c>
-      <c r="C17" s="408"/>
-      <c r="D17" s="408"/>
-      <c r="E17" s="408"/>
-      <c r="F17" s="408"/>
-      <c r="G17" s="408"/>
-      <c r="H17" s="408"/>
-      <c r="I17" s="409"/>
+      <c r="C17" s="410"/>
+      <c r="D17" s="410"/>
+      <c r="E17" s="410"/>
+      <c r="F17" s="410"/>
+      <c r="G17" s="410"/>
+      <c r="H17" s="410"/>
+      <c r="I17" s="411"/>
       <c r="J17" s="148" t="s">
         <v>131</v>
       </c>
@@ -8759,19 +8756,19 @@
       </c>
     </row>
     <row r="18" spans="1:12" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="313" t="s">
-        <v>167</v>
-      </c>
-      <c r="B18" s="385" t="s">
+      <c r="A18" s="343" t="s">
+        <v>166</v>
+      </c>
+      <c r="B18" s="387" t="s">
         <v>132</v>
       </c>
-      <c r="C18" s="386"/>
-      <c r="D18" s="386"/>
-      <c r="E18" s="386"/>
-      <c r="F18" s="386"/>
-      <c r="G18" s="386"/>
-      <c r="H18" s="386"/>
-      <c r="I18" s="386"/>
+      <c r="C18" s="388"/>
+      <c r="D18" s="388"/>
+      <c r="E18" s="388"/>
+      <c r="F18" s="388"/>
+      <c r="G18" s="388"/>
+      <c r="H18" s="388"/>
+      <c r="I18" s="388"/>
       <c r="J18" s="148" t="s">
         <v>136</v>
       </c>
@@ -8782,17 +8779,17 @@
       </c>
     </row>
     <row r="19" spans="1:12" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="314"/>
-      <c r="B19" s="387" t="s">
+      <c r="A19" s="344"/>
+      <c r="B19" s="389" t="s">
         <v>115</v>
       </c>
-      <c r="C19" s="388"/>
-      <c r="D19" s="388"/>
-      <c r="E19" s="388"/>
-      <c r="F19" s="388"/>
-      <c r="G19" s="388"/>
-      <c r="H19" s="388"/>
-      <c r="I19" s="388"/>
+      <c r="C19" s="390"/>
+      <c r="D19" s="390"/>
+      <c r="E19" s="390"/>
+      <c r="F19" s="390"/>
+      <c r="G19" s="390"/>
+      <c r="H19" s="390"/>
+      <c r="I19" s="390"/>
       <c r="J19" s="146" t="s">
         <v>137</v>
       </c>
@@ -8914,6 +8911,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:I18"/>
+    <mergeCell ref="B19:I19"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C10:F10"/>
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="B17:I17"/>
     <mergeCell ref="A2:I2"/>
@@ -8923,12 +8926,6 @@
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="J13:K13"/>
     <mergeCell ref="J14:K14"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:I18"/>
-    <mergeCell ref="B19:I19"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C10:F10"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -9538,17 +9535,17 @@
   <sheetData>
     <row r="1" spans="1:12" s="113" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="410" t="s">
+      <c r="A2" s="412" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="410"/>
-      <c r="C2" s="410"/>
-      <c r="D2" s="410"/>
-      <c r="E2" s="410"/>
-      <c r="F2" s="410"/>
-      <c r="G2" s="410"/>
-      <c r="H2" s="410"/>
-      <c r="I2" s="410"/>
+      <c r="B2" s="412"/>
+      <c r="C2" s="412"/>
+      <c r="D2" s="412"/>
+      <c r="E2" s="412"/>
+      <c r="F2" s="412"/>
+      <c r="G2" s="412"/>
+      <c r="H2" s="412"/>
+      <c r="I2" s="412"/>
       <c r="J2" s="143"/>
       <c r="K2" s="143"/>
       <c r="L2" s="143"/>
@@ -9593,10 +9590,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="11"/>
-      <c r="C5" s="367"/>
-      <c r="D5" s="367"/>
-      <c r="E5" s="367"/>
-      <c r="F5" s="367"/>
+      <c r="C5" s="369"/>
+      <c r="D5" s="369"/>
+      <c r="E5" s="369"/>
+      <c r="F5" s="369"/>
       <c r="G5" s="142"/>
       <c r="H5" s="13"/>
       <c r="I5" s="14" t="s">
@@ -9611,10 +9608,10 @@
         <v>8</v>
       </c>
       <c r="B6" s="11"/>
-      <c r="C6" s="367"/>
-      <c r="D6" s="367"/>
-      <c r="E6" s="367"/>
-      <c r="F6" s="367"/>
+      <c r="C6" s="369"/>
+      <c r="D6" s="369"/>
+      <c r="E6" s="369"/>
+      <c r="F6" s="369"/>
       <c r="G6" s="141"/>
       <c r="H6" s="13"/>
       <c r="I6" s="14" t="s">
@@ -9645,10 +9642,10 @@
         <v>0</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="368"/>
-      <c r="D8" s="368"/>
-      <c r="E8" s="368"/>
-      <c r="F8" s="368"/>
+      <c r="C8" s="370"/>
+      <c r="D8" s="370"/>
+      <c r="E8" s="370"/>
+      <c r="F8" s="370"/>
       <c r="G8" s="151"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -9663,10 +9660,10 @@
         <v>6</v>
       </c>
       <c r="B9" s="11"/>
-      <c r="C9" s="367"/>
-      <c r="D9" s="367"/>
-      <c r="E9" s="367"/>
-      <c r="F9" s="367"/>
+      <c r="C9" s="369"/>
+      <c r="D9" s="369"/>
+      <c r="E9" s="369"/>
+      <c r="F9" s="369"/>
       <c r="G9" s="151"/>
       <c r="H9" s="141"/>
       <c r="I9" s="141"/>
@@ -9679,15 +9676,15 @@
         <v>7</v>
       </c>
       <c r="B10" s="11"/>
-      <c r="C10" s="367"/>
-      <c r="D10" s="367"/>
-      <c r="E10" s="367"/>
-      <c r="F10" s="367"/>
+      <c r="C10" s="369"/>
+      <c r="D10" s="369"/>
+      <c r="E10" s="369"/>
+      <c r="F10" s="369"/>
       <c r="G10" s="151"/>
       <c r="H10" s="141"/>
       <c r="I10" s="141"/>
-      <c r="J10" s="406"/>
-      <c r="K10" s="406"/>
+      <c r="J10" s="408"/>
+      <c r="K10" s="408"/>
       <c r="L10" s="152"/>
     </row>
     <row r="11" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -9714,10 +9711,10 @@
       <c r="C13" s="255" t="s">
         <v>125</v>
       </c>
-      <c r="D13" s="411" t="s">
+      <c r="D13" s="413" t="s">
         <v>126</v>
       </c>
-      <c r="E13" s="412"/>
+      <c r="E13" s="414"/>
       <c r="F13" s="255" t="s">
         <v>127</v>
       </c>
@@ -9730,29 +9727,29 @@
       <c r="I13" s="257" t="s">
         <v>97</v>
       </c>
-      <c r="J13" s="415" t="s">
+      <c r="J13" s="417" t="s">
         <v>134</v>
       </c>
-      <c r="K13" s="416"/>
+      <c r="K13" s="418"/>
       <c r="L13" s="150"/>
     </row>
     <row r="14" spans="1:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="274"/>
       <c r="C14" s="275"/>
-      <c r="D14" s="413"/>
-      <c r="E14" s="414"/>
+      <c r="D14" s="415"/>
+      <c r="E14" s="416"/>
       <c r="F14" s="275"/>
-      <c r="G14" s="419"/>
-      <c r="H14" s="420"/>
+      <c r="G14" s="306"/>
+      <c r="H14" s="307"/>
       <c r="I14" s="277">
         <f>SUM(B14:F14)</f>
         <v>0</v>
       </c>
-      <c r="J14" s="417">
+      <c r="J14" s="419">
         <f>I14/4</f>
         <v>0</v>
       </c>
-      <c r="K14" s="418"/>
+      <c r="K14" s="420"/>
       <c r="L14" s="150"/>
     </row>
     <row r="15" spans="1:12" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -9768,16 +9765,16 @@
       <c r="A17" s="300" t="s">
         <v>133</v>
       </c>
-      <c r="B17" s="407" t="s">
+      <c r="B17" s="409" t="s">
         <v>130</v>
       </c>
-      <c r="C17" s="408"/>
-      <c r="D17" s="408"/>
-      <c r="E17" s="408"/>
-      <c r="F17" s="408"/>
-      <c r="G17" s="408"/>
-      <c r="H17" s="408"/>
-      <c r="I17" s="409"/>
+      <c r="C17" s="410"/>
+      <c r="D17" s="410"/>
+      <c r="E17" s="410"/>
+      <c r="F17" s="410"/>
+      <c r="G17" s="410"/>
+      <c r="H17" s="410"/>
+      <c r="I17" s="411"/>
       <c r="J17" s="148" t="s">
         <v>131</v>
       </c>
@@ -9791,19 +9788,19 @@
       </c>
     </row>
     <row r="18" spans="1:12" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="313" t="s">
-        <v>167</v>
-      </c>
-      <c r="B18" s="385" t="s">
+      <c r="A18" s="343" t="s">
+        <v>166</v>
+      </c>
+      <c r="B18" s="387" t="s">
         <v>132</v>
       </c>
-      <c r="C18" s="386"/>
-      <c r="D18" s="386"/>
-      <c r="E18" s="386"/>
-      <c r="F18" s="386"/>
-      <c r="G18" s="386"/>
-      <c r="H18" s="386"/>
-      <c r="I18" s="386"/>
+      <c r="C18" s="388"/>
+      <c r="D18" s="388"/>
+      <c r="E18" s="388"/>
+      <c r="F18" s="388"/>
+      <c r="G18" s="388"/>
+      <c r="H18" s="388"/>
+      <c r="I18" s="388"/>
       <c r="J18" s="148" t="s">
         <v>136</v>
       </c>
@@ -9814,17 +9811,17 @@
       </c>
     </row>
     <row r="19" spans="1:12" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="314"/>
-      <c r="B19" s="387" t="s">
+      <c r="A19" s="344"/>
+      <c r="B19" s="389" t="s">
         <v>115</v>
       </c>
-      <c r="C19" s="388"/>
-      <c r="D19" s="388"/>
-      <c r="E19" s="388"/>
-      <c r="F19" s="388"/>
-      <c r="G19" s="388"/>
-      <c r="H19" s="388"/>
-      <c r="I19" s="388"/>
+      <c r="C19" s="390"/>
+      <c r="D19" s="390"/>
+      <c r="E19" s="390"/>
+      <c r="F19" s="390"/>
+      <c r="G19" s="390"/>
+      <c r="H19" s="390"/>
+      <c r="I19" s="390"/>
       <c r="J19" s="146" t="s">
         <v>137</v>
       </c>
@@ -9946,6 +9943,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C9:F9"/>
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="B18:I18"/>
     <mergeCell ref="B19:I19"/>
@@ -9955,11 +9957,6 @@
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="J14:K14"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C9:F9"/>
     <mergeCell ref="C10:F10"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="0.19685039370078741"/>
@@ -10031,8 +10028,8 @@
         <v>4</v>
       </c>
       <c r="B3" s="160"/>
-      <c r="C3" s="307"/>
-      <c r="D3" s="307"/>
+      <c r="C3" s="364"/>
+      <c r="D3" s="364"/>
       <c r="E3" s="283"/>
       <c r="F3" s="283"/>
       <c r="H3" s="155"/>
@@ -10048,10 +10045,10 @@
         <v>5</v>
       </c>
       <c r="B4" s="136"/>
-      <c r="C4" s="306"/>
-      <c r="D4" s="306"/>
-      <c r="E4" s="306"/>
-      <c r="F4" s="306"/>
+      <c r="C4" s="363"/>
+      <c r="D4" s="363"/>
+      <c r="E4" s="363"/>
+      <c r="F4" s="363"/>
       <c r="H4" s="155"/>
       <c r="I4" s="156" t="s">
         <v>11</v>
@@ -10065,10 +10062,10 @@
         <v>8</v>
       </c>
       <c r="B5" s="136"/>
-      <c r="C5" s="306"/>
-      <c r="D5" s="306"/>
-      <c r="E5" s="306"/>
-      <c r="F5" s="306"/>
+      <c r="C5" s="363"/>
+      <c r="D5" s="363"/>
+      <c r="E5" s="363"/>
+      <c r="F5" s="363"/>
       <c r="K5" s="30"/>
     </row>
     <row r="6" spans="1:12" s="113" customFormat="1" ht="17.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -10091,10 +10088,10 @@
         <v>0</v>
       </c>
       <c r="B7" s="160"/>
-      <c r="C7" s="306"/>
-      <c r="D7" s="306"/>
-      <c r="E7" s="306"/>
-      <c r="F7" s="306"/>
+      <c r="C7" s="363"/>
+      <c r="D7" s="363"/>
+      <c r="E7" s="363"/>
+      <c r="F7" s="363"/>
       <c r="K7" s="30"/>
     </row>
     <row r="8" spans="1:12" s="113" customFormat="1" ht="17.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -10102,10 +10099,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="136"/>
-      <c r="C8" s="306"/>
-      <c r="D8" s="306"/>
-      <c r="E8" s="306"/>
-      <c r="F8" s="306"/>
+      <c r="C8" s="363"/>
+      <c r="D8" s="363"/>
+      <c r="E8" s="363"/>
+      <c r="F8" s="363"/>
       <c r="K8" s="30"/>
     </row>
     <row r="9" spans="1:12" s="113" customFormat="1" ht="17.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -10113,10 +10110,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="136"/>
-      <c r="C9" s="306"/>
-      <c r="D9" s="306"/>
-      <c r="E9" s="306"/>
-      <c r="F9" s="306"/>
+      <c r="C9" s="363"/>
+      <c r="D9" s="363"/>
+      <c r="E9" s="363"/>
+      <c r="F9" s="363"/>
       <c r="K9" s="30"/>
     </row>
     <row r="10" spans="1:12" s="113" customFormat="1" ht="17.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -10131,112 +10128,112 @@
       <c r="D11" s="286"/>
       <c r="E11" s="286"/>
       <c r="F11" s="286"/>
-      <c r="H11" s="308" t="s">
+      <c r="H11" s="338" t="s">
         <v>16</v>
       </c>
-      <c r="I11" s="309"/>
-      <c r="J11" s="310" t="s">
+      <c r="I11" s="339"/>
+      <c r="J11" s="340" t="s">
         <v>17</v>
       </c>
-      <c r="K11" s="311"/>
-      <c r="L11" s="312"/>
+      <c r="K11" s="341"/>
+      <c r="L11" s="342"/>
     </row>
     <row r="12" spans="1:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="313" t="s">
+      <c r="A12" s="343" t="s">
+        <v>167</v>
+      </c>
+      <c r="B12" s="347" t="s">
         <v>168</v>
       </c>
-      <c r="B12" s="317" t="s">
+      <c r="C12" s="348"/>
+      <c r="D12" s="348"/>
+      <c r="E12" s="348"/>
+      <c r="F12" s="348"/>
+      <c r="G12" s="348"/>
+      <c r="H12" s="351"/>
+      <c r="I12" s="352"/>
+      <c r="J12" s="357" t="s">
         <v>169</v>
       </c>
-      <c r="C12" s="318"/>
-      <c r="D12" s="318"/>
-      <c r="E12" s="318"/>
-      <c r="F12" s="318"/>
-      <c r="G12" s="318"/>
-      <c r="H12" s="321"/>
-      <c r="I12" s="322"/>
-      <c r="J12" s="327" t="s">
-        <v>170</v>
-      </c>
-      <c r="K12" s="330">
+      <c r="K12" s="359">
         <f>SUM(B17:G17)/6</f>
         <v>0</v>
       </c>
-      <c r="L12" s="333">
+      <c r="L12" s="327">
         <f>ROUND(K12*0.6,3)</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="314"/>
-      <c r="B13" s="319"/>
-      <c r="C13" s="320"/>
-      <c r="D13" s="320"/>
-      <c r="E13" s="320"/>
-      <c r="F13" s="320"/>
-      <c r="G13" s="320"/>
-      <c r="H13" s="323"/>
-      <c r="I13" s="324"/>
-      <c r="J13" s="328"/>
-      <c r="K13" s="331"/>
-      <c r="L13" s="334"/>
+      <c r="A13" s="344"/>
+      <c r="B13" s="349"/>
+      <c r="C13" s="350"/>
+      <c r="D13" s="350"/>
+      <c r="E13" s="350"/>
+      <c r="F13" s="350"/>
+      <c r="G13" s="350"/>
+      <c r="H13" s="353"/>
+      <c r="I13" s="354"/>
+      <c r="J13" s="336"/>
+      <c r="K13" s="360"/>
+      <c r="L13" s="328"/>
     </row>
     <row r="14" spans="1:12" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="314"/>
-      <c r="B14" s="319"/>
-      <c r="C14" s="320"/>
-      <c r="D14" s="320"/>
-      <c r="E14" s="320"/>
-      <c r="F14" s="320"/>
-      <c r="G14" s="320"/>
-      <c r="H14" s="323"/>
-      <c r="I14" s="324"/>
-      <c r="J14" s="328"/>
-      <c r="K14" s="331"/>
-      <c r="L14" s="334"/>
+      <c r="A14" s="344"/>
+      <c r="B14" s="349"/>
+      <c r="C14" s="350"/>
+      <c r="D14" s="350"/>
+      <c r="E14" s="350"/>
+      <c r="F14" s="350"/>
+      <c r="G14" s="350"/>
+      <c r="H14" s="353"/>
+      <c r="I14" s="354"/>
+      <c r="J14" s="336"/>
+      <c r="K14" s="360"/>
+      <c r="L14" s="328"/>
     </row>
     <row r="15" spans="1:12" ht="70.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="314"/>
-      <c r="B15" s="319"/>
-      <c r="C15" s="320"/>
-      <c r="D15" s="320"/>
-      <c r="E15" s="320"/>
-      <c r="F15" s="320"/>
-      <c r="G15" s="320"/>
-      <c r="H15" s="323"/>
-      <c r="I15" s="324"/>
-      <c r="J15" s="328"/>
-      <c r="K15" s="331"/>
-      <c r="L15" s="334"/>
+      <c r="A15" s="344"/>
+      <c r="B15" s="349"/>
+      <c r="C15" s="350"/>
+      <c r="D15" s="350"/>
+      <c r="E15" s="350"/>
+      <c r="F15" s="350"/>
+      <c r="G15" s="350"/>
+      <c r="H15" s="353"/>
+      <c r="I15" s="354"/>
+      <c r="J15" s="336"/>
+      <c r="K15" s="360"/>
+      <c r="L15" s="328"/>
     </row>
     <row r="16" spans="1:12" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="315"/>
+      <c r="A16" s="345"/>
       <c r="B16" s="287" t="s">
+        <v>170</v>
+      </c>
+      <c r="C16" s="288" t="s">
         <v>171</v>
       </c>
-      <c r="C16" s="288" t="s">
+      <c r="D16" s="289" t="s">
         <v>172</v>
       </c>
-      <c r="D16" s="289" t="s">
+      <c r="E16" s="288" t="s">
         <v>173</v>
       </c>
-      <c r="E16" s="288" t="s">
+      <c r="F16" s="288" t="s">
         <v>174</v>
       </c>
-      <c r="F16" s="288" t="s">
+      <c r="G16" s="290" t="s">
         <v>175</v>
       </c>
-      <c r="G16" s="290" t="s">
-        <v>176</v>
-      </c>
-      <c r="H16" s="323"/>
-      <c r="I16" s="324"/>
-      <c r="J16" s="328"/>
-      <c r="K16" s="331"/>
-      <c r="L16" s="334"/>
+      <c r="H16" s="353"/>
+      <c r="I16" s="354"/>
+      <c r="J16" s="336"/>
+      <c r="K16" s="360"/>
+      <c r="L16" s="328"/>
     </row>
     <row r="17" spans="1:12" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="316"/>
+      <c r="A17" s="346"/>
       <c r="B17" s="291"/>
       <c r="C17" s="292">
         <v>0</v>
@@ -10245,69 +10242,69 @@
       <c r="E17" s="292"/>
       <c r="F17" s="292"/>
       <c r="G17" s="293"/>
-      <c r="H17" s="325"/>
-      <c r="I17" s="326"/>
-      <c r="J17" s="329"/>
-      <c r="K17" s="332"/>
-      <c r="L17" s="335"/>
+      <c r="H17" s="355"/>
+      <c r="I17" s="356"/>
+      <c r="J17" s="358"/>
+      <c r="K17" s="361"/>
+      <c r="L17" s="362"/>
     </row>
     <row r="18" spans="1:12" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="338" t="s">
+      <c r="A18" s="310" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="341" t="s">
-        <v>177</v>
-      </c>
-      <c r="C18" s="341"/>
-      <c r="D18" s="341"/>
-      <c r="E18" s="341"/>
-      <c r="F18" s="341"/>
-      <c r="G18" s="341"/>
-      <c r="H18" s="344"/>
-      <c r="I18" s="345"/>
-      <c r="J18" s="350" t="s">
+      <c r="B18" s="313" t="s">
+        <v>176</v>
+      </c>
+      <c r="C18" s="313"/>
+      <c r="D18" s="313"/>
+      <c r="E18" s="313"/>
+      <c r="F18" s="313"/>
+      <c r="G18" s="313"/>
+      <c r="H18" s="316"/>
+      <c r="I18" s="317"/>
+      <c r="J18" s="322" t="s">
         <v>1</v>
       </c>
-      <c r="K18" s="353">
+      <c r="K18" s="325">
         <v>0</v>
       </c>
-      <c r="L18" s="333">
+      <c r="L18" s="327">
         <f>IF(K18-K21 &gt;=0, (ROUND((K18-K21)*0.25,3)),0.00000000001)</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="339"/>
-      <c r="B19" s="342"/>
-      <c r="C19" s="342"/>
-      <c r="D19" s="342"/>
-      <c r="E19" s="342"/>
-      <c r="F19" s="342"/>
-      <c r="G19" s="342"/>
-      <c r="H19" s="346"/>
-      <c r="I19" s="347"/>
-      <c r="J19" s="351"/>
-      <c r="K19" s="354"/>
-      <c r="L19" s="334"/>
+      <c r="A19" s="311"/>
+      <c r="B19" s="314"/>
+      <c r="C19" s="314"/>
+      <c r="D19" s="314"/>
+      <c r="E19" s="314"/>
+      <c r="F19" s="314"/>
+      <c r="G19" s="314"/>
+      <c r="H19" s="318"/>
+      <c r="I19" s="319"/>
+      <c r="J19" s="323"/>
+      <c r="K19" s="326"/>
+      <c r="L19" s="328"/>
     </row>
     <row r="20" spans="1:12" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="339"/>
-      <c r="B20" s="343"/>
-      <c r="C20" s="343"/>
-      <c r="D20" s="343"/>
-      <c r="E20" s="343"/>
-      <c r="F20" s="343"/>
-      <c r="G20" s="342"/>
-      <c r="H20" s="346"/>
-      <c r="I20" s="347"/>
-      <c r="J20" s="351"/>
-      <c r="K20" s="354"/>
-      <c r="L20" s="334"/>
+      <c r="A20" s="311"/>
+      <c r="B20" s="315"/>
+      <c r="C20" s="315"/>
+      <c r="D20" s="315"/>
+      <c r="E20" s="315"/>
+      <c r="F20" s="315"/>
+      <c r="G20" s="314"/>
+      <c r="H20" s="318"/>
+      <c r="I20" s="319"/>
+      <c r="J20" s="323"/>
+      <c r="K20" s="326"/>
+      <c r="L20" s="328"/>
     </row>
     <row r="21" spans="1:12" ht="28.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="340"/>
+      <c r="A21" s="312"/>
       <c r="B21" s="294" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C21" s="295">
         <v>0</v>
@@ -10316,44 +10313,44 @@
       <c r="E21" s="295"/>
       <c r="F21" s="295"/>
       <c r="G21" s="295"/>
-      <c r="H21" s="348"/>
-      <c r="I21" s="349"/>
-      <c r="J21" s="352"/>
+      <c r="H21" s="320"/>
+      <c r="I21" s="321"/>
+      <c r="J21" s="324"/>
       <c r="K21" s="296">
         <f>SUM(C21:G21)</f>
         <v>0</v>
       </c>
-      <c r="L21" s="355"/>
+      <c r="L21" s="329"/>
     </row>
     <row r="22" spans="1:12" ht="87.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="338" t="s">
+      <c r="A22" s="310" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="341" t="s">
+      <c r="B22" s="313" t="s">
+        <v>178</v>
+      </c>
+      <c r="C22" s="330"/>
+      <c r="D22" s="330"/>
+      <c r="E22" s="330"/>
+      <c r="F22" s="330"/>
+      <c r="G22" s="331"/>
+      <c r="H22" s="332"/>
+      <c r="I22" s="333"/>
+      <c r="J22" s="336" t="s">
         <v>179</v>
-      </c>
-      <c r="C22" s="356"/>
-      <c r="D22" s="356"/>
-      <c r="E22" s="356"/>
-      <c r="F22" s="356"/>
-      <c r="G22" s="357"/>
-      <c r="H22" s="358"/>
-      <c r="I22" s="359"/>
-      <c r="J22" s="328" t="s">
-        <v>180</v>
       </c>
       <c r="K22" s="297">
         <v>0</v>
       </c>
-      <c r="L22" s="334">
+      <c r="L22" s="328">
         <f>IF((K22-K23)&gt;=0,(ROUND((K22-K23)*0.15,3)),0.000000001)</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="28.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="340"/>
+      <c r="A23" s="312"/>
       <c r="B23" s="298" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C23" s="295">
         <v>0</v>
@@ -10366,14 +10363,14 @@
       </c>
       <c r="F23" s="295"/>
       <c r="G23" s="295"/>
-      <c r="H23" s="360"/>
-      <c r="I23" s="361"/>
-      <c r="J23" s="362"/>
+      <c r="H23" s="334"/>
+      <c r="I23" s="335"/>
+      <c r="J23" s="337"/>
       <c r="K23" s="296">
         <f>SUM(C23:G23)</f>
         <v>0</v>
       </c>
-      <c r="L23" s="355"/>
+      <c r="L23" s="329"/>
     </row>
     <row r="24" spans="1:12" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="21"/>
@@ -10390,11 +10387,11 @@
         <v>3</v>
       </c>
       <c r="J25" s="23"/>
-      <c r="K25" s="336">
+      <c r="K25" s="308">
         <f>SUM(L12:L22)</f>
         <v>0</v>
       </c>
-      <c r="L25" s="337"/>
+      <c r="L25" s="309"/>
     </row>
     <row r="26" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -10417,6 +10414,20 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="A12:A17"/>
+    <mergeCell ref="B12:G15"/>
+    <mergeCell ref="H12:I17"/>
+    <mergeCell ref="J12:J17"/>
+    <mergeCell ref="K12:K17"/>
+    <mergeCell ref="L12:L17"/>
     <mergeCell ref="K25:L25"/>
     <mergeCell ref="A18:A21"/>
     <mergeCell ref="B18:G20"/>
@@ -10429,20 +10440,6 @@
     <mergeCell ref="H22:I23"/>
     <mergeCell ref="J22:J23"/>
     <mergeCell ref="L22:L23"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="A12:A17"/>
-    <mergeCell ref="B12:G15"/>
-    <mergeCell ref="H12:I17"/>
-    <mergeCell ref="J12:J17"/>
-    <mergeCell ref="K12:K17"/>
-    <mergeCell ref="L12:L17"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="C8:F8"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" scale="91" orientation="portrait" r:id="rId1"/>
@@ -10527,10 +10524,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="136"/>
-      <c r="C5" s="363"/>
-      <c r="D5" s="363"/>
-      <c r="E5" s="363"/>
-      <c r="F5" s="363"/>
+      <c r="C5" s="365"/>
+      <c r="D5" s="365"/>
+      <c r="E5" s="365"/>
+      <c r="F5" s="365"/>
       <c r="H5" s="155"/>
       <c r="I5" s="156" t="s">
         <v>11</v>
@@ -10544,10 +10541,10 @@
         <v>8</v>
       </c>
       <c r="B6" s="136"/>
-      <c r="C6" s="363"/>
-      <c r="D6" s="363"/>
-      <c r="E6" s="363"/>
-      <c r="F6" s="363"/>
+      <c r="C6" s="365"/>
+      <c r="D6" s="365"/>
+      <c r="E6" s="365"/>
+      <c r="F6" s="365"/>
       <c r="K6" s="30"/>
     </row>
     <row r="7" spans="1:12" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -10570,30 +10567,30 @@
         <v>0</v>
       </c>
       <c r="B8" s="160"/>
-      <c r="C8" s="363"/>
-      <c r="D8" s="363"/>
-      <c r="E8" s="363"/>
-      <c r="F8" s="363"/>
+      <c r="C8" s="365"/>
+      <c r="D8" s="365"/>
+      <c r="E8" s="365"/>
+      <c r="F8" s="365"/>
     </row>
     <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="136" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="136"/>
-      <c r="C9" s="363"/>
-      <c r="D9" s="363"/>
-      <c r="E9" s="363"/>
-      <c r="F9" s="363"/>
+      <c r="C9" s="365"/>
+      <c r="D9" s="365"/>
+      <c r="E9" s="365"/>
+      <c r="F9" s="365"/>
     </row>
     <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="136" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="136"/>
-      <c r="C10" s="363"/>
-      <c r="D10" s="363"/>
-      <c r="E10" s="363"/>
-      <c r="F10" s="363"/>
+      <c r="C10" s="365"/>
+      <c r="D10" s="365"/>
+      <c r="E10" s="365"/>
+      <c r="F10" s="365"/>
     </row>
     <row r="11" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:12" ht="57.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -10924,10 +10921,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="11"/>
-      <c r="C5" s="367"/>
-      <c r="D5" s="367"/>
-      <c r="E5" s="367"/>
-      <c r="F5" s="367"/>
+      <c r="C5" s="369"/>
+      <c r="D5" s="369"/>
+      <c r="E5" s="369"/>
+      <c r="F5" s="369"/>
       <c r="H5" s="13"/>
       <c r="I5" s="14" t="s">
         <v>11</v>
@@ -10941,10 +10938,10 @@
         <v>8</v>
       </c>
       <c r="B6" s="11"/>
-      <c r="C6" s="367"/>
-      <c r="D6" s="367"/>
-      <c r="E6" s="367"/>
-      <c r="F6" s="367"/>
+      <c r="C6" s="369"/>
+      <c r="D6" s="369"/>
+      <c r="E6" s="369"/>
+      <c r="F6" s="369"/>
       <c r="K6" s="30"/>
     </row>
     <row r="7" spans="1:12" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -10967,30 +10964,30 @@
         <v>0</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="368"/>
-      <c r="D8" s="368"/>
-      <c r="E8" s="368"/>
-      <c r="F8" s="368"/>
+      <c r="C8" s="370"/>
+      <c r="D8" s="370"/>
+      <c r="E8" s="370"/>
+      <c r="F8" s="370"/>
     </row>
     <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="11"/>
-      <c r="C9" s="367"/>
-      <c r="D9" s="367"/>
-      <c r="E9" s="367"/>
-      <c r="F9" s="367"/>
+      <c r="C9" s="369"/>
+      <c r="D9" s="369"/>
+      <c r="E9" s="369"/>
+      <c r="F9" s="369"/>
     </row>
     <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="11"/>
-      <c r="C10" s="367"/>
-      <c r="D10" s="367"/>
-      <c r="E10" s="367"/>
-      <c r="F10" s="367"/>
+      <c r="C10" s="369"/>
+      <c r="D10" s="369"/>
+      <c r="E10" s="369"/>
+      <c r="F10" s="369"/>
     </row>
     <row r="11" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -11126,13 +11123,13 @@
       <c r="L21" s="263"/>
     </row>
     <row r="22" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="364" t="s">
-        <v>181</v>
-      </c>
-      <c r="B22" s="365"/>
-      <c r="C22" s="365"/>
-      <c r="D22" s="365"/>
-      <c r="E22" s="366"/>
+      <c r="A22" s="366" t="s">
+        <v>180</v>
+      </c>
+      <c r="B22" s="367"/>
+      <c r="C22" s="367"/>
+      <c r="D22" s="367"/>
+      <c r="E22" s="368"/>
       <c r="F22" s="33"/>
       <c r="G22" s="33"/>
       <c r="H22" s="33"/>
@@ -11328,10 +11325,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="11"/>
-      <c r="C5" s="367"/>
-      <c r="D5" s="367"/>
-      <c r="E5" s="367"/>
-      <c r="F5" s="367"/>
+      <c r="C5" s="369"/>
+      <c r="D5" s="369"/>
+      <c r="E5" s="369"/>
+      <c r="F5" s="369"/>
       <c r="H5" s="13"/>
       <c r="I5" s="14" t="s">
         <v>11</v>
@@ -11345,10 +11342,10 @@
         <v>8</v>
       </c>
       <c r="B6" s="11"/>
-      <c r="C6" s="367"/>
-      <c r="D6" s="367"/>
-      <c r="E6" s="367"/>
-      <c r="F6" s="367"/>
+      <c r="C6" s="369"/>
+      <c r="D6" s="369"/>
+      <c r="E6" s="369"/>
+      <c r="F6" s="369"/>
       <c r="K6" s="30"/>
     </row>
     <row r="7" spans="1:12" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -11371,30 +11368,30 @@
         <v>0</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="368"/>
-      <c r="D8" s="368"/>
-      <c r="E8" s="368"/>
-      <c r="F8" s="368"/>
+      <c r="C8" s="370"/>
+      <c r="D8" s="370"/>
+      <c r="E8" s="370"/>
+      <c r="F8" s="370"/>
     </row>
     <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="11"/>
-      <c r="C9" s="367"/>
-      <c r="D9" s="367"/>
-      <c r="E9" s="367"/>
-      <c r="F9" s="367"/>
+      <c r="C9" s="369"/>
+      <c r="D9" s="369"/>
+      <c r="E9" s="369"/>
+      <c r="F9" s="369"/>
     </row>
     <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="11"/>
-      <c r="C10" s="367"/>
-      <c r="D10" s="367"/>
-      <c r="E10" s="367"/>
-      <c r="F10" s="367"/>
+      <c r="C10" s="369"/>
+      <c r="D10" s="369"/>
+      <c r="E10" s="369"/>
+      <c r="F10" s="369"/>
     </row>
     <row r="11" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -11686,7 +11683,7 @@
     <row r="1" spans="1:12" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:12" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="154" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H2" s="155"/>
       <c r="I2" s="156" t="s">
@@ -11730,10 +11727,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="136"/>
-      <c r="C5" s="363"/>
-      <c r="D5" s="363"/>
-      <c r="E5" s="363"/>
-      <c r="F5" s="363"/>
+      <c r="C5" s="365"/>
+      <c r="D5" s="365"/>
+      <c r="E5" s="365"/>
+      <c r="F5" s="365"/>
       <c r="H5" s="155"/>
       <c r="I5" s="156" t="s">
         <v>11</v>
@@ -11747,10 +11744,10 @@
         <v>8</v>
       </c>
       <c r="B6" s="136"/>
-      <c r="C6" s="363"/>
-      <c r="D6" s="363"/>
-      <c r="E6" s="363"/>
-      <c r="F6" s="363"/>
+      <c r="C6" s="365"/>
+      <c r="D6" s="365"/>
+      <c r="E6" s="365"/>
+      <c r="F6" s="365"/>
       <c r="K6" s="30"/>
     </row>
     <row r="7" spans="1:12" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -11773,30 +11770,30 @@
         <v>0</v>
       </c>
       <c r="B8" s="160"/>
-      <c r="C8" s="369"/>
-      <c r="D8" s="369"/>
-      <c r="E8" s="369"/>
-      <c r="F8" s="369"/>
+      <c r="C8" s="371"/>
+      <c r="D8" s="371"/>
+      <c r="E8" s="371"/>
+      <c r="F8" s="371"/>
     </row>
     <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="136" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="136"/>
-      <c r="C9" s="363"/>
-      <c r="D9" s="363"/>
-      <c r="E9" s="363"/>
-      <c r="F9" s="363"/>
+      <c r="C9" s="365"/>
+      <c r="D9" s="365"/>
+      <c r="E9" s="365"/>
+      <c r="F9" s="365"/>
     </row>
     <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="136" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="136"/>
-      <c r="C10" s="363"/>
-      <c r="D10" s="363"/>
-      <c r="E10" s="363"/>
-      <c r="F10" s="363"/>
+      <c r="C10" s="365"/>
+      <c r="D10" s="365"/>
+      <c r="E10" s="365"/>
+      <c r="F10" s="365"/>
     </row>
     <row r="11" spans="1:12" ht="33.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -12007,7 +12004,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView showZeros="0" view="pageLayout" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showZeros="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A13" sqref="A13:L14"/>
     </sheetView>
   </sheetViews>
@@ -12705,10 +12702,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="11"/>
-      <c r="C5" s="367"/>
-      <c r="D5" s="367"/>
-      <c r="E5" s="367"/>
-      <c r="F5" s="367"/>
+      <c r="C5" s="369"/>
+      <c r="D5" s="369"/>
+      <c r="E5" s="369"/>
+      <c r="F5" s="369"/>
       <c r="H5" s="13"/>
       <c r="I5" s="14" t="s">
         <v>11</v>
@@ -12722,10 +12719,10 @@
         <v>8</v>
       </c>
       <c r="B6" s="11"/>
-      <c r="C6" s="367"/>
-      <c r="D6" s="367"/>
-      <c r="E6" s="367"/>
-      <c r="F6" s="367"/>
+      <c r="C6" s="369"/>
+      <c r="D6" s="369"/>
+      <c r="E6" s="369"/>
+      <c r="F6" s="369"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -12754,30 +12751,30 @@
         <v>0</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="368"/>
-      <c r="D8" s="368"/>
-      <c r="E8" s="368"/>
-      <c r="F8" s="368"/>
+      <c r="C8" s="370"/>
+      <c r="D8" s="370"/>
+      <c r="E8" s="370"/>
+      <c r="F8" s="370"/>
     </row>
     <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="11"/>
-      <c r="C9" s="367"/>
-      <c r="D9" s="367"/>
-      <c r="E9" s="367"/>
-      <c r="F9" s="367"/>
+      <c r="C9" s="369"/>
+      <c r="D9" s="369"/>
+      <c r="E9" s="369"/>
+      <c r="F9" s="369"/>
     </row>
     <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="11"/>
-      <c r="C10" s="367"/>
-      <c r="D10" s="367"/>
-      <c r="E10" s="367"/>
-      <c r="F10" s="367"/>
+      <c r="C10" s="369"/>
+      <c r="D10" s="369"/>
+      <c r="E10" s="369"/>
+      <c r="F10" s="369"/>
     </row>
     <row r="11" spans="1:12" ht="51.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -12797,32 +12794,32 @@
       <c r="L12" s="67"/>
     </row>
     <row r="13" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="370"/>
-      <c r="B13" s="371"/>
-      <c r="C13" s="371"/>
-      <c r="D13" s="371"/>
-      <c r="E13" s="371"/>
-      <c r="F13" s="371"/>
-      <c r="G13" s="371"/>
-      <c r="H13" s="371"/>
-      <c r="I13" s="371"/>
-      <c r="J13" s="371"/>
-      <c r="K13" s="371"/>
-      <c r="L13" s="372"/>
+      <c r="A13" s="372"/>
+      <c r="B13" s="373"/>
+      <c r="C13" s="373"/>
+      <c r="D13" s="373"/>
+      <c r="E13" s="373"/>
+      <c r="F13" s="373"/>
+      <c r="G13" s="373"/>
+      <c r="H13" s="373"/>
+      <c r="I13" s="373"/>
+      <c r="J13" s="373"/>
+      <c r="K13" s="373"/>
+      <c r="L13" s="374"/>
     </row>
     <row r="14" spans="1:12" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="373"/>
-      <c r="B14" s="374"/>
-      <c r="C14" s="374"/>
-      <c r="D14" s="374"/>
-      <c r="E14" s="374"/>
-      <c r="F14" s="374"/>
-      <c r="G14" s="374"/>
-      <c r="H14" s="374"/>
-      <c r="I14" s="374"/>
-      <c r="J14" s="374"/>
-      <c r="K14" s="374"/>
-      <c r="L14" s="375"/>
+      <c r="A14" s="375"/>
+      <c r="B14" s="376"/>
+      <c r="C14" s="376"/>
+      <c r="D14" s="376"/>
+      <c r="E14" s="376"/>
+      <c r="F14" s="376"/>
+      <c r="G14" s="376"/>
+      <c r="H14" s="376"/>
+      <c r="I14" s="376"/>
+      <c r="J14" s="376"/>
+      <c r="K14" s="376"/>
+      <c r="L14" s="377"/>
     </row>
     <row r="15" spans="1:12" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="32" t="s">
@@ -12905,7 +12902,7 @@
     </row>
     <row r="20" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="73" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C20" s="54"/>
       <c r="D20" s="55"/>
@@ -13111,8 +13108,8 @@
   <sheetPr codeName="Blad7"/>
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView showZeros="0" view="pageLayout" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView showZeros="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
@@ -13765,7 +13762,7 @@
     <row r="1" spans="1:12" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:12" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="50" t="s">
-        <v>144</v>
+        <v>184</v>
       </c>
       <c r="H2" s="13"/>
       <c r="I2" s="14" t="s">
@@ -13809,10 +13806,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="11"/>
-      <c r="C5" s="367"/>
-      <c r="D5" s="367"/>
-      <c r="E5" s="367"/>
-      <c r="F5" s="367"/>
+      <c r="C5" s="369"/>
+      <c r="D5" s="369"/>
+      <c r="E5" s="369"/>
+      <c r="F5" s="369"/>
       <c r="H5" s="13"/>
       <c r="I5" s="14" t="s">
         <v>11</v>
@@ -13826,10 +13823,10 @@
         <v>8</v>
       </c>
       <c r="B6" s="11"/>
-      <c r="C6" s="367"/>
-      <c r="D6" s="367"/>
-      <c r="E6" s="367"/>
-      <c r="F6" s="367"/>
+      <c r="C6" s="369"/>
+      <c r="D6" s="369"/>
+      <c r="E6" s="369"/>
+      <c r="F6" s="369"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -13858,30 +13855,30 @@
         <v>0</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="368"/>
-      <c r="D8" s="368"/>
-      <c r="E8" s="368"/>
-      <c r="F8" s="368"/>
+      <c r="C8" s="370"/>
+      <c r="D8" s="370"/>
+      <c r="E8" s="370"/>
+      <c r="F8" s="370"/>
     </row>
     <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="11"/>
-      <c r="C9" s="367"/>
-      <c r="D9" s="367"/>
-      <c r="E9" s="367"/>
-      <c r="F9" s="367"/>
+      <c r="C9" s="369"/>
+      <c r="D9" s="369"/>
+      <c r="E9" s="369"/>
+      <c r="F9" s="369"/>
     </row>
     <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="11"/>
-      <c r="C10" s="367"/>
-      <c r="D10" s="367"/>
-      <c r="E10" s="367"/>
-      <c r="F10" s="367"/>
+      <c r="C10" s="369"/>
+      <c r="D10" s="369"/>
+      <c r="E10" s="369"/>
+      <c r="F10" s="369"/>
     </row>
     <row r="11" spans="1:12" ht="51.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -13901,32 +13898,32 @@
       <c r="L12" s="67"/>
     </row>
     <row r="13" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="370"/>
-      <c r="B13" s="371"/>
-      <c r="C13" s="371"/>
-      <c r="D13" s="371"/>
-      <c r="E13" s="371"/>
-      <c r="F13" s="371"/>
-      <c r="G13" s="371"/>
-      <c r="H13" s="371"/>
-      <c r="I13" s="371"/>
-      <c r="J13" s="371"/>
-      <c r="K13" s="371"/>
-      <c r="L13" s="372"/>
+      <c r="A13" s="372"/>
+      <c r="B13" s="373"/>
+      <c r="C13" s="373"/>
+      <c r="D13" s="373"/>
+      <c r="E13" s="373"/>
+      <c r="F13" s="373"/>
+      <c r="G13" s="373"/>
+      <c r="H13" s="373"/>
+      <c r="I13" s="373"/>
+      <c r="J13" s="373"/>
+      <c r="K13" s="373"/>
+      <c r="L13" s="374"/>
     </row>
     <row r="14" spans="1:12" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="373"/>
-      <c r="B14" s="374"/>
-      <c r="C14" s="374"/>
-      <c r="D14" s="374"/>
-      <c r="E14" s="374"/>
-      <c r="F14" s="374"/>
-      <c r="G14" s="374"/>
-      <c r="H14" s="374"/>
-      <c r="I14" s="374"/>
-      <c r="J14" s="374"/>
-      <c r="K14" s="374"/>
-      <c r="L14" s="375"/>
+      <c r="A14" s="375"/>
+      <c r="B14" s="376"/>
+      <c r="C14" s="376"/>
+      <c r="D14" s="376"/>
+      <c r="E14" s="376"/>
+      <c r="F14" s="376"/>
+      <c r="G14" s="376"/>
+      <c r="H14" s="376"/>
+      <c r="I14" s="376"/>
+      <c r="J14" s="376"/>
+      <c r="K14" s="376"/>
+      <c r="L14" s="377"/>
     </row>
     <row r="15" spans="1:12" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="32" t="s">
@@ -14009,7 +14006,7 @@
     </row>
     <row r="20" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="73" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C20" s="54"/>
       <c r="D20" s="55"/>
@@ -14805,7 +14802,7 @@
     <row r="1" spans="1:12" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="50" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H2" s="13"/>
       <c r="I2" s="14" t="s">
@@ -14849,10 +14846,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="11"/>
-      <c r="C5" s="367"/>
-      <c r="D5" s="367"/>
-      <c r="E5" s="367"/>
-      <c r="F5" s="367"/>
+      <c r="C5" s="369"/>
+      <c r="D5" s="369"/>
+      <c r="E5" s="369"/>
+      <c r="F5" s="369"/>
       <c r="H5" s="13"/>
       <c r="I5" s="14" t="s">
         <v>11</v>
@@ -14866,10 +14863,10 @@
         <v>8</v>
       </c>
       <c r="B6" s="11"/>
-      <c r="C6" s="367"/>
-      <c r="D6" s="367"/>
-      <c r="E6" s="367"/>
-      <c r="F6" s="367"/>
+      <c r="C6" s="369"/>
+      <c r="D6" s="369"/>
+      <c r="E6" s="369"/>
+      <c r="F6" s="369"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -14898,30 +14895,30 @@
         <v>0</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="368"/>
-      <c r="D8" s="368"/>
-      <c r="E8" s="368"/>
-      <c r="F8" s="368"/>
+      <c r="C8" s="370"/>
+      <c r="D8" s="370"/>
+      <c r="E8" s="370"/>
+      <c r="F8" s="370"/>
     </row>
     <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="11"/>
-      <c r="C9" s="367"/>
-      <c r="D9" s="367"/>
-      <c r="E9" s="367"/>
-      <c r="F9" s="367"/>
+      <c r="C9" s="369"/>
+      <c r="D9" s="369"/>
+      <c r="E9" s="369"/>
+      <c r="F9" s="369"/>
     </row>
     <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="11"/>
-      <c r="C10" s="367"/>
-      <c r="D10" s="367"/>
-      <c r="E10" s="367"/>
-      <c r="F10" s="367"/>
+      <c r="C10" s="369"/>
+      <c r="D10" s="369"/>
+      <c r="E10" s="369"/>
+      <c r="F10" s="369"/>
     </row>
     <row r="11" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -14934,21 +14931,21 @@
       </c>
     </row>
     <row r="14" spans="1:12" ht="59.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="376" t="s">
-        <v>162</v>
-      </c>
-      <c r="B14" s="378" t="s">
+      <c r="A14" s="378" t="s">
+        <v>161</v>
+      </c>
+      <c r="B14" s="380" t="s">
         <v>114</v>
       </c>
-      <c r="C14" s="379"/>
-      <c r="D14" s="379"/>
-      <c r="E14" s="379"/>
-      <c r="F14" s="379"/>
-      <c r="G14" s="379"/>
-      <c r="H14" s="379"/>
-      <c r="I14" s="380"/>
+      <c r="C14" s="381"/>
+      <c r="D14" s="381"/>
+      <c r="E14" s="381"/>
+      <c r="F14" s="381"/>
+      <c r="G14" s="381"/>
+      <c r="H14" s="381"/>
+      <c r="I14" s="382"/>
       <c r="J14" s="18" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K14" s="268"/>
       <c r="L14" s="149">
@@ -14957,19 +14954,19 @@
       </c>
     </row>
     <row r="15" spans="1:12" ht="69" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="377"/>
-      <c r="B15" s="381" t="s">
-        <v>182</v>
-      </c>
-      <c r="C15" s="382"/>
-      <c r="D15" s="382"/>
-      <c r="E15" s="382"/>
-      <c r="F15" s="382"/>
-      <c r="G15" s="382"/>
-      <c r="H15" s="382"/>
-      <c r="I15" s="382"/>
+      <c r="A15" s="379"/>
+      <c r="B15" s="383" t="s">
+        <v>181</v>
+      </c>
+      <c r="C15" s="384"/>
+      <c r="D15" s="384"/>
+      <c r="E15" s="384"/>
+      <c r="F15" s="384"/>
+      <c r="G15" s="384"/>
+      <c r="H15" s="384"/>
+      <c r="I15" s="384"/>
       <c r="J15" s="20" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K15" s="269"/>
       <c r="L15" s="251">
@@ -14978,21 +14975,21 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="383" t="s">
-        <v>163</v>
-      </c>
-      <c r="B16" s="385" t="s">
-        <v>160</v>
-      </c>
-      <c r="C16" s="386"/>
-      <c r="D16" s="386"/>
-      <c r="E16" s="386"/>
-      <c r="F16" s="386"/>
-      <c r="G16" s="386"/>
-      <c r="H16" s="386"/>
-      <c r="I16" s="386"/>
+      <c r="A16" s="385" t="s">
+        <v>162</v>
+      </c>
+      <c r="B16" s="387" t="s">
+        <v>159</v>
+      </c>
+      <c r="C16" s="388"/>
+      <c r="D16" s="388"/>
+      <c r="E16" s="388"/>
+      <c r="F16" s="388"/>
+      <c r="G16" s="388"/>
+      <c r="H16" s="388"/>
+      <c r="I16" s="388"/>
       <c r="J16" s="18" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K16" s="270"/>
       <c r="L16" s="147">
@@ -15001,19 +14998,19 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="80.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="384"/>
-      <c r="B17" s="387" t="s">
-        <v>156</v>
-      </c>
-      <c r="C17" s="388"/>
-      <c r="D17" s="388"/>
-      <c r="E17" s="388"/>
-      <c r="F17" s="388"/>
-      <c r="G17" s="388"/>
-      <c r="H17" s="388"/>
-      <c r="I17" s="388"/>
+      <c r="A17" s="386"/>
+      <c r="B17" s="389" t="s">
+        <v>155</v>
+      </c>
+      <c r="C17" s="390"/>
+      <c r="D17" s="390"/>
+      <c r="E17" s="390"/>
+      <c r="F17" s="390"/>
+      <c r="G17" s="390"/>
+      <c r="H17" s="390"/>
+      <c r="I17" s="390"/>
       <c r="J17" s="19" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K17" s="271"/>
       <c r="L17" s="145">
@@ -15122,17 +15119,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C10:F10"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="B14:I14"/>
     <mergeCell ref="B15:I15"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="B16:I16"/>
     <mergeCell ref="B17:I17"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C10:F10"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -15145,24 +15142,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100570C130F412EDB4EBF3E80DF6A9149FD" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cfaa3b10b9be17ef9f56bd19dc71004c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ddb0c952b897a810c8a4e377cff6bff8" ns1:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -15228,30 +15207,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF64F18F-372D-43EC-AE22-C51BFB121B01}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28A807C1-6DB8-4C6A-8DCB-8B5F61EFE299}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A00BD0D-8423-4FFE-92A4-D273D2078383}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15266,4 +15240,27 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28A807C1-6DB8-4C6A-8DCB-8B5F61EFE299}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF64F18F-372D-43EC-AE22-C51BFB121B01}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Protokoll justerat med postheader för att kunna lägga till ribrik
</commit_message>
<xml_diff>
--- a/mallar/Protokoll/Protokoll 2019 individuell klass_(mall).xlsx
+++ b/mallar/Protokoll/Protokoll 2019 individuell klass_(mall).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26501"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\episerver\voltige\VoltigeClosedXML\mallar\Protokoll\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{676523AE-DD02-4086-818D-58F2C8C4D94B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7883E6EC-A81B-45BE-B4D6-85B4ADFA7DC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" tabRatio="966" firstSheet="9" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" tabRatio="966" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="37" r:id="rId1"/>
@@ -90,6 +90,7 @@
     <definedName name="domare" localSheetId="11">'Individuell tekniska övningar'!$C$34</definedName>
     <definedName name="domare" localSheetId="14">'Individuellt tekniskt artis YV'!$C$28</definedName>
     <definedName name="domare" localSheetId="13">'Individuellt tekniskt artistisk'!$C$28</definedName>
+    <definedName name="header" localSheetId="1">'Häst, individuell'!$A$1</definedName>
     <definedName name="header" localSheetId="9">'Ind kür artistisk junior'!$A$2</definedName>
     <definedName name="header" localSheetId="8">'Ind kür artistisk minior'!$A$2</definedName>
     <definedName name="header" localSheetId="6">'Ind kür tekn junior'!$A$2</definedName>
@@ -1415,7 +1416,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="64">
+  <borders count="65">
     <border>
       <left/>
       <right/>
@@ -2194,6 +2195,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2205,7 +2217,7 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="430">
+  <cellXfs count="435">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2974,6 +2986,113 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="40" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="28" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="40" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="41" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="53" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="50" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="45" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="56" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="64" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="59" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="55" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="56" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="58" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="59" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="23" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="43" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="57" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="46" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="166" fontId="6" fillId="0" borderId="14" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3033,12 +3152,6 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="57" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="59" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3060,95 +3173,9 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="59" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="40" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="28" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="40" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="41" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="53" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="50" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="45" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="55" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="56" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="58" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="59" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="23" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="43" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="46" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="8" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3308,6 +3335,18 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="19" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3346,18 +3385,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="19" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="justify" wrapText="1"/>
@@ -3431,9 +3458,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3471,9 +3498,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3506,26 +3533,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3558,26 +3568,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -5763,10 +5756,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="11"/>
-      <c r="C5" s="366"/>
-      <c r="D5" s="366"/>
-      <c r="E5" s="366"/>
-      <c r="F5" s="366"/>
+      <c r="C5" s="371"/>
+      <c r="D5" s="371"/>
+      <c r="E5" s="371"/>
+      <c r="F5" s="371"/>
       <c r="H5" s="13"/>
       <c r="I5" s="14" t="s">
         <v>11</v>
@@ -5780,10 +5773,10 @@
         <v>8</v>
       </c>
       <c r="B6" s="11"/>
-      <c r="C6" s="366"/>
-      <c r="D6" s="366"/>
-      <c r="E6" s="366"/>
-      <c r="F6" s="366"/>
+      <c r="C6" s="371"/>
+      <c r="D6" s="371"/>
+      <c r="E6" s="371"/>
+      <c r="F6" s="371"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -5812,30 +5805,30 @@
         <v>0</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="367"/>
-      <c r="D8" s="367"/>
-      <c r="E8" s="367"/>
-      <c r="F8" s="367"/>
+      <c r="C8" s="372"/>
+      <c r="D8" s="372"/>
+      <c r="E8" s="372"/>
+      <c r="F8" s="372"/>
     </row>
     <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="11"/>
-      <c r="C9" s="366"/>
-      <c r="D9" s="366"/>
-      <c r="E9" s="366"/>
-      <c r="F9" s="366"/>
+      <c r="C9" s="371"/>
+      <c r="D9" s="371"/>
+      <c r="E9" s="371"/>
+      <c r="F9" s="371"/>
     </row>
     <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="11"/>
-      <c r="C10" s="366"/>
-      <c r="D10" s="366"/>
-      <c r="E10" s="366"/>
-      <c r="F10" s="366"/>
+      <c r="C10" s="371"/>
+      <c r="D10" s="371"/>
+      <c r="E10" s="371"/>
+      <c r="F10" s="371"/>
     </row>
     <row r="11" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -5848,19 +5841,19 @@
       </c>
     </row>
     <row r="14" spans="1:12" ht="59.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="377" t="s">
+      <c r="A14" s="382" t="s">
         <v>151</v>
       </c>
-      <c r="B14" s="379" t="s">
+      <c r="B14" s="384" t="s">
         <v>108</v>
       </c>
-      <c r="C14" s="380"/>
-      <c r="D14" s="380"/>
-      <c r="E14" s="380"/>
-      <c r="F14" s="380"/>
-      <c r="G14" s="380"/>
-      <c r="H14" s="380"/>
-      <c r="I14" s="381"/>
+      <c r="C14" s="385"/>
+      <c r="D14" s="385"/>
+      <c r="E14" s="385"/>
+      <c r="F14" s="385"/>
+      <c r="G14" s="385"/>
+      <c r="H14" s="385"/>
+      <c r="I14" s="386"/>
       <c r="J14" s="18" t="s">
         <v>115</v>
       </c>
@@ -5873,17 +5866,17 @@
       </c>
     </row>
     <row r="15" spans="1:12" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="390"/>
-      <c r="B15" s="382" t="s">
+      <c r="A15" s="395"/>
+      <c r="B15" s="387" t="s">
         <v>169</v>
       </c>
-      <c r="C15" s="383"/>
-      <c r="D15" s="383"/>
-      <c r="E15" s="383"/>
-      <c r="F15" s="383"/>
-      <c r="G15" s="383"/>
-      <c r="H15" s="383"/>
-      <c r="I15" s="383"/>
+      <c r="C15" s="388"/>
+      <c r="D15" s="388"/>
+      <c r="E15" s="388"/>
+      <c r="F15" s="388"/>
+      <c r="G15" s="388"/>
+      <c r="H15" s="388"/>
+      <c r="I15" s="388"/>
       <c r="J15" s="20" t="s">
         <v>116</v>
       </c>
@@ -5896,19 +5889,19 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="85.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="377" t="s">
+      <c r="A16" s="382" t="s">
         <v>152</v>
       </c>
-      <c r="B16" s="386" t="s">
+      <c r="B16" s="391" t="s">
         <v>142</v>
       </c>
-      <c r="C16" s="387"/>
-      <c r="D16" s="387"/>
-      <c r="E16" s="387"/>
-      <c r="F16" s="387"/>
-      <c r="G16" s="387"/>
-      <c r="H16" s="387"/>
-      <c r="I16" s="387"/>
+      <c r="C16" s="392"/>
+      <c r="D16" s="392"/>
+      <c r="E16" s="392"/>
+      <c r="F16" s="392"/>
+      <c r="G16" s="392"/>
+      <c r="H16" s="392"/>
+      <c r="I16" s="392"/>
       <c r="J16" s="18" t="s">
         <v>141</v>
       </c>
@@ -5921,17 +5914,17 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="378"/>
-      <c r="B17" s="388" t="s">
+      <c r="A17" s="383"/>
+      <c r="B17" s="393" t="s">
         <v>143</v>
       </c>
-      <c r="C17" s="389"/>
-      <c r="D17" s="389"/>
-      <c r="E17" s="389"/>
-      <c r="F17" s="389"/>
-      <c r="G17" s="389"/>
-      <c r="H17" s="389"/>
-      <c r="I17" s="389"/>
+      <c r="C17" s="394"/>
+      <c r="D17" s="394"/>
+      <c r="E17" s="394"/>
+      <c r="F17" s="394"/>
+      <c r="G17" s="394"/>
+      <c r="H17" s="394"/>
+      <c r="I17" s="394"/>
       <c r="J17" s="19" t="s">
         <v>148</v>
       </c>
@@ -6706,10 +6699,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="11"/>
-      <c r="C5" s="366"/>
-      <c r="D5" s="366"/>
-      <c r="E5" s="366"/>
-      <c r="F5" s="366"/>
+      <c r="C5" s="371"/>
+      <c r="D5" s="371"/>
+      <c r="E5" s="371"/>
+      <c r="F5" s="371"/>
       <c r="H5" s="13"/>
       <c r="I5" s="14" t="s">
         <v>11</v>
@@ -6723,10 +6716,10 @@
         <v>8</v>
       </c>
       <c r="B6" s="11"/>
-      <c r="C6" s="366"/>
-      <c r="D6" s="366"/>
-      <c r="E6" s="366"/>
-      <c r="F6" s="366"/>
+      <c r="C6" s="371"/>
+      <c r="D6" s="371"/>
+      <c r="E6" s="371"/>
+      <c r="F6" s="371"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -6755,30 +6748,30 @@
         <v>0</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="367"/>
-      <c r="D8" s="367"/>
-      <c r="E8" s="367"/>
-      <c r="F8" s="367"/>
+      <c r="C8" s="372"/>
+      <c r="D8" s="372"/>
+      <c r="E8" s="372"/>
+      <c r="F8" s="372"/>
     </row>
     <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="11"/>
-      <c r="C9" s="366"/>
-      <c r="D9" s="366"/>
-      <c r="E9" s="366"/>
-      <c r="F9" s="366"/>
+      <c r="C9" s="371"/>
+      <c r="D9" s="371"/>
+      <c r="E9" s="371"/>
+      <c r="F9" s="371"/>
     </row>
     <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="11"/>
-      <c r="C10" s="366"/>
-      <c r="D10" s="366"/>
-      <c r="E10" s="366"/>
-      <c r="F10" s="366"/>
+      <c r="C10" s="371"/>
+      <c r="D10" s="371"/>
+      <c r="E10" s="371"/>
+      <c r="F10" s="371"/>
     </row>
     <row r="11" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -6791,19 +6784,19 @@
       </c>
     </row>
     <row r="14" spans="1:12" ht="59.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="377" t="s">
+      <c r="A14" s="382" t="s">
         <v>151</v>
       </c>
-      <c r="B14" s="379" t="s">
+      <c r="B14" s="384" t="s">
         <v>108</v>
       </c>
-      <c r="C14" s="380"/>
-      <c r="D14" s="380"/>
-      <c r="E14" s="380"/>
-      <c r="F14" s="380"/>
-      <c r="G14" s="380"/>
-      <c r="H14" s="380"/>
-      <c r="I14" s="381"/>
+      <c r="C14" s="385"/>
+      <c r="D14" s="385"/>
+      <c r="E14" s="385"/>
+      <c r="F14" s="385"/>
+      <c r="G14" s="385"/>
+      <c r="H14" s="385"/>
+      <c r="I14" s="386"/>
       <c r="J14" s="18" t="s">
         <v>115</v>
       </c>
@@ -6816,17 +6809,17 @@
       </c>
     </row>
     <row r="15" spans="1:12" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="390"/>
-      <c r="B15" s="382" t="s">
+      <c r="A15" s="395"/>
+      <c r="B15" s="387" t="s">
         <v>169</v>
       </c>
-      <c r="C15" s="383"/>
-      <c r="D15" s="383"/>
-      <c r="E15" s="383"/>
-      <c r="F15" s="383"/>
-      <c r="G15" s="383"/>
-      <c r="H15" s="383"/>
-      <c r="I15" s="383"/>
+      <c r="C15" s="388"/>
+      <c r="D15" s="388"/>
+      <c r="E15" s="388"/>
+      <c r="F15" s="388"/>
+      <c r="G15" s="388"/>
+      <c r="H15" s="388"/>
+      <c r="I15" s="388"/>
       <c r="J15" s="20" t="s">
         <v>116</v>
       </c>
@@ -6839,19 +6832,19 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="85.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="377" t="s">
+      <c r="A16" s="382" t="s">
         <v>152</v>
       </c>
-      <c r="B16" s="386" t="s">
+      <c r="B16" s="391" t="s">
         <v>142</v>
       </c>
-      <c r="C16" s="387"/>
-      <c r="D16" s="387"/>
-      <c r="E16" s="387"/>
-      <c r="F16" s="387"/>
-      <c r="G16" s="387"/>
-      <c r="H16" s="387"/>
-      <c r="I16" s="387"/>
+      <c r="C16" s="392"/>
+      <c r="D16" s="392"/>
+      <c r="E16" s="392"/>
+      <c r="F16" s="392"/>
+      <c r="G16" s="392"/>
+      <c r="H16" s="392"/>
+      <c r="I16" s="392"/>
       <c r="J16" s="18" t="s">
         <v>141</v>
       </c>
@@ -6864,17 +6857,17 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="378"/>
-      <c r="B17" s="388" t="s">
+      <c r="A17" s="383"/>
+      <c r="B17" s="393" t="s">
         <v>143</v>
       </c>
-      <c r="C17" s="389"/>
-      <c r="D17" s="389"/>
-      <c r="E17" s="389"/>
-      <c r="F17" s="389"/>
-      <c r="G17" s="389"/>
-      <c r="H17" s="389"/>
-      <c r="I17" s="389"/>
+      <c r="C17" s="394"/>
+      <c r="D17" s="394"/>
+      <c r="E17" s="394"/>
+      <c r="F17" s="394"/>
+      <c r="G17" s="394"/>
+      <c r="H17" s="394"/>
+      <c r="I17" s="394"/>
       <c r="J17" s="19" t="s">
         <v>148</v>
       </c>
@@ -6987,17 +6980,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C10:F10"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="B14:I14"/>
     <mergeCell ref="B15:I15"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="B16:I16"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="C10:F10"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7081,10 +7074,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="11"/>
-      <c r="C5" s="366"/>
-      <c r="D5" s="366"/>
-      <c r="E5" s="366"/>
-      <c r="F5" s="366"/>
+      <c r="C5" s="371"/>
+      <c r="D5" s="371"/>
+      <c r="E5" s="371"/>
+      <c r="F5" s="371"/>
       <c r="H5" s="13"/>
       <c r="I5" s="14" t="s">
         <v>11</v>
@@ -7098,10 +7091,10 @@
         <v>8</v>
       </c>
       <c r="B6" s="11"/>
-      <c r="C6" s="366"/>
-      <c r="D6" s="366"/>
-      <c r="E6" s="366"/>
-      <c r="F6" s="366"/>
+      <c r="C6" s="371"/>
+      <c r="D6" s="371"/>
+      <c r="E6" s="371"/>
+      <c r="F6" s="371"/>
       <c r="K6" s="30"/>
     </row>
     <row r="7" spans="1:12" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -7124,30 +7117,30 @@
         <v>0</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="367"/>
-      <c r="D8" s="367"/>
-      <c r="E8" s="367"/>
-      <c r="F8" s="367"/>
+      <c r="C8" s="372"/>
+      <c r="D8" s="372"/>
+      <c r="E8" s="372"/>
+      <c r="F8" s="372"/>
     </row>
     <row r="9" spans="1:12" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="11"/>
-      <c r="C9" s="366"/>
-      <c r="D9" s="366"/>
-      <c r="E9" s="366"/>
-      <c r="F9" s="366"/>
+      <c r="C9" s="371"/>
+      <c r="D9" s="371"/>
+      <c r="E9" s="371"/>
+      <c r="F9" s="371"/>
     </row>
     <row r="10" spans="1:12" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="11"/>
-      <c r="C10" s="366"/>
-      <c r="D10" s="366"/>
-      <c r="E10" s="366"/>
-      <c r="F10" s="366"/>
+      <c r="C10" s="371"/>
+      <c r="D10" s="371"/>
+      <c r="E10" s="371"/>
+      <c r="F10" s="371"/>
     </row>
     <row r="11" spans="1:12" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:12" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -7173,14 +7166,14 @@
       </c>
     </row>
     <row r="15" spans="1:12" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="391" t="s">
+      <c r="A15" s="396" t="s">
         <v>178</v>
       </c>
-      <c r="B15" s="392"/>
-      <c r="C15" s="392"/>
-      <c r="D15" s="392"/>
-      <c r="E15" s="392"/>
-      <c r="F15" s="393"/>
+      <c r="B15" s="397"/>
+      <c r="C15" s="397"/>
+      <c r="D15" s="397"/>
+      <c r="E15" s="397"/>
+      <c r="F15" s="398"/>
       <c r="G15" s="33"/>
       <c r="H15" s="33"/>
       <c r="I15" s="11"/>
@@ -7189,14 +7182,14 @@
       <c r="L15" s="259"/>
     </row>
     <row r="16" spans="1:12" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="394" t="s">
+      <c r="A16" s="399" t="s">
         <v>170</v>
       </c>
-      <c r="B16" s="395"/>
-      <c r="C16" s="395"/>
-      <c r="D16" s="395"/>
-      <c r="E16" s="395"/>
-      <c r="F16" s="396"/>
+      <c r="B16" s="400"/>
+      <c r="C16" s="400"/>
+      <c r="D16" s="400"/>
+      <c r="E16" s="400"/>
+      <c r="F16" s="401"/>
       <c r="G16" s="33"/>
       <c r="H16" s="33"/>
       <c r="I16" s="11"/>
@@ -7257,27 +7250,27 @@
       <c r="L20" s="140"/>
     </row>
     <row r="21" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="400" t="s">
+      <c r="A21" s="405" t="s">
         <v>66</v>
       </c>
-      <c r="B21" s="401"/>
-      <c r="C21" s="401"/>
-      <c r="D21" s="401"/>
-      <c r="E21" s="401"/>
-      <c r="F21" s="401"/>
-      <c r="G21" s="401"/>
-      <c r="H21" s="401"/>
-      <c r="I21" s="401"/>
+      <c r="B21" s="406"/>
+      <c r="C21" s="406"/>
+      <c r="D21" s="406"/>
+      <c r="E21" s="406"/>
+      <c r="F21" s="406"/>
+      <c r="G21" s="406"/>
+      <c r="H21" s="406"/>
+      <c r="I21" s="406"/>
       <c r="J21" s="139"/>
       <c r="K21" s="138"/>
       <c r="L21" s="8"/>
       <c r="R21" s="133"/>
     </row>
     <row r="22" spans="1:18" ht="66" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="408" t="s">
+      <c r="A22" s="413" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="409"/>
+      <c r="B22" s="414"/>
       <c r="C22" s="137"/>
       <c r="D22" s="137"/>
       <c r="E22" s="137"/>
@@ -7291,15 +7284,15 @@
       <c r="R22" s="133"/>
     </row>
     <row r="23" spans="1:18" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="404" t="s">
+      <c r="A23" s="409" t="s">
         <v>55</v>
       </c>
-      <c r="B23" s="405"/>
+      <c r="B23" s="410"/>
       <c r="C23" s="268"/>
-      <c r="D23" s="402" t="s">
+      <c r="D23" s="407" t="s">
         <v>48</v>
       </c>
-      <c r="E23" s="403"/>
+      <c r="E23" s="408"/>
       <c r="F23" s="269"/>
       <c r="G23" s="228" t="s">
         <v>65</v>
@@ -7322,11 +7315,11 @@
       <c r="R23" s="133"/>
     </row>
     <row r="24" spans="1:18" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="406" t="s">
+      <c r="A24" s="411" t="s">
         <v>14</v>
       </c>
-      <c r="B24" s="407"/>
-      <c r="C24" s="407"/>
+      <c r="B24" s="412"/>
+      <c r="C24" s="412"/>
       <c r="D24" s="232"/>
       <c r="E24" s="232"/>
       <c r="F24" s="232"/>
@@ -7338,19 +7331,19 @@
       <c r="R24" s="133"/>
     </row>
     <row r="25" spans="1:18" ht="16.350000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="397" t="s">
+      <c r="A25" s="402" t="s">
         <v>57</v>
       </c>
-      <c r="B25" s="398"/>
-      <c r="C25" s="398"/>
-      <c r="D25" s="398"/>
-      <c r="E25" s="398"/>
-      <c r="F25" s="398"/>
-      <c r="G25" s="398"/>
-      <c r="H25" s="398"/>
-      <c r="I25" s="398"/>
-      <c r="J25" s="398"/>
-      <c r="K25" s="399"/>
+      <c r="B25" s="403"/>
+      <c r="C25" s="403"/>
+      <c r="D25" s="403"/>
+      <c r="E25" s="403"/>
+      <c r="F25" s="403"/>
+      <c r="G25" s="403"/>
+      <c r="H25" s="403"/>
+      <c r="I25" s="403"/>
+      <c r="J25" s="403"/>
+      <c r="K25" s="404"/>
       <c r="L25" s="9">
         <f>IFERROR(K23-K24,0)</f>
         <v>0</v>
@@ -7483,7 +7476,7 @@
     <mergeCell ref="C10:F10"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="0.19685039370078741"/>
-  <pageSetup paperSize="9" scale="99" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;L&amp;G&amp;C&amp;"Verdana,Normal"&amp;12PROTOKOLL FÖR INDIVIDUELL TÄVLAN</oddHeader>
     <oddFooter>&amp;R2022-01-01</oddFooter>
@@ -7564,10 +7557,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="11"/>
-      <c r="C5" s="366"/>
-      <c r="D5" s="366"/>
-      <c r="E5" s="366"/>
-      <c r="F5" s="366"/>
+      <c r="C5" s="371"/>
+      <c r="D5" s="371"/>
+      <c r="E5" s="371"/>
+      <c r="F5" s="371"/>
       <c r="H5" s="13"/>
       <c r="I5" s="14" t="s">
         <v>11</v>
@@ -7581,10 +7574,10 @@
         <v>8</v>
       </c>
       <c r="B6" s="11"/>
-      <c r="C6" s="366"/>
-      <c r="D6" s="366"/>
-      <c r="E6" s="366"/>
-      <c r="F6" s="366"/>
+      <c r="C6" s="371"/>
+      <c r="D6" s="371"/>
+      <c r="E6" s="371"/>
+      <c r="F6" s="371"/>
       <c r="K6" s="30"/>
     </row>
     <row r="7" spans="1:12" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -7607,30 +7600,30 @@
         <v>0</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="367"/>
-      <c r="D8" s="367"/>
-      <c r="E8" s="367"/>
-      <c r="F8" s="367"/>
+      <c r="C8" s="372"/>
+      <c r="D8" s="372"/>
+      <c r="E8" s="372"/>
+      <c r="F8" s="372"/>
     </row>
     <row r="9" spans="1:12" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="11"/>
-      <c r="C9" s="366"/>
-      <c r="D9" s="366"/>
-      <c r="E9" s="366"/>
-      <c r="F9" s="366"/>
+      <c r="C9" s="371"/>
+      <c r="D9" s="371"/>
+      <c r="E9" s="371"/>
+      <c r="F9" s="371"/>
     </row>
     <row r="10" spans="1:12" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="11"/>
-      <c r="C10" s="366"/>
-      <c r="D10" s="366"/>
-      <c r="E10" s="366"/>
-      <c r="F10" s="366"/>
+      <c r="C10" s="371"/>
+      <c r="D10" s="371"/>
+      <c r="E10" s="371"/>
+      <c r="F10" s="371"/>
     </row>
     <row r="11" spans="1:12" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:12" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -7656,14 +7649,14 @@
       </c>
     </row>
     <row r="15" spans="1:12" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="391" t="s">
+      <c r="A15" s="396" t="s">
         <v>178</v>
       </c>
-      <c r="B15" s="392"/>
-      <c r="C15" s="392"/>
-      <c r="D15" s="392"/>
-      <c r="E15" s="392"/>
-      <c r="F15" s="393"/>
+      <c r="B15" s="397"/>
+      <c r="C15" s="397"/>
+      <c r="D15" s="397"/>
+      <c r="E15" s="397"/>
+      <c r="F15" s="398"/>
       <c r="G15" s="33"/>
       <c r="H15" s="33"/>
       <c r="I15" s="11"/>
@@ -7672,14 +7665,14 @@
       <c r="L15" s="259"/>
     </row>
     <row r="16" spans="1:12" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="394" t="s">
+      <c r="A16" s="399" t="s">
         <v>170</v>
       </c>
-      <c r="B16" s="395"/>
-      <c r="C16" s="395"/>
-      <c r="D16" s="395"/>
-      <c r="E16" s="395"/>
-      <c r="F16" s="396"/>
+      <c r="B16" s="400"/>
+      <c r="C16" s="400"/>
+      <c r="D16" s="400"/>
+      <c r="E16" s="400"/>
+      <c r="F16" s="401"/>
       <c r="G16" s="33"/>
       <c r="H16" s="33"/>
       <c r="I16" s="11"/>
@@ -7740,27 +7733,27 @@
       <c r="L20" s="140"/>
     </row>
     <row r="21" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="400" t="s">
+      <c r="A21" s="405" t="s">
         <v>66</v>
       </c>
-      <c r="B21" s="401"/>
-      <c r="C21" s="401"/>
-      <c r="D21" s="401"/>
-      <c r="E21" s="401"/>
-      <c r="F21" s="401"/>
-      <c r="G21" s="401"/>
-      <c r="H21" s="401"/>
-      <c r="I21" s="401"/>
+      <c r="B21" s="406"/>
+      <c r="C21" s="406"/>
+      <c r="D21" s="406"/>
+      <c r="E21" s="406"/>
+      <c r="F21" s="406"/>
+      <c r="G21" s="406"/>
+      <c r="H21" s="406"/>
+      <c r="I21" s="406"/>
       <c r="J21" s="139"/>
       <c r="K21" s="138"/>
       <c r="L21" s="8"/>
       <c r="R21" s="133"/>
     </row>
     <row r="22" spans="1:18" ht="66" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="408" t="s">
+      <c r="A22" s="413" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="409"/>
+      <c r="B22" s="414"/>
       <c r="C22" s="137"/>
       <c r="D22" s="137"/>
       <c r="E22" s="137"/>
@@ -7774,15 +7767,15 @@
       <c r="R22" s="133"/>
     </row>
     <row r="23" spans="1:18" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="404" t="s">
+      <c r="A23" s="409" t="s">
         <v>55</v>
       </c>
-      <c r="B23" s="405"/>
+      <c r="B23" s="410"/>
       <c r="C23" s="268"/>
-      <c r="D23" s="402" t="s">
+      <c r="D23" s="407" t="s">
         <v>48</v>
       </c>
-      <c r="E23" s="403"/>
+      <c r="E23" s="408"/>
       <c r="F23" s="269"/>
       <c r="G23" s="228" t="s">
         <v>65</v>
@@ -7805,11 +7798,11 @@
       <c r="R23" s="133"/>
     </row>
     <row r="24" spans="1:18" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="406" t="s">
+      <c r="A24" s="411" t="s">
         <v>14</v>
       </c>
-      <c r="B24" s="407"/>
-      <c r="C24" s="407"/>
+      <c r="B24" s="412"/>
+      <c r="C24" s="412"/>
       <c r="D24" s="232"/>
       <c r="E24" s="232"/>
       <c r="F24" s="232"/>
@@ -7821,19 +7814,19 @@
       <c r="R24" s="133"/>
     </row>
     <row r="25" spans="1:18" ht="16.350000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="397" t="s">
+      <c r="A25" s="402" t="s">
         <v>57</v>
       </c>
-      <c r="B25" s="398"/>
-      <c r="C25" s="398"/>
-      <c r="D25" s="398"/>
-      <c r="E25" s="398"/>
-      <c r="F25" s="398"/>
-      <c r="G25" s="398"/>
-      <c r="H25" s="398"/>
-      <c r="I25" s="398"/>
-      <c r="J25" s="398"/>
-      <c r="K25" s="399"/>
+      <c r="B25" s="403"/>
+      <c r="C25" s="403"/>
+      <c r="D25" s="403"/>
+      <c r="E25" s="403"/>
+      <c r="F25" s="403"/>
+      <c r="G25" s="403"/>
+      <c r="H25" s="403"/>
+      <c r="I25" s="403"/>
+      <c r="J25" s="403"/>
+      <c r="K25" s="404"/>
       <c r="L25" s="9">
         <f>IFERROR(K23-K24,0)</f>
         <v>0</v>
@@ -7951,12 +7944,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A15:F15"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C10:F10"/>
     <mergeCell ref="A25:K25"/>
     <mergeCell ref="A16:F16"/>
     <mergeCell ref="A21:I21"/>
@@ -7964,9 +7951,15 @@
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="D23:E23"/>
     <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A15:F15"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C10:F10"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="0.19685039370078741"/>
-  <pageSetup paperSize="9" scale="99" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;L&amp;G&amp;C&amp;"Verdana,Normal"&amp;12PROTOKOLL FÖR INDIVIDUELL TÄVLAN</oddHeader>
     <oddFooter>&amp;R2022-01-01</oddFooter>
@@ -8573,17 +8566,17 @@
   <sheetData>
     <row r="1" spans="1:12" s="113" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="414" t="s">
+      <c r="A2" s="423" t="s">
         <v>179</v>
       </c>
-      <c r="B2" s="414"/>
-      <c r="C2" s="414"/>
-      <c r="D2" s="414"/>
-      <c r="E2" s="414"/>
-      <c r="F2" s="414"/>
-      <c r="G2" s="414"/>
-      <c r="H2" s="414"/>
-      <c r="I2" s="414"/>
+      <c r="B2" s="423"/>
+      <c r="C2" s="423"/>
+      <c r="D2" s="423"/>
+      <c r="E2" s="423"/>
+      <c r="F2" s="423"/>
+      <c r="G2" s="423"/>
+      <c r="H2" s="423"/>
+      <c r="I2" s="423"/>
       <c r="J2" s="143"/>
       <c r="K2" s="143"/>
       <c r="L2" s="143"/>
@@ -8628,10 +8621,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="11"/>
-      <c r="C5" s="366"/>
-      <c r="D5" s="366"/>
-      <c r="E5" s="366"/>
-      <c r="F5" s="366"/>
+      <c r="C5" s="371"/>
+      <c r="D5" s="371"/>
+      <c r="E5" s="371"/>
+      <c r="F5" s="371"/>
       <c r="G5" s="142"/>
       <c r="H5" s="13"/>
       <c r="I5" s="14" t="s">
@@ -8646,10 +8639,10 @@
         <v>8</v>
       </c>
       <c r="B6" s="11"/>
-      <c r="C6" s="366"/>
-      <c r="D6" s="366"/>
-      <c r="E6" s="366"/>
-      <c r="F6" s="366"/>
+      <c r="C6" s="371"/>
+      <c r="D6" s="371"/>
+      <c r="E6" s="371"/>
+      <c r="F6" s="371"/>
       <c r="G6" s="141"/>
       <c r="H6" s="13"/>
       <c r="I6" s="14" t="s">
@@ -8680,10 +8673,10 @@
         <v>0</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="367"/>
-      <c r="D8" s="367"/>
-      <c r="E8" s="367"/>
-      <c r="F8" s="367"/>
+      <c r="C8" s="372"/>
+      <c r="D8" s="372"/>
+      <c r="E8" s="372"/>
+      <c r="F8" s="372"/>
       <c r="G8" s="151"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -8698,10 +8691,10 @@
         <v>6</v>
       </c>
       <c r="B9" s="11"/>
-      <c r="C9" s="366"/>
-      <c r="D9" s="366"/>
-      <c r="E9" s="366"/>
-      <c r="F9" s="366"/>
+      <c r="C9" s="371"/>
+      <c r="D9" s="371"/>
+      <c r="E9" s="371"/>
+      <c r="F9" s="371"/>
       <c r="G9" s="151"/>
       <c r="H9" s="141"/>
       <c r="I9" s="141"/>
@@ -8714,15 +8707,15 @@
         <v>7</v>
       </c>
       <c r="B10" s="11"/>
-      <c r="C10" s="366"/>
-      <c r="D10" s="366"/>
-      <c r="E10" s="366"/>
-      <c r="F10" s="366"/>
+      <c r="C10" s="371"/>
+      <c r="D10" s="371"/>
+      <c r="E10" s="371"/>
+      <c r="F10" s="371"/>
       <c r="G10" s="151"/>
       <c r="H10" s="141"/>
       <c r="I10" s="141"/>
-      <c r="J10" s="410"/>
-      <c r="K10" s="410"/>
+      <c r="J10" s="419"/>
+      <c r="K10" s="419"/>
       <c r="L10" s="152"/>
     </row>
     <row r="11" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -8749,10 +8742,10 @@
       <c r="C13" s="251" t="s">
         <v>118</v>
       </c>
-      <c r="D13" s="415" t="s">
+      <c r="D13" s="424" t="s">
         <v>119</v>
       </c>
-      <c r="E13" s="416"/>
+      <c r="E13" s="425"/>
       <c r="F13" s="251" t="s">
         <v>120</v>
       </c>
@@ -8765,17 +8758,17 @@
       <c r="I13" s="253" t="s">
         <v>91</v>
       </c>
-      <c r="J13" s="419" t="s">
+      <c r="J13" s="428" t="s">
         <v>125</v>
       </c>
-      <c r="K13" s="420"/>
+      <c r="K13" s="429"/>
       <c r="L13" s="150"/>
     </row>
     <row r="14" spans="1:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="270"/>
       <c r="C14" s="271"/>
-      <c r="D14" s="417"/>
-      <c r="E14" s="418"/>
+      <c r="D14" s="426"/>
+      <c r="E14" s="427"/>
       <c r="F14" s="271"/>
       <c r="G14" s="271"/>
       <c r="H14" s="272"/>
@@ -8783,11 +8776,11 @@
         <f>SUM(B14:H14)</f>
         <v>0</v>
       </c>
-      <c r="J14" s="421">
+      <c r="J14" s="430">
         <f>I14/6</f>
         <v>0</v>
       </c>
-      <c r="K14" s="422"/>
+      <c r="K14" s="431"/>
       <c r="L14" s="150"/>
     </row>
     <row r="15" spans="1:12" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -8803,16 +8796,16 @@
       <c r="A17" s="246" t="s">
         <v>124</v>
       </c>
-      <c r="B17" s="411" t="s">
+      <c r="B17" s="420" t="s">
         <v>184</v>
       </c>
-      <c r="C17" s="412"/>
-      <c r="D17" s="412"/>
-      <c r="E17" s="412"/>
-      <c r="F17" s="412"/>
-      <c r="G17" s="412"/>
-      <c r="H17" s="412"/>
-      <c r="I17" s="413"/>
+      <c r="C17" s="421"/>
+      <c r="D17" s="421"/>
+      <c r="E17" s="421"/>
+      <c r="F17" s="421"/>
+      <c r="G17" s="421"/>
+      <c r="H17" s="421"/>
+      <c r="I17" s="422"/>
       <c r="J17" s="148" t="s">
         <v>123</v>
       </c>
@@ -8826,19 +8819,19 @@
       </c>
     </row>
     <row r="18" spans="1:12" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="335" t="s">
+      <c r="A18" s="307" t="s">
         <v>154</v>
       </c>
-      <c r="B18" s="423" t="s">
+      <c r="B18" s="415" t="s">
         <v>185</v>
       </c>
-      <c r="C18" s="424"/>
-      <c r="D18" s="424"/>
-      <c r="E18" s="424"/>
-      <c r="F18" s="424"/>
-      <c r="G18" s="424"/>
-      <c r="H18" s="424"/>
-      <c r="I18" s="424"/>
+      <c r="C18" s="416"/>
+      <c r="D18" s="416"/>
+      <c r="E18" s="416"/>
+      <c r="F18" s="416"/>
+      <c r="G18" s="416"/>
+      <c r="H18" s="416"/>
+      <c r="I18" s="416"/>
       <c r="J18" s="148" t="s">
         <v>127</v>
       </c>
@@ -8849,17 +8842,17 @@
       </c>
     </row>
     <row r="19" spans="1:12" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="336"/>
-      <c r="B19" s="425" t="s">
+      <c r="A19" s="308"/>
+      <c r="B19" s="417" t="s">
         <v>186</v>
       </c>
-      <c r="C19" s="426"/>
-      <c r="D19" s="426"/>
-      <c r="E19" s="426"/>
-      <c r="F19" s="426"/>
-      <c r="G19" s="426"/>
-      <c r="H19" s="426"/>
-      <c r="I19" s="426"/>
+      <c r="C19" s="418"/>
+      <c r="D19" s="418"/>
+      <c r="E19" s="418"/>
+      <c r="F19" s="418"/>
+      <c r="G19" s="418"/>
+      <c r="H19" s="418"/>
+      <c r="I19" s="418"/>
       <c r="J19" s="146" t="s">
         <v>128</v>
       </c>
@@ -8981,12 +8974,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:I18"/>
-    <mergeCell ref="B19:I19"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C10:F10"/>
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="B17:I17"/>
     <mergeCell ref="A2:I2"/>
@@ -8996,9 +8983,15 @@
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="J13:K13"/>
     <mergeCell ref="J14:K14"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:I18"/>
+    <mergeCell ref="B19:I19"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C10:F10"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="0.19685039370078741"/>
-  <pageSetup paperSize="9" scale="99" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;L&amp;G&amp;C&amp;"Verdana,Normal"&amp;12PROTOKOLL FÖR INDIVIDUELL TÄVLAN</oddHeader>
     <oddFooter>&amp;R2019-06-01</oddFooter>
@@ -9014,7 +9007,7 @@
   </sheetPr>
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showZeros="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -9605,17 +9598,17 @@
   <sheetData>
     <row r="1" spans="1:12" s="113" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="414" t="s">
+      <c r="A2" s="423" t="s">
         <v>181</v>
       </c>
-      <c r="B2" s="414"/>
-      <c r="C2" s="414"/>
-      <c r="D2" s="414"/>
-      <c r="E2" s="414"/>
-      <c r="F2" s="414"/>
-      <c r="G2" s="414"/>
-      <c r="H2" s="414"/>
-      <c r="I2" s="414"/>
+      <c r="B2" s="423"/>
+      <c r="C2" s="423"/>
+      <c r="D2" s="423"/>
+      <c r="E2" s="423"/>
+      <c r="F2" s="423"/>
+      <c r="G2" s="423"/>
+      <c r="H2" s="423"/>
+      <c r="I2" s="423"/>
       <c r="J2" s="143"/>
       <c r="K2" s="143"/>
       <c r="L2" s="143"/>
@@ -9660,10 +9653,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="11"/>
-      <c r="C5" s="366"/>
-      <c r="D5" s="366"/>
-      <c r="E5" s="366"/>
-      <c r="F5" s="366"/>
+      <c r="C5" s="371"/>
+      <c r="D5" s="371"/>
+      <c r="E5" s="371"/>
+      <c r="F5" s="371"/>
       <c r="G5" s="142"/>
       <c r="H5" s="13"/>
       <c r="I5" s="14" t="s">
@@ -9678,10 +9671,10 @@
         <v>8</v>
       </c>
       <c r="B6" s="11"/>
-      <c r="C6" s="366"/>
-      <c r="D6" s="366"/>
-      <c r="E6" s="366"/>
-      <c r="F6" s="366"/>
+      <c r="C6" s="371"/>
+      <c r="D6" s="371"/>
+      <c r="E6" s="371"/>
+      <c r="F6" s="371"/>
       <c r="G6" s="141"/>
       <c r="H6" s="13"/>
       <c r="I6" s="14" t="s">
@@ -9712,10 +9705,10 @@
         <v>0</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="367"/>
-      <c r="D8" s="367"/>
-      <c r="E8" s="367"/>
-      <c r="F8" s="367"/>
+      <c r="C8" s="372"/>
+      <c r="D8" s="372"/>
+      <c r="E8" s="372"/>
+      <c r="F8" s="372"/>
       <c r="G8" s="151"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -9730,10 +9723,10 @@
         <v>6</v>
       </c>
       <c r="B9" s="11"/>
-      <c r="C9" s="366"/>
-      <c r="D9" s="366"/>
-      <c r="E9" s="366"/>
-      <c r="F9" s="366"/>
+      <c r="C9" s="371"/>
+      <c r="D9" s="371"/>
+      <c r="E9" s="371"/>
+      <c r="F9" s="371"/>
       <c r="G9" s="151"/>
       <c r="H9" s="141"/>
       <c r="I9" s="141"/>
@@ -9746,15 +9739,15 @@
         <v>7</v>
       </c>
       <c r="B10" s="11"/>
-      <c r="C10" s="366"/>
-      <c r="D10" s="366"/>
-      <c r="E10" s="366"/>
-      <c r="F10" s="366"/>
+      <c r="C10" s="371"/>
+      <c r="D10" s="371"/>
+      <c r="E10" s="371"/>
+      <c r="F10" s="371"/>
       <c r="G10" s="151"/>
       <c r="H10" s="141"/>
       <c r="I10" s="141"/>
-      <c r="J10" s="410"/>
-      <c r="K10" s="410"/>
+      <c r="J10" s="419"/>
+      <c r="K10" s="419"/>
       <c r="L10" s="152"/>
     </row>
     <row r="11" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -9781,10 +9774,10 @@
       <c r="C13" s="251" t="s">
         <v>118</v>
       </c>
-      <c r="D13" s="415" t="s">
+      <c r="D13" s="424" t="s">
         <v>119</v>
       </c>
-      <c r="E13" s="416"/>
+      <c r="E13" s="425"/>
       <c r="F13" s="251" t="s">
         <v>120</v>
       </c>
@@ -9793,17 +9786,17 @@
       <c r="I13" s="253" t="s">
         <v>91</v>
       </c>
-      <c r="J13" s="419" t="s">
+      <c r="J13" s="428" t="s">
         <v>125</v>
       </c>
-      <c r="K13" s="420"/>
+      <c r="K13" s="429"/>
       <c r="L13" s="150"/>
     </row>
     <row r="14" spans="1:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="270"/>
       <c r="C14" s="271"/>
-      <c r="D14" s="417"/>
-      <c r="E14" s="418"/>
+      <c r="D14" s="426"/>
+      <c r="E14" s="427"/>
       <c r="F14" s="271"/>
       <c r="G14" s="296"/>
       <c r="H14" s="297"/>
@@ -9811,11 +9804,11 @@
         <f>SUM(B14:F14)</f>
         <v>0</v>
       </c>
-      <c r="J14" s="421">
+      <c r="J14" s="430">
         <f>I14/4</f>
         <v>0</v>
       </c>
-      <c r="K14" s="422"/>
+      <c r="K14" s="431"/>
       <c r="L14" s="150"/>
     </row>
     <row r="15" spans="1:12" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -9831,16 +9824,16 @@
       <c r="A17" s="246" t="s">
         <v>124</v>
       </c>
-      <c r="B17" s="427" t="s">
+      <c r="B17" s="432" t="s">
         <v>187</v>
       </c>
-      <c r="C17" s="428"/>
-      <c r="D17" s="428"/>
-      <c r="E17" s="428"/>
-      <c r="F17" s="428"/>
-      <c r="G17" s="428"/>
-      <c r="H17" s="428"/>
-      <c r="I17" s="429"/>
+      <c r="C17" s="433"/>
+      <c r="D17" s="433"/>
+      <c r="E17" s="433"/>
+      <c r="F17" s="433"/>
+      <c r="G17" s="433"/>
+      <c r="H17" s="433"/>
+      <c r="I17" s="434"/>
       <c r="J17" s="148" t="s">
         <v>123</v>
       </c>
@@ -9854,19 +9847,19 @@
       </c>
     </row>
     <row r="18" spans="1:12" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="335" t="s">
+      <c r="A18" s="307" t="s">
         <v>154</v>
       </c>
-      <c r="B18" s="423" t="s">
+      <c r="B18" s="415" t="s">
         <v>185</v>
       </c>
-      <c r="C18" s="424"/>
-      <c r="D18" s="424"/>
-      <c r="E18" s="424"/>
-      <c r="F18" s="424"/>
-      <c r="G18" s="424"/>
-      <c r="H18" s="424"/>
-      <c r="I18" s="424"/>
+      <c r="C18" s="416"/>
+      <c r="D18" s="416"/>
+      <c r="E18" s="416"/>
+      <c r="F18" s="416"/>
+      <c r="G18" s="416"/>
+      <c r="H18" s="416"/>
+      <c r="I18" s="416"/>
       <c r="J18" s="148" t="s">
         <v>127</v>
       </c>
@@ -9877,17 +9870,17 @@
       </c>
     </row>
     <row r="19" spans="1:12" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="336"/>
-      <c r="B19" s="425" t="s">
+      <c r="A19" s="308"/>
+      <c r="B19" s="417" t="s">
         <v>186</v>
       </c>
-      <c r="C19" s="426"/>
-      <c r="D19" s="426"/>
-      <c r="E19" s="426"/>
-      <c r="F19" s="426"/>
-      <c r="G19" s="426"/>
-      <c r="H19" s="426"/>
-      <c r="I19" s="426"/>
+      <c r="C19" s="418"/>
+      <c r="D19" s="418"/>
+      <c r="E19" s="418"/>
+      <c r="F19" s="418"/>
+      <c r="G19" s="418"/>
+      <c r="H19" s="418"/>
+      <c r="I19" s="418"/>
       <c r="J19" s="146" t="s">
         <v>128</v>
       </c>
@@ -10009,11 +10002,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C9:F9"/>
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="B18:I18"/>
     <mergeCell ref="B19:I19"/>
@@ -10024,9 +10012,14 @@
     <mergeCell ref="J14:K14"/>
     <mergeCell ref="B17:I17"/>
     <mergeCell ref="C10:F10"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C9:F9"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="0.19685039370078741"/>
-  <pageSetup paperSize="9" scale="99" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;L&amp;G&amp;C&amp;"Verdana,Normal"&amp;12PROTOKOLL FÖR INDIVIDUELL TÄVLAN</oddHeader>
     <oddFooter>&amp;R2019-06-01</oddFooter>
@@ -10042,7 +10035,7 @@
   </sheetPr>
   <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView showZeros="0" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+    <sheetView showZeros="0" tabSelected="1" showRuler="0" topLeftCell="A2" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -10094,8 +10087,8 @@
         <v>4</v>
       </c>
       <c r="B3" s="160"/>
-      <c r="C3" s="356"/>
-      <c r="D3" s="356"/>
+      <c r="C3" s="301"/>
+      <c r="D3" s="301"/>
       <c r="E3" s="279"/>
       <c r="F3" s="279"/>
       <c r="H3" s="155"/>
@@ -10111,10 +10104,10 @@
         <v>5</v>
       </c>
       <c r="B4" s="136"/>
-      <c r="C4" s="355"/>
-      <c r="D4" s="355"/>
-      <c r="E4" s="355"/>
-      <c r="F4" s="355"/>
+      <c r="C4" s="300"/>
+      <c r="D4" s="300"/>
+      <c r="E4" s="300"/>
+      <c r="F4" s="300"/>
       <c r="H4" s="155"/>
       <c r="I4" s="156" t="s">
         <v>11</v>
@@ -10128,10 +10121,10 @@
         <v>8</v>
       </c>
       <c r="B5" s="136"/>
-      <c r="C5" s="355"/>
-      <c r="D5" s="355"/>
-      <c r="E5" s="355"/>
-      <c r="F5" s="355"/>
+      <c r="C5" s="300"/>
+      <c r="D5" s="300"/>
+      <c r="E5" s="300"/>
+      <c r="F5" s="300"/>
       <c r="K5" s="30"/>
     </row>
     <row r="6" spans="1:12" s="113" customFormat="1" ht="17.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -10154,10 +10147,10 @@
         <v>0</v>
       </c>
       <c r="B7" s="160"/>
-      <c r="C7" s="355"/>
-      <c r="D7" s="355"/>
-      <c r="E7" s="355"/>
-      <c r="F7" s="355"/>
+      <c r="C7" s="300"/>
+      <c r="D7" s="300"/>
+      <c r="E7" s="300"/>
+      <c r="F7" s="300"/>
       <c r="K7" s="30"/>
     </row>
     <row r="8" spans="1:12" s="113" customFormat="1" ht="17.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -10165,10 +10158,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="136"/>
-      <c r="C8" s="355"/>
-      <c r="D8" s="355"/>
-      <c r="E8" s="355"/>
-      <c r="F8" s="355"/>
+      <c r="C8" s="300"/>
+      <c r="D8" s="300"/>
+      <c r="E8" s="300"/>
+      <c r="F8" s="300"/>
       <c r="K8" s="30"/>
     </row>
     <row r="9" spans="1:12" s="113" customFormat="1" ht="17.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -10176,10 +10169,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="136"/>
-      <c r="C9" s="355"/>
-      <c r="D9" s="355"/>
-      <c r="E9" s="355"/>
-      <c r="F9" s="355"/>
+      <c r="C9" s="300"/>
+      <c r="D9" s="300"/>
+      <c r="E9" s="300"/>
+      <c r="F9" s="300"/>
       <c r="K9" s="30"/>
     </row>
     <row r="10" spans="1:12" s="113" customFormat="1" ht="17.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -10194,86 +10187,86 @@
       <c r="D11" s="282"/>
       <c r="E11" s="282"/>
       <c r="F11" s="282"/>
-      <c r="H11" s="330" t="s">
+      <c r="H11" s="302" t="s">
         <v>16</v>
       </c>
-      <c r="I11" s="331"/>
-      <c r="J11" s="332" t="s">
+      <c r="I11" s="303"/>
+      <c r="J11" s="304" t="s">
         <v>17</v>
       </c>
-      <c r="K11" s="333"/>
-      <c r="L11" s="334"/>
+      <c r="K11" s="305"/>
+      <c r="L11" s="306"/>
     </row>
     <row r="12" spans="1:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="335" t="s">
+      <c r="A12" s="307" t="s">
         <v>155</v>
       </c>
-      <c r="B12" s="339" t="s">
+      <c r="B12" s="311" t="s">
         <v>156</v>
       </c>
-      <c r="C12" s="340"/>
-      <c r="D12" s="340"/>
-      <c r="E12" s="340"/>
-      <c r="F12" s="340"/>
-      <c r="G12" s="340"/>
-      <c r="H12" s="343"/>
-      <c r="I12" s="344"/>
-      <c r="J12" s="349" t="s">
+      <c r="C12" s="312"/>
+      <c r="D12" s="312"/>
+      <c r="E12" s="312"/>
+      <c r="F12" s="312"/>
+      <c r="G12" s="313"/>
+      <c r="H12" s="320"/>
+      <c r="I12" s="321"/>
+      <c r="J12" s="326" t="s">
         <v>157</v>
       </c>
-      <c r="K12" s="351">
+      <c r="K12" s="329">
         <f>SUM(B17:G17)/6</f>
         <v>0</v>
       </c>
-      <c r="L12" s="319">
+      <c r="L12" s="332">
         <f>ROUND(K12*0.6,3)</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="336"/>
-      <c r="B13" s="341"/>
-      <c r="C13" s="342"/>
-      <c r="D13" s="342"/>
-      <c r="E13" s="342"/>
-      <c r="F13" s="342"/>
-      <c r="G13" s="342"/>
-      <c r="H13" s="345"/>
-      <c r="I13" s="346"/>
-      <c r="J13" s="328"/>
-      <c r="K13" s="352"/>
-      <c r="L13" s="320"/>
+      <c r="A13" s="308"/>
+      <c r="B13" s="314"/>
+      <c r="C13" s="315"/>
+      <c r="D13" s="315"/>
+      <c r="E13" s="315"/>
+      <c r="F13" s="315"/>
+      <c r="G13" s="316"/>
+      <c r="H13" s="322"/>
+      <c r="I13" s="323"/>
+      <c r="J13" s="327"/>
+      <c r="K13" s="330"/>
+      <c r="L13" s="333"/>
     </row>
     <row r="14" spans="1:12" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="336"/>
-      <c r="B14" s="341"/>
-      <c r="C14" s="342"/>
-      <c r="D14" s="342"/>
-      <c r="E14" s="342"/>
-      <c r="F14" s="342"/>
-      <c r="G14" s="342"/>
-      <c r="H14" s="345"/>
-      <c r="I14" s="346"/>
-      <c r="J14" s="328"/>
-      <c r="K14" s="352"/>
-      <c r="L14" s="320"/>
+      <c r="A14" s="308"/>
+      <c r="B14" s="314"/>
+      <c r="C14" s="315"/>
+      <c r="D14" s="315"/>
+      <c r="E14" s="315"/>
+      <c r="F14" s="315"/>
+      <c r="G14" s="316"/>
+      <c r="H14" s="322"/>
+      <c r="I14" s="323"/>
+      <c r="J14" s="327"/>
+      <c r="K14" s="330"/>
+      <c r="L14" s="333"/>
     </row>
     <row r="15" spans="1:12" ht="70.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="336"/>
-      <c r="B15" s="341"/>
-      <c r="C15" s="342"/>
-      <c r="D15" s="342"/>
-      <c r="E15" s="342"/>
-      <c r="F15" s="342"/>
-      <c r="G15" s="342"/>
-      <c r="H15" s="345"/>
-      <c r="I15" s="346"/>
-      <c r="J15" s="328"/>
-      <c r="K15" s="352"/>
-      <c r="L15" s="320"/>
+      <c r="A15" s="308"/>
+      <c r="B15" s="317"/>
+      <c r="C15" s="318"/>
+      <c r="D15" s="318"/>
+      <c r="E15" s="318"/>
+      <c r="F15" s="318"/>
+      <c r="G15" s="319"/>
+      <c r="H15" s="322"/>
+      <c r="I15" s="323"/>
+      <c r="J15" s="327"/>
+      <c r="K15" s="330"/>
+      <c r="L15" s="333"/>
     </row>
     <row r="16" spans="1:12" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="337"/>
+      <c r="A16" s="309"/>
       <c r="B16" s="283" t="s">
         <v>158</v>
       </c>
@@ -10292,14 +10285,14 @@
       <c r="G16" s="286" t="s">
         <v>163</v>
       </c>
-      <c r="H16" s="345"/>
-      <c r="I16" s="346"/>
-      <c r="J16" s="328"/>
-      <c r="K16" s="352"/>
-      <c r="L16" s="320"/>
+      <c r="H16" s="322"/>
+      <c r="I16" s="323"/>
+      <c r="J16" s="327"/>
+      <c r="K16" s="330"/>
+      <c r="L16" s="333"/>
     </row>
     <row r="17" spans="1:12" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="338"/>
+      <c r="A17" s="310"/>
       <c r="B17" s="287"/>
       <c r="C17" s="288">
         <v>0</v>
@@ -10308,67 +10301,67 @@
       <c r="E17" s="288"/>
       <c r="F17" s="288"/>
       <c r="G17" s="289"/>
-      <c r="H17" s="347"/>
-      <c r="I17" s="348"/>
-      <c r="J17" s="350"/>
-      <c r="K17" s="353"/>
-      <c r="L17" s="354"/>
+      <c r="H17" s="324"/>
+      <c r="I17" s="325"/>
+      <c r="J17" s="328"/>
+      <c r="K17" s="331"/>
+      <c r="L17" s="334"/>
     </row>
     <row r="18" spans="1:12" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="302" t="s">
+      <c r="A18" s="337" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="305" t="s">
+      <c r="B18" s="340" t="s">
         <v>164</v>
       </c>
-      <c r="C18" s="305"/>
-      <c r="D18" s="305"/>
-      <c r="E18" s="305"/>
-      <c r="F18" s="305"/>
-      <c r="G18" s="305"/>
-      <c r="H18" s="308"/>
-      <c r="I18" s="309"/>
-      <c r="J18" s="314" t="s">
+      <c r="C18" s="340"/>
+      <c r="D18" s="340"/>
+      <c r="E18" s="340"/>
+      <c r="F18" s="340"/>
+      <c r="G18" s="340"/>
+      <c r="H18" s="343"/>
+      <c r="I18" s="344"/>
+      <c r="J18" s="349" t="s">
         <v>1</v>
       </c>
-      <c r="K18" s="317">
+      <c r="K18" s="352">
         <v>0</v>
       </c>
-      <c r="L18" s="319">
+      <c r="L18" s="332">
         <f>IF(K18-K21 &gt;=0, (ROUND((K18-K21)*0.25,3)),0.00000000001)</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="303"/>
-      <c r="B19" s="306"/>
-      <c r="C19" s="306"/>
-      <c r="D19" s="306"/>
-      <c r="E19" s="306"/>
-      <c r="F19" s="306"/>
-      <c r="G19" s="306"/>
-      <c r="H19" s="310"/>
-      <c r="I19" s="311"/>
-      <c r="J19" s="315"/>
-      <c r="K19" s="318"/>
-      <c r="L19" s="320"/>
+      <c r="A19" s="338"/>
+      <c r="B19" s="341"/>
+      <c r="C19" s="341"/>
+      <c r="D19" s="341"/>
+      <c r="E19" s="341"/>
+      <c r="F19" s="341"/>
+      <c r="G19" s="341"/>
+      <c r="H19" s="345"/>
+      <c r="I19" s="346"/>
+      <c r="J19" s="350"/>
+      <c r="K19" s="353"/>
+      <c r="L19" s="333"/>
     </row>
     <row r="20" spans="1:12" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="303"/>
-      <c r="B20" s="307"/>
-      <c r="C20" s="307"/>
-      <c r="D20" s="307"/>
-      <c r="E20" s="307"/>
-      <c r="F20" s="307"/>
-      <c r="G20" s="306"/>
-      <c r="H20" s="310"/>
-      <c r="I20" s="311"/>
-      <c r="J20" s="315"/>
-      <c r="K20" s="318"/>
-      <c r="L20" s="320"/>
+      <c r="A20" s="338"/>
+      <c r="B20" s="342"/>
+      <c r="C20" s="342"/>
+      <c r="D20" s="342"/>
+      <c r="E20" s="342"/>
+      <c r="F20" s="342"/>
+      <c r="G20" s="341"/>
+      <c r="H20" s="345"/>
+      <c r="I20" s="346"/>
+      <c r="J20" s="350"/>
+      <c r="K20" s="353"/>
+      <c r="L20" s="333"/>
     </row>
     <row r="21" spans="1:12" ht="28.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="304"/>
+      <c r="A21" s="339"/>
       <c r="B21" s="290" t="s">
         <v>165</v>
       </c>
@@ -10379,42 +10372,42 @@
       <c r="E21" s="291"/>
       <c r="F21" s="291"/>
       <c r="G21" s="291"/>
-      <c r="H21" s="312"/>
-      <c r="I21" s="313"/>
-      <c r="J21" s="316"/>
+      <c r="H21" s="347"/>
+      <c r="I21" s="348"/>
+      <c r="J21" s="351"/>
       <c r="K21" s="292">
         <f>SUM(C21:G21)</f>
         <v>0</v>
       </c>
-      <c r="L21" s="321"/>
+      <c r="L21" s="354"/>
     </row>
     <row r="22" spans="1:12" ht="87.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="302" t="s">
+      <c r="A22" s="337" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="305" t="s">
+      <c r="B22" s="340" t="s">
         <v>166</v>
       </c>
-      <c r="C22" s="322"/>
-      <c r="D22" s="322"/>
-      <c r="E22" s="322"/>
-      <c r="F22" s="322"/>
-      <c r="G22" s="323"/>
-      <c r="H22" s="324"/>
-      <c r="I22" s="325"/>
-      <c r="J22" s="328" t="s">
+      <c r="C22" s="355"/>
+      <c r="D22" s="355"/>
+      <c r="E22" s="355"/>
+      <c r="F22" s="355"/>
+      <c r="G22" s="356"/>
+      <c r="H22" s="357"/>
+      <c r="I22" s="358"/>
+      <c r="J22" s="327" t="s">
         <v>167</v>
       </c>
       <c r="K22" s="293">
         <v>0</v>
       </c>
-      <c r="L22" s="320">
+      <c r="L22" s="333">
         <f>IF((K22-K23)&gt;=0,(ROUND((K22-K23)*0.15,3)),0.000000001)</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="28.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="304"/>
+      <c r="A23" s="339"/>
       <c r="B23" s="294" t="s">
         <v>165</v>
       </c>
@@ -10429,14 +10422,14 @@
       </c>
       <c r="F23" s="291"/>
       <c r="G23" s="291"/>
-      <c r="H23" s="326"/>
-      <c r="I23" s="327"/>
-      <c r="J23" s="329"/>
+      <c r="H23" s="359"/>
+      <c r="I23" s="360"/>
+      <c r="J23" s="361"/>
       <c r="K23" s="292">
         <f>SUM(C23:G23)</f>
         <v>0</v>
       </c>
-      <c r="L23" s="321"/>
+      <c r="L23" s="354"/>
     </row>
     <row r="24" spans="1:12" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="21"/>
@@ -10453,11 +10446,11 @@
         <v>3</v>
       </c>
       <c r="J25" s="23"/>
-      <c r="K25" s="300">
+      <c r="K25" s="335">
         <f>SUM(L12:L22)</f>
         <v>0</v>
       </c>
-      <c r="L25" s="301"/>
+      <c r="L25" s="336"/>
     </row>
     <row r="26" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -10480,20 +10473,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="A12:A17"/>
-    <mergeCell ref="B12:G15"/>
-    <mergeCell ref="H12:I17"/>
-    <mergeCell ref="J12:J17"/>
-    <mergeCell ref="K12:K17"/>
-    <mergeCell ref="L12:L17"/>
     <mergeCell ref="K25:L25"/>
     <mergeCell ref="A18:A21"/>
     <mergeCell ref="B18:G20"/>
@@ -10506,6 +10485,20 @@
     <mergeCell ref="H22:I23"/>
     <mergeCell ref="J22:J23"/>
     <mergeCell ref="L22:L23"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="A12:A17"/>
+    <mergeCell ref="B12:G15"/>
+    <mergeCell ref="H12:I17"/>
+    <mergeCell ref="J12:J17"/>
+    <mergeCell ref="K12:K17"/>
+    <mergeCell ref="L12:L17"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="C8:F8"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" scale="90" orientation="portrait" r:id="rId1"/>
@@ -10525,7 +10518,7 @@
   <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView showZeros="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
@@ -10592,10 +10585,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="136"/>
-      <c r="C5" s="360"/>
-      <c r="D5" s="360"/>
-      <c r="E5" s="360"/>
-      <c r="F5" s="360"/>
+      <c r="C5" s="365"/>
+      <c r="D5" s="365"/>
+      <c r="E5" s="365"/>
+      <c r="F5" s="365"/>
       <c r="H5" s="155"/>
       <c r="I5" s="156" t="s">
         <v>11</v>
@@ -10609,10 +10602,10 @@
         <v>8</v>
       </c>
       <c r="B6" s="136"/>
-      <c r="C6" s="360"/>
-      <c r="D6" s="360"/>
-      <c r="E6" s="360"/>
-      <c r="F6" s="360"/>
+      <c r="C6" s="365"/>
+      <c r="D6" s="365"/>
+      <c r="E6" s="365"/>
+      <c r="F6" s="365"/>
       <c r="K6" s="30"/>
     </row>
     <row r="7" spans="1:12" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -10635,30 +10628,30 @@
         <v>0</v>
       </c>
       <c r="B8" s="160"/>
-      <c r="C8" s="360"/>
-      <c r="D8" s="360"/>
-      <c r="E8" s="360"/>
-      <c r="F8" s="360"/>
+      <c r="C8" s="365"/>
+      <c r="D8" s="365"/>
+      <c r="E8" s="365"/>
+      <c r="F8" s="365"/>
     </row>
     <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="136" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="136"/>
-      <c r="C9" s="360"/>
-      <c r="D9" s="360"/>
-      <c r="E9" s="360"/>
-      <c r="F9" s="360"/>
+      <c r="C9" s="365"/>
+      <c r="D9" s="365"/>
+      <c r="E9" s="365"/>
+      <c r="F9" s="365"/>
     </row>
     <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="136" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="136"/>
-      <c r="C10" s="360"/>
-      <c r="D10" s="360"/>
-      <c r="E10" s="360"/>
-      <c r="F10" s="360"/>
+      <c r="C10" s="365"/>
+      <c r="D10" s="365"/>
+      <c r="E10" s="365"/>
+      <c r="F10" s="365"/>
     </row>
     <row r="11" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:12" ht="57.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -10689,12 +10682,12 @@
       <c r="C15" s="196"/>
       <c r="D15" s="199"/>
       <c r="E15" s="227"/>
-      <c r="F15" s="358"/>
-      <c r="G15" s="358"/>
-      <c r="H15" s="358"/>
-      <c r="I15" s="358"/>
-      <c r="J15" s="358"/>
-      <c r="K15" s="359"/>
+      <c r="F15" s="363"/>
+      <c r="G15" s="363"/>
+      <c r="H15" s="363"/>
+      <c r="I15" s="363"/>
+      <c r="J15" s="363"/>
+      <c r="K15" s="364"/>
       <c r="L15" s="258"/>
     </row>
     <row r="16" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -10705,12 +10698,12 @@
       <c r="C16" s="196"/>
       <c r="D16" s="199"/>
       <c r="E16" s="227"/>
-      <c r="F16" s="358"/>
-      <c r="G16" s="358"/>
-      <c r="H16" s="358"/>
-      <c r="I16" s="358"/>
-      <c r="J16" s="358"/>
-      <c r="K16" s="359"/>
+      <c r="F16" s="363"/>
+      <c r="G16" s="363"/>
+      <c r="H16" s="363"/>
+      <c r="I16" s="363"/>
+      <c r="J16" s="363"/>
+      <c r="K16" s="364"/>
       <c r="L16" s="258"/>
     </row>
     <row r="17" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -10721,12 +10714,12 @@
       <c r="C17" s="196"/>
       <c r="D17" s="199"/>
       <c r="E17" s="227"/>
-      <c r="F17" s="358"/>
-      <c r="G17" s="358"/>
-      <c r="H17" s="358"/>
-      <c r="I17" s="358"/>
-      <c r="J17" s="358"/>
-      <c r="K17" s="359"/>
+      <c r="F17" s="363"/>
+      <c r="G17" s="363"/>
+      <c r="H17" s="363"/>
+      <c r="I17" s="363"/>
+      <c r="J17" s="363"/>
+      <c r="K17" s="364"/>
       <c r="L17" s="258"/>
     </row>
     <row r="18" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -10737,12 +10730,12 @@
       <c r="C18" s="196"/>
       <c r="D18" s="199"/>
       <c r="E18" s="227"/>
-      <c r="F18" s="358"/>
-      <c r="G18" s="358"/>
-      <c r="H18" s="358"/>
-      <c r="I18" s="358"/>
-      <c r="J18" s="358"/>
-      <c r="K18" s="359"/>
+      <c r="F18" s="363"/>
+      <c r="G18" s="363"/>
+      <c r="H18" s="363"/>
+      <c r="I18" s="363"/>
+      <c r="J18" s="363"/>
+      <c r="K18" s="364"/>
       <c r="L18" s="258"/>
     </row>
     <row r="19" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -10752,13 +10745,13 @@
       <c r="B19" s="187"/>
       <c r="C19" s="187"/>
       <c r="D19" s="187"/>
-      <c r="E19" s="361"/>
-      <c r="F19" s="361"/>
-      <c r="G19" s="361"/>
-      <c r="H19" s="361"/>
-      <c r="I19" s="361"/>
-      <c r="J19" s="361"/>
-      <c r="K19" s="362"/>
+      <c r="E19" s="366"/>
+      <c r="F19" s="366"/>
+      <c r="G19" s="366"/>
+      <c r="H19" s="366"/>
+      <c r="I19" s="366"/>
+      <c r="J19" s="366"/>
+      <c r="K19" s="367"/>
       <c r="L19" s="258"/>
     </row>
     <row r="20" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -10768,13 +10761,13 @@
       <c r="B20" s="182"/>
       <c r="C20" s="182"/>
       <c r="D20" s="200"/>
-      <c r="E20" s="357"/>
-      <c r="F20" s="358"/>
-      <c r="G20" s="358"/>
-      <c r="H20" s="358"/>
-      <c r="I20" s="358"/>
-      <c r="J20" s="358"/>
-      <c r="K20" s="359"/>
+      <c r="E20" s="362"/>
+      <c r="F20" s="363"/>
+      <c r="G20" s="363"/>
+      <c r="H20" s="363"/>
+      <c r="I20" s="363"/>
+      <c r="J20" s="363"/>
+      <c r="K20" s="364"/>
       <c r="L20" s="258"/>
     </row>
     <row r="21" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -10786,11 +10779,11 @@
       <c r="D21" s="182"/>
       <c r="E21" s="183"/>
       <c r="F21" s="197"/>
-      <c r="G21" s="358"/>
-      <c r="H21" s="358"/>
-      <c r="I21" s="358"/>
-      <c r="J21" s="358"/>
-      <c r="K21" s="359"/>
+      <c r="G21" s="363"/>
+      <c r="H21" s="363"/>
+      <c r="I21" s="363"/>
+      <c r="J21" s="363"/>
+      <c r="K21" s="364"/>
       <c r="L21" s="258"/>
     </row>
     <row r="22" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -10998,10 +10991,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="11"/>
-      <c r="C5" s="366"/>
-      <c r="D5" s="366"/>
-      <c r="E5" s="366"/>
-      <c r="F5" s="366"/>
+      <c r="C5" s="371"/>
+      <c r="D5" s="371"/>
+      <c r="E5" s="371"/>
+      <c r="F5" s="371"/>
       <c r="H5" s="13"/>
       <c r="I5" s="14" t="s">
         <v>11</v>
@@ -11015,10 +11008,10 @@
         <v>8</v>
       </c>
       <c r="B6" s="11"/>
-      <c r="C6" s="366"/>
-      <c r="D6" s="366"/>
-      <c r="E6" s="366"/>
-      <c r="F6" s="366"/>
+      <c r="C6" s="371"/>
+      <c r="D6" s="371"/>
+      <c r="E6" s="371"/>
+      <c r="F6" s="371"/>
       <c r="K6" s="30"/>
     </row>
     <row r="7" spans="1:12" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -11041,30 +11034,30 @@
         <v>0</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="367"/>
-      <c r="D8" s="367"/>
-      <c r="E8" s="367"/>
-      <c r="F8" s="367"/>
+      <c r="C8" s="372"/>
+      <c r="D8" s="372"/>
+      <c r="E8" s="372"/>
+      <c r="F8" s="372"/>
     </row>
     <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="11"/>
-      <c r="C9" s="366"/>
-      <c r="D9" s="366"/>
-      <c r="E9" s="366"/>
-      <c r="F9" s="366"/>
+      <c r="C9" s="371"/>
+      <c r="D9" s="371"/>
+      <c r="E9" s="371"/>
+      <c r="F9" s="371"/>
     </row>
     <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="11"/>
-      <c r="C10" s="366"/>
-      <c r="D10" s="366"/>
-      <c r="E10" s="366"/>
-      <c r="F10" s="366"/>
+      <c r="C10" s="371"/>
+      <c r="D10" s="371"/>
+      <c r="E10" s="371"/>
+      <c r="F10" s="371"/>
     </row>
     <row r="11" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -11200,13 +11193,13 @@
       <c r="L21" s="259"/>
     </row>
     <row r="22" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="363" t="s">
+      <c r="A22" s="368" t="s">
         <v>168</v>
       </c>
-      <c r="B22" s="364"/>
-      <c r="C22" s="364"/>
-      <c r="D22" s="364"/>
-      <c r="E22" s="365"/>
+      <c r="B22" s="369"/>
+      <c r="C22" s="369"/>
+      <c r="D22" s="369"/>
+      <c r="E22" s="370"/>
       <c r="F22" s="33"/>
       <c r="G22" s="33"/>
       <c r="H22" s="33"/>
@@ -11402,10 +11395,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="11"/>
-      <c r="C5" s="366"/>
-      <c r="D5" s="366"/>
-      <c r="E5" s="366"/>
-      <c r="F5" s="366"/>
+      <c r="C5" s="371"/>
+      <c r="D5" s="371"/>
+      <c r="E5" s="371"/>
+      <c r="F5" s="371"/>
       <c r="H5" s="13"/>
       <c r="I5" s="14" t="s">
         <v>11</v>
@@ -11419,10 +11412,10 @@
         <v>8</v>
       </c>
       <c r="B6" s="11"/>
-      <c r="C6" s="366"/>
-      <c r="D6" s="366"/>
-      <c r="E6" s="366"/>
-      <c r="F6" s="366"/>
+      <c r="C6" s="371"/>
+      <c r="D6" s="371"/>
+      <c r="E6" s="371"/>
+      <c r="F6" s="371"/>
       <c r="K6" s="30"/>
     </row>
     <row r="7" spans="1:12" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -11445,30 +11438,30 @@
         <v>0</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="367"/>
-      <c r="D8" s="367"/>
-      <c r="E8" s="367"/>
-      <c r="F8" s="367"/>
+      <c r="C8" s="372"/>
+      <c r="D8" s="372"/>
+      <c r="E8" s="372"/>
+      <c r="F8" s="372"/>
     </row>
     <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="11"/>
-      <c r="C9" s="366"/>
-      <c r="D9" s="366"/>
-      <c r="E9" s="366"/>
-      <c r="F9" s="366"/>
+      <c r="C9" s="371"/>
+      <c r="D9" s="371"/>
+      <c r="E9" s="371"/>
+      <c r="F9" s="371"/>
     </row>
     <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="11"/>
-      <c r="C10" s="366"/>
-      <c r="D10" s="366"/>
-      <c r="E10" s="366"/>
-      <c r="F10" s="366"/>
+      <c r="C10" s="371"/>
+      <c r="D10" s="371"/>
+      <c r="E10" s="371"/>
+      <c r="F10" s="371"/>
     </row>
     <row r="11" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -11767,14 +11760,14 @@
   <sheetData>
     <row r="1" spans="1:12" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:12" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="368" t="s">
+      <c r="A2" s="373" t="s">
         <v>190</v>
       </c>
-      <c r="B2" s="368"/>
-      <c r="C2" s="368"/>
-      <c r="D2" s="368"/>
-      <c r="E2" s="368"/>
-      <c r="F2" s="368"/>
+      <c r="B2" s="373"/>
+      <c r="C2" s="373"/>
+      <c r="D2" s="373"/>
+      <c r="E2" s="373"/>
+      <c r="F2" s="373"/>
       <c r="H2" s="155"/>
       <c r="I2" s="156" t="s">
         <v>61</v>
@@ -11817,10 +11810,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="136"/>
-      <c r="C5" s="360"/>
-      <c r="D5" s="360"/>
-      <c r="E5" s="360"/>
-      <c r="F5" s="360"/>
+      <c r="C5" s="365"/>
+      <c r="D5" s="365"/>
+      <c r="E5" s="365"/>
+      <c r="F5" s="365"/>
       <c r="H5" s="155"/>
       <c r="I5" s="156" t="s">
         <v>11</v>
@@ -11834,10 +11827,10 @@
         <v>8</v>
       </c>
       <c r="B6" s="136"/>
-      <c r="C6" s="360"/>
-      <c r="D6" s="360"/>
-      <c r="E6" s="360"/>
-      <c r="F6" s="360"/>
+      <c r="C6" s="365"/>
+      <c r="D6" s="365"/>
+      <c r="E6" s="365"/>
+      <c r="F6" s="365"/>
       <c r="K6" s="30"/>
     </row>
     <row r="7" spans="1:12" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -11860,30 +11853,30 @@
         <v>0</v>
       </c>
       <c r="B8" s="160"/>
-      <c r="C8" s="369"/>
-      <c r="D8" s="369"/>
-      <c r="E8" s="369"/>
-      <c r="F8" s="369"/>
+      <c r="C8" s="374"/>
+      <c r="D8" s="374"/>
+      <c r="E8" s="374"/>
+      <c r="F8" s="374"/>
     </row>
     <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="136" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="136"/>
-      <c r="C9" s="360"/>
-      <c r="D9" s="360"/>
-      <c r="E9" s="360"/>
-      <c r="F9" s="360"/>
+      <c r="C9" s="365"/>
+      <c r="D9" s="365"/>
+      <c r="E9" s="365"/>
+      <c r="F9" s="365"/>
     </row>
     <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="136" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="136"/>
-      <c r="C10" s="360"/>
-      <c r="D10" s="360"/>
-      <c r="E10" s="360"/>
-      <c r="F10" s="360"/>
+      <c r="C10" s="365"/>
+      <c r="D10" s="365"/>
+      <c r="E10" s="365"/>
+      <c r="F10" s="365"/>
     </row>
     <row r="11" spans="1:12" ht="33.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -12751,14 +12744,14 @@
   <sheetData>
     <row r="1" spans="1:12" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:12" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="370" t="s">
+      <c r="A2" s="375" t="s">
         <v>188</v>
       </c>
-      <c r="B2" s="370"/>
-      <c r="C2" s="370"/>
-      <c r="D2" s="370"/>
-      <c r="E2" s="370"/>
-      <c r="F2" s="370"/>
+      <c r="B2" s="375"/>
+      <c r="C2" s="375"/>
+      <c r="D2" s="375"/>
+      <c r="E2" s="375"/>
+      <c r="F2" s="375"/>
       <c r="H2" s="13"/>
       <c r="I2" s="14" t="s">
         <v>61</v>
@@ -12801,10 +12794,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="11"/>
-      <c r="C5" s="366"/>
-      <c r="D5" s="366"/>
-      <c r="E5" s="366"/>
-      <c r="F5" s="366"/>
+      <c r="C5" s="371"/>
+      <c r="D5" s="371"/>
+      <c r="E5" s="371"/>
+      <c r="F5" s="371"/>
       <c r="H5" s="13"/>
       <c r="I5" s="14" t="s">
         <v>11</v>
@@ -12818,10 +12811,10 @@
         <v>8</v>
       </c>
       <c r="B6" s="11"/>
-      <c r="C6" s="366"/>
-      <c r="D6" s="366"/>
-      <c r="E6" s="366"/>
-      <c r="F6" s="366"/>
+      <c r="C6" s="371"/>
+      <c r="D6" s="371"/>
+      <c r="E6" s="371"/>
+      <c r="F6" s="371"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -12850,30 +12843,30 @@
         <v>0</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="367"/>
-      <c r="D8" s="367"/>
-      <c r="E8" s="367"/>
-      <c r="F8" s="367"/>
+      <c r="C8" s="372"/>
+      <c r="D8" s="372"/>
+      <c r="E8" s="372"/>
+      <c r="F8" s="372"/>
     </row>
     <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="11"/>
-      <c r="C9" s="366"/>
-      <c r="D9" s="366"/>
-      <c r="E9" s="366"/>
-      <c r="F9" s="366"/>
+      <c r="C9" s="371"/>
+      <c r="D9" s="371"/>
+      <c r="E9" s="371"/>
+      <c r="F9" s="371"/>
     </row>
     <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="11"/>
-      <c r="C10" s="366"/>
-      <c r="D10" s="366"/>
-      <c r="E10" s="366"/>
-      <c r="F10" s="366"/>
+      <c r="C10" s="371"/>
+      <c r="D10" s="371"/>
+      <c r="E10" s="371"/>
+      <c r="F10" s="371"/>
     </row>
     <row r="11" spans="1:12" ht="51.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -12893,32 +12886,32 @@
       <c r="L12" s="67"/>
     </row>
     <row r="13" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="371"/>
-      <c r="B13" s="372"/>
-      <c r="C13" s="372"/>
-      <c r="D13" s="372"/>
-      <c r="E13" s="372"/>
-      <c r="F13" s="372"/>
-      <c r="G13" s="372"/>
-      <c r="H13" s="372"/>
-      <c r="I13" s="372"/>
-      <c r="J13" s="372"/>
-      <c r="K13" s="372"/>
-      <c r="L13" s="373"/>
+      <c r="A13" s="376"/>
+      <c r="B13" s="377"/>
+      <c r="C13" s="377"/>
+      <c r="D13" s="377"/>
+      <c r="E13" s="377"/>
+      <c r="F13" s="377"/>
+      <c r="G13" s="377"/>
+      <c r="H13" s="377"/>
+      <c r="I13" s="377"/>
+      <c r="J13" s="377"/>
+      <c r="K13" s="377"/>
+      <c r="L13" s="378"/>
     </row>
     <row r="14" spans="1:12" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="374"/>
-      <c r="B14" s="375"/>
-      <c r="C14" s="375"/>
-      <c r="D14" s="375"/>
-      <c r="E14" s="375"/>
-      <c r="F14" s="375"/>
-      <c r="G14" s="375"/>
-      <c r="H14" s="375"/>
-      <c r="I14" s="375"/>
-      <c r="J14" s="375"/>
-      <c r="K14" s="375"/>
-      <c r="L14" s="376"/>
+      <c r="A14" s="379"/>
+      <c r="B14" s="380"/>
+      <c r="C14" s="380"/>
+      <c r="D14" s="380"/>
+      <c r="E14" s="380"/>
+      <c r="F14" s="380"/>
+      <c r="G14" s="380"/>
+      <c r="H14" s="380"/>
+      <c r="I14" s="380"/>
+      <c r="J14" s="380"/>
+      <c r="K14" s="380"/>
+      <c r="L14" s="381"/>
     </row>
     <row r="15" spans="1:12" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="32" t="s">
@@ -13908,10 +13901,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="11"/>
-      <c r="C5" s="366"/>
-      <c r="D5" s="366"/>
-      <c r="E5" s="366"/>
-      <c r="F5" s="366"/>
+      <c r="C5" s="371"/>
+      <c r="D5" s="371"/>
+      <c r="E5" s="371"/>
+      <c r="F5" s="371"/>
       <c r="H5" s="13"/>
       <c r="I5" s="14" t="s">
         <v>11</v>
@@ -13925,10 +13918,10 @@
         <v>8</v>
       </c>
       <c r="B6" s="11"/>
-      <c r="C6" s="366"/>
-      <c r="D6" s="366"/>
-      <c r="E6" s="366"/>
-      <c r="F6" s="366"/>
+      <c r="C6" s="371"/>
+      <c r="D6" s="371"/>
+      <c r="E6" s="371"/>
+      <c r="F6" s="371"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -13957,30 +13950,30 @@
         <v>0</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="367"/>
-      <c r="D8" s="367"/>
-      <c r="E8" s="367"/>
-      <c r="F8" s="367"/>
+      <c r="C8" s="372"/>
+      <c r="D8" s="372"/>
+      <c r="E8" s="372"/>
+      <c r="F8" s="372"/>
     </row>
     <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="11"/>
-      <c r="C9" s="366"/>
-      <c r="D9" s="366"/>
-      <c r="E9" s="366"/>
-      <c r="F9" s="366"/>
+      <c r="C9" s="371"/>
+      <c r="D9" s="371"/>
+      <c r="E9" s="371"/>
+      <c r="F9" s="371"/>
     </row>
     <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="11"/>
-      <c r="C10" s="366"/>
-      <c r="D10" s="366"/>
-      <c r="E10" s="366"/>
-      <c r="F10" s="366"/>
+      <c r="C10" s="371"/>
+      <c r="D10" s="371"/>
+      <c r="E10" s="371"/>
+      <c r="F10" s="371"/>
     </row>
     <row r="11" spans="1:12" ht="51.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -14000,32 +13993,32 @@
       <c r="L12" s="67"/>
     </row>
     <row r="13" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="371"/>
-      <c r="B13" s="372"/>
-      <c r="C13" s="372"/>
-      <c r="D13" s="372"/>
-      <c r="E13" s="372"/>
-      <c r="F13" s="372"/>
-      <c r="G13" s="372"/>
-      <c r="H13" s="372"/>
-      <c r="I13" s="372"/>
-      <c r="J13" s="372"/>
-      <c r="K13" s="372"/>
-      <c r="L13" s="373"/>
+      <c r="A13" s="376"/>
+      <c r="B13" s="377"/>
+      <c r="C13" s="377"/>
+      <c r="D13" s="377"/>
+      <c r="E13" s="377"/>
+      <c r="F13" s="377"/>
+      <c r="G13" s="377"/>
+      <c r="H13" s="377"/>
+      <c r="I13" s="377"/>
+      <c r="J13" s="377"/>
+      <c r="K13" s="377"/>
+      <c r="L13" s="378"/>
     </row>
     <row r="14" spans="1:12" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="374"/>
-      <c r="B14" s="375"/>
-      <c r="C14" s="375"/>
-      <c r="D14" s="375"/>
-      <c r="E14" s="375"/>
-      <c r="F14" s="375"/>
-      <c r="G14" s="375"/>
-      <c r="H14" s="375"/>
-      <c r="I14" s="375"/>
-      <c r="J14" s="375"/>
-      <c r="K14" s="375"/>
-      <c r="L14" s="376"/>
+      <c r="A14" s="379"/>
+      <c r="B14" s="380"/>
+      <c r="C14" s="380"/>
+      <c r="D14" s="380"/>
+      <c r="E14" s="380"/>
+      <c r="F14" s="380"/>
+      <c r="G14" s="380"/>
+      <c r="H14" s="380"/>
+      <c r="I14" s="380"/>
+      <c r="J14" s="380"/>
+      <c r="K14" s="380"/>
+      <c r="L14" s="381"/>
     </row>
     <row r="15" spans="1:12" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="32" t="s">
@@ -14906,14 +14899,14 @@
   <sheetData>
     <row r="1" spans="1:12" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="370" t="s">
+      <c r="A2" s="375" t="s">
         <v>190</v>
       </c>
-      <c r="B2" s="370"/>
-      <c r="C2" s="370"/>
-      <c r="D2" s="370"/>
-      <c r="E2" s="370"/>
-      <c r="F2" s="370"/>
+      <c r="B2" s="375"/>
+      <c r="C2" s="375"/>
+      <c r="D2" s="375"/>
+      <c r="E2" s="375"/>
+      <c r="F2" s="375"/>
       <c r="H2" s="13"/>
       <c r="I2" s="14" t="s">
         <v>61</v>
@@ -14956,10 +14949,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="11"/>
-      <c r="C5" s="366"/>
-      <c r="D5" s="366"/>
-      <c r="E5" s="366"/>
-      <c r="F5" s="366"/>
+      <c r="C5" s="371"/>
+      <c r="D5" s="371"/>
+      <c r="E5" s="371"/>
+      <c r="F5" s="371"/>
       <c r="H5" s="13"/>
       <c r="I5" s="14" t="s">
         <v>11</v>
@@ -14973,10 +14966,10 @@
         <v>8</v>
       </c>
       <c r="B6" s="11"/>
-      <c r="C6" s="366"/>
-      <c r="D6" s="366"/>
-      <c r="E6" s="366"/>
-      <c r="F6" s="366"/>
+      <c r="C6" s="371"/>
+      <c r="D6" s="371"/>
+      <c r="E6" s="371"/>
+      <c r="F6" s="371"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -15005,30 +14998,30 @@
         <v>0</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="367"/>
-      <c r="D8" s="367"/>
-      <c r="E8" s="367"/>
-      <c r="F8" s="367"/>
+      <c r="C8" s="372"/>
+      <c r="D8" s="372"/>
+      <c r="E8" s="372"/>
+      <c r="F8" s="372"/>
     </row>
     <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="11"/>
-      <c r="C9" s="366"/>
-      <c r="D9" s="366"/>
-      <c r="E9" s="366"/>
-      <c r="F9" s="366"/>
+      <c r="C9" s="371"/>
+      <c r="D9" s="371"/>
+      <c r="E9" s="371"/>
+      <c r="F9" s="371"/>
     </row>
     <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="11"/>
-      <c r="C10" s="366"/>
-      <c r="D10" s="366"/>
-      <c r="E10" s="366"/>
-      <c r="F10" s="366"/>
+      <c r="C10" s="371"/>
+      <c r="D10" s="371"/>
+      <c r="E10" s="371"/>
+      <c r="F10" s="371"/>
     </row>
     <row r="11" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -15041,19 +15034,19 @@
       </c>
     </row>
     <row r="14" spans="1:12" ht="59.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="377" t="s">
+      <c r="A14" s="382" t="s">
         <v>149</v>
       </c>
-      <c r="B14" s="379" t="s">
+      <c r="B14" s="384" t="s">
         <v>108</v>
       </c>
-      <c r="C14" s="380"/>
-      <c r="D14" s="380"/>
-      <c r="E14" s="380"/>
-      <c r="F14" s="380"/>
-      <c r="G14" s="380"/>
-      <c r="H14" s="380"/>
-      <c r="I14" s="381"/>
+      <c r="C14" s="385"/>
+      <c r="D14" s="385"/>
+      <c r="E14" s="385"/>
+      <c r="F14" s="385"/>
+      <c r="G14" s="385"/>
+      <c r="H14" s="385"/>
+      <c r="I14" s="386"/>
       <c r="J14" s="18" t="s">
         <v>144</v>
       </c>
@@ -15064,17 +15057,17 @@
       </c>
     </row>
     <row r="15" spans="1:12" ht="69" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="378"/>
-      <c r="B15" s="382" t="s">
+      <c r="A15" s="383"/>
+      <c r="B15" s="387" t="s">
         <v>169</v>
       </c>
-      <c r="C15" s="383"/>
-      <c r="D15" s="383"/>
-      <c r="E15" s="383"/>
-      <c r="F15" s="383"/>
-      <c r="G15" s="383"/>
-      <c r="H15" s="383"/>
-      <c r="I15" s="383"/>
+      <c r="C15" s="388"/>
+      <c r="D15" s="388"/>
+      <c r="E15" s="388"/>
+      <c r="F15" s="388"/>
+      <c r="G15" s="388"/>
+      <c r="H15" s="388"/>
+      <c r="I15" s="388"/>
       <c r="J15" s="20" t="s">
         <v>145</v>
       </c>
@@ -15085,19 +15078,19 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="384" t="s">
+      <c r="A16" s="389" t="s">
         <v>150</v>
       </c>
-      <c r="B16" s="386" t="s">
+      <c r="B16" s="391" t="s">
         <v>147</v>
       </c>
-      <c r="C16" s="387"/>
-      <c r="D16" s="387"/>
-      <c r="E16" s="387"/>
-      <c r="F16" s="387"/>
-      <c r="G16" s="387"/>
-      <c r="H16" s="387"/>
-      <c r="I16" s="387"/>
+      <c r="C16" s="392"/>
+      <c r="D16" s="392"/>
+      <c r="E16" s="392"/>
+      <c r="F16" s="392"/>
+      <c r="G16" s="392"/>
+      <c r="H16" s="392"/>
+      <c r="I16" s="392"/>
       <c r="J16" s="18" t="s">
         <v>141</v>
       </c>
@@ -15108,17 +15101,17 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="80.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="385"/>
-      <c r="B17" s="388" t="s">
+      <c r="A17" s="390"/>
+      <c r="B17" s="393" t="s">
         <v>143</v>
       </c>
-      <c r="C17" s="389"/>
-      <c r="D17" s="389"/>
-      <c r="E17" s="389"/>
-      <c r="F17" s="389"/>
-      <c r="G17" s="389"/>
-      <c r="H17" s="389"/>
-      <c r="I17" s="389"/>
+      <c r="C17" s="394"/>
+      <c r="D17" s="394"/>
+      <c r="E17" s="394"/>
+      <c r="F17" s="394"/>
+      <c r="G17" s="394"/>
+      <c r="H17" s="394"/>
+      <c r="I17" s="394"/>
       <c r="J17" s="19" t="s">
         <v>146</v>
       </c>
@@ -15262,15 +15255,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100570C130F412EDB4EBF3E80DF6A9149FD" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cfaa3b10b9be17ef9f56bd19dc71004c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ddb0c952b897a810c8a4e377cff6bff8" ns1:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -15336,6 +15320,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28A807C1-6DB8-4C6A-8DCB-8B5F61EFE299}">
   <ds:schemaRefs>
@@ -15345,21 +15338,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF64F18F-372D-43EC-AE22-C51BFB121B01}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A00BD0D-8423-4FFE-92A4-D273D2078383}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15374,4 +15352,19 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF64F18F-372D-43EC-AE22-C51BFB121B01}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fix av formler Kontroll av att det är siffror som matas in
</commit_message>
<xml_diff>
--- a/mallar/Protokoll/Protokoll 2019 individuell klass_(mall).xlsx
+++ b/mallar/Protokoll/Protokoll 2019 individuell klass_(mall).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28324"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\episerver\voltige\VoltigeClosedXML\mallar\Protokoll\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69004016-1765-42FD-8C4F-E78FB020941C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58F562D3-2DC2-4A94-AEA0-6B5B9B2E15B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43080" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="966" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43080" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="966" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="37" r:id="rId1"/>
@@ -3169,206 +3169,43 @@
     <xf numFmtId="172" fontId="1" fillId="2" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="14" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="61" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="45" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="11" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="11" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="23" fillId="0" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="55" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="23" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="56" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="66" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="58" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="58" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="59" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="48" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="24" xfId="3" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="55" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="25" xfId="3" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="58" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="59" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="49" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="56" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="59" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="45" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="58" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="59" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="57" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="64" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="65" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="23" fillId="0" borderId="51" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="40" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="28" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="40" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="41" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="53" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="50" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="45" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="56" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="63" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="59" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="55" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="56" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="58" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="59" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="23" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="2" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="2" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="46" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -3378,6 +3215,207 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="40" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="19" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="28" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="40" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="41" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="53" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="50" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="45" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="56" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="63" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="59" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="55" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="56" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="58" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="59" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="23" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="2" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="2" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="57" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="46" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="14" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="61" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="47" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="45" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="55" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="56" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="58" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="59" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="55" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="58" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="49" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="56" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="59" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="45" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="54" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="49" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="58" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="59" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="48" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="64" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="65" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="23" fillId="0" borderId="51" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="166" fontId="1" fillId="2" borderId="35" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -3390,82 +3428,50 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="9" fontId="23" fillId="0" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="23" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="66" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="58" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="48" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="24" xfId="3" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="25" xfId="3" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="59" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="8" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="8" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3494,6 +3500,24 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3650,6 +3674,18 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="19" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3689,18 +3725,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="19" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="justify" wrapText="1"/>
     </xf>
@@ -3709,30 +3733,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="justify" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="11" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="11" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -5734,8 +5734,8 @@
   </sheetPr>
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView showZeros="0" view="pageLayout" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:I16"/>
+    <sheetView showZeros="0" view="pageLayout" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
@@ -6374,10 +6374,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="11"/>
-      <c r="C5" s="394"/>
-      <c r="D5" s="394"/>
-      <c r="E5" s="394"/>
-      <c r="F5" s="394"/>
+      <c r="C5" s="396"/>
+      <c r="D5" s="396"/>
+      <c r="E5" s="396"/>
+      <c r="F5" s="396"/>
       <c r="H5" s="13"/>
       <c r="I5" s="14" t="s">
         <v>11</v>
@@ -6391,10 +6391,10 @@
         <v>8</v>
       </c>
       <c r="B6" s="11"/>
-      <c r="C6" s="394"/>
-      <c r="D6" s="394"/>
-      <c r="E6" s="394"/>
-      <c r="F6" s="394"/>
+      <c r="C6" s="396"/>
+      <c r="D6" s="396"/>
+      <c r="E6" s="396"/>
+      <c r="F6" s="396"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -6423,30 +6423,30 @@
         <v>0</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="395"/>
-      <c r="D8" s="395"/>
-      <c r="E8" s="395"/>
-      <c r="F8" s="395"/>
+      <c r="C8" s="397"/>
+      <c r="D8" s="397"/>
+      <c r="E8" s="397"/>
+      <c r="F8" s="397"/>
     </row>
     <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="11"/>
-      <c r="C9" s="394"/>
-      <c r="D9" s="394"/>
-      <c r="E9" s="394"/>
-      <c r="F9" s="394"/>
+      <c r="C9" s="396"/>
+      <c r="D9" s="396"/>
+      <c r="E9" s="396"/>
+      <c r="F9" s="396"/>
     </row>
     <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="11"/>
-      <c r="C10" s="394"/>
-      <c r="D10" s="394"/>
-      <c r="E10" s="394"/>
-      <c r="F10" s="394"/>
+      <c r="C10" s="396"/>
+      <c r="D10" s="396"/>
+      <c r="E10" s="396"/>
+      <c r="F10" s="396"/>
     </row>
     <row r="11" spans="1:12" ht="8.65" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:12" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -6460,16 +6460,16 @@
       <c r="A13" s="283" t="s">
         <v>178</v>
       </c>
-      <c r="B13" s="424" t="s">
+      <c r="B13" s="432" t="s">
         <v>179</v>
       </c>
-      <c r="C13" s="425"/>
-      <c r="D13" s="425"/>
-      <c r="E13" s="425"/>
-      <c r="F13" s="425"/>
-      <c r="G13" s="425"/>
-      <c r="H13" s="425"/>
-      <c r="I13" s="426"/>
+      <c r="C13" s="433"/>
+      <c r="D13" s="433"/>
+      <c r="E13" s="433"/>
+      <c r="F13" s="433"/>
+      <c r="G13" s="433"/>
+      <c r="H13" s="433"/>
+      <c r="I13" s="434"/>
       <c r="J13" s="18" t="s">
         <v>180</v>
       </c>
@@ -6480,96 +6480,88 @@
       </c>
     </row>
     <row r="14" spans="1:12" ht="91.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="408" t="s">
+      <c r="A14" s="416" t="s">
         <v>141</v>
       </c>
-      <c r="B14" s="410" t="s">
+      <c r="B14" s="418" t="s">
         <v>181</v>
       </c>
-      <c r="C14" s="411"/>
-      <c r="D14" s="411"/>
-      <c r="E14" s="411"/>
-      <c r="F14" s="411"/>
-      <c r="G14" s="411"/>
-      <c r="H14" s="411"/>
-      <c r="I14" s="412"/>
+      <c r="C14" s="419"/>
+      <c r="D14" s="419"/>
+      <c r="E14" s="419"/>
+      <c r="F14" s="419"/>
+      <c r="G14" s="419"/>
+      <c r="H14" s="419"/>
+      <c r="I14" s="420"/>
       <c r="J14" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="K14" s="250">
-        <v>0</v>
-      </c>
+      <c r="K14" s="250"/>
       <c r="L14" s="147">
         <f>K14*0.2</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="123" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="430"/>
-      <c r="B15" s="431" t="s">
+      <c r="A15" s="438"/>
+      <c r="B15" s="439" t="s">
         <v>182</v>
       </c>
-      <c r="C15" s="414"/>
-      <c r="D15" s="414"/>
-      <c r="E15" s="414"/>
-      <c r="F15" s="414"/>
-      <c r="G15" s="414"/>
-      <c r="H15" s="414"/>
-      <c r="I15" s="415"/>
+      <c r="C15" s="422"/>
+      <c r="D15" s="422"/>
+      <c r="E15" s="422"/>
+      <c r="F15" s="422"/>
+      <c r="G15" s="422"/>
+      <c r="H15" s="422"/>
+      <c r="I15" s="423"/>
       <c r="J15" s="20" t="s">
         <v>185</v>
       </c>
-      <c r="K15" s="251">
-        <v>0</v>
-      </c>
+      <c r="K15" s="251"/>
       <c r="L15" s="233">
         <f>K15*0.1</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="85.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="408" t="s">
+      <c r="A16" s="416" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="427" t="s">
+      <c r="B16" s="435" t="s">
         <v>183</v>
       </c>
-      <c r="C16" s="428"/>
-      <c r="D16" s="428"/>
-      <c r="E16" s="428"/>
-      <c r="F16" s="428"/>
-      <c r="G16" s="428"/>
-      <c r="H16" s="428"/>
-      <c r="I16" s="429"/>
+      <c r="C16" s="436"/>
+      <c r="D16" s="436"/>
+      <c r="E16" s="436"/>
+      <c r="F16" s="436"/>
+      <c r="G16" s="436"/>
+      <c r="H16" s="436"/>
+      <c r="I16" s="437"/>
       <c r="J16" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="K16" s="252">
-        <v>0</v>
-      </c>
+      <c r="K16" s="252"/>
       <c r="L16" s="145">
         <f>K16*0.25</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="409"/>
-      <c r="B17" s="421" t="s">
+      <c r="A17" s="417"/>
+      <c r="B17" s="429" t="s">
         <v>184</v>
       </c>
-      <c r="C17" s="422"/>
-      <c r="D17" s="422"/>
-      <c r="E17" s="422"/>
-      <c r="F17" s="422"/>
-      <c r="G17" s="422"/>
-      <c r="H17" s="422"/>
-      <c r="I17" s="423"/>
+      <c r="C17" s="430"/>
+      <c r="D17" s="430"/>
+      <c r="E17" s="430"/>
+      <c r="F17" s="430"/>
+      <c r="G17" s="430"/>
+      <c r="H17" s="430"/>
+      <c r="I17" s="431"/>
       <c r="J17" s="19" t="s">
         <v>187</v>
       </c>
-      <c r="K17" s="253">
-        <v>0</v>
-      </c>
+      <c r="K17" s="253"/>
       <c r="L17" s="143">
         <f>K17*0.25</f>
         <v>0</v>
@@ -6588,7 +6580,7 @@
       <c r="J18" s="21"/>
       <c r="K18" s="21"/>
       <c r="L18" s="53">
-        <f>SUM(L14:L17)</f>
+        <f>SUM(L13:L17)</f>
         <v>0</v>
       </c>
       <c r="M18" s="21"/>
@@ -6689,6 +6681,12 @@
     <mergeCell ref="B15:I15"/>
     <mergeCell ref="B13:I13"/>
   </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Du kan endast mata in siffror mellan 0 och 10. Var noga med punkt eller komma beroende på språk" sqref="K13:K17 L20" xr:uid="{4161595A-2953-4F7B-837A-33E2B7048019}">
+      <formula1>1</formula1>
+      <formula2>10</formula2>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" scale="94" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
@@ -6707,7 +6705,7 @@
   </sheetPr>
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView showZeros="0" view="pageLayout" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showZeros="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
@@ -7342,10 +7340,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="11"/>
-      <c r="C5" s="394"/>
-      <c r="D5" s="394"/>
-      <c r="E5" s="394"/>
-      <c r="F5" s="394"/>
+      <c r="C5" s="396"/>
+      <c r="D5" s="396"/>
+      <c r="E5" s="396"/>
+      <c r="F5" s="396"/>
       <c r="H5" s="13"/>
       <c r="I5" s="14" t="s">
         <v>11</v>
@@ -7359,10 +7357,10 @@
         <v>8</v>
       </c>
       <c r="B6" s="11"/>
-      <c r="C6" s="394"/>
-      <c r="D6" s="394"/>
-      <c r="E6" s="394"/>
-      <c r="F6" s="394"/>
+      <c r="C6" s="396"/>
+      <c r="D6" s="396"/>
+      <c r="E6" s="396"/>
+      <c r="F6" s="396"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -7391,30 +7389,30 @@
         <v>0</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="395"/>
-      <c r="D8" s="395"/>
-      <c r="E8" s="395"/>
-      <c r="F8" s="395"/>
+      <c r="C8" s="397"/>
+      <c r="D8" s="397"/>
+      <c r="E8" s="397"/>
+      <c r="F8" s="397"/>
     </row>
     <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="11"/>
-      <c r="C9" s="394"/>
-      <c r="D9" s="394"/>
-      <c r="E9" s="394"/>
-      <c r="F9" s="394"/>
+      <c r="C9" s="396"/>
+      <c r="D9" s="396"/>
+      <c r="E9" s="396"/>
+      <c r="F9" s="396"/>
     </row>
     <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="11"/>
-      <c r="C10" s="394"/>
-      <c r="D10" s="394"/>
-      <c r="E10" s="394"/>
-      <c r="F10" s="394"/>
+      <c r="C10" s="396"/>
+      <c r="D10" s="396"/>
+      <c r="E10" s="396"/>
+      <c r="F10" s="396"/>
     </row>
     <row r="11" spans="1:12" ht="10.15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:12" ht="22.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -7428,16 +7426,16 @@
       <c r="A13" s="283" t="s">
         <v>178</v>
       </c>
-      <c r="B13" s="424" t="s">
+      <c r="B13" s="432" t="s">
         <v>179</v>
       </c>
-      <c r="C13" s="425"/>
-      <c r="D13" s="425"/>
-      <c r="E13" s="425"/>
-      <c r="F13" s="425"/>
-      <c r="G13" s="425"/>
-      <c r="H13" s="425"/>
-      <c r="I13" s="426"/>
+      <c r="C13" s="433"/>
+      <c r="D13" s="433"/>
+      <c r="E13" s="433"/>
+      <c r="F13" s="433"/>
+      <c r="G13" s="433"/>
+      <c r="H13" s="433"/>
+      <c r="I13" s="434"/>
       <c r="J13" s="18" t="s">
         <v>180</v>
       </c>
@@ -7448,96 +7446,88 @@
       </c>
     </row>
     <row r="14" spans="1:12" ht="85.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="408" t="s">
+      <c r="A14" s="416" t="s">
         <v>141</v>
       </c>
-      <c r="B14" s="410" t="s">
+      <c r="B14" s="418" t="s">
         <v>181</v>
       </c>
-      <c r="C14" s="411"/>
-      <c r="D14" s="411"/>
-      <c r="E14" s="411"/>
-      <c r="F14" s="411"/>
-      <c r="G14" s="411"/>
-      <c r="H14" s="411"/>
-      <c r="I14" s="412"/>
+      <c r="C14" s="419"/>
+      <c r="D14" s="419"/>
+      <c r="E14" s="419"/>
+      <c r="F14" s="419"/>
+      <c r="G14" s="419"/>
+      <c r="H14" s="419"/>
+      <c r="I14" s="420"/>
       <c r="J14" s="18" t="s">
         <v>200</v>
       </c>
-      <c r="K14" s="250">
-        <v>0</v>
-      </c>
+      <c r="K14" s="250"/>
       <c r="L14" s="147">
         <f>K14*0.1</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="110.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="430"/>
-      <c r="B15" s="410" t="s">
+      <c r="A15" s="438"/>
+      <c r="B15" s="418" t="s">
         <v>198</v>
       </c>
-      <c r="C15" s="411"/>
-      <c r="D15" s="411"/>
-      <c r="E15" s="411"/>
-      <c r="F15" s="411"/>
-      <c r="G15" s="411"/>
-      <c r="H15" s="411"/>
-      <c r="I15" s="412"/>
+      <c r="C15" s="419"/>
+      <c r="D15" s="419"/>
+      <c r="E15" s="419"/>
+      <c r="F15" s="419"/>
+      <c r="G15" s="419"/>
+      <c r="H15" s="419"/>
+      <c r="I15" s="420"/>
       <c r="J15" s="20" t="s">
         <v>185</v>
       </c>
-      <c r="K15" s="251">
-        <v>0</v>
-      </c>
+      <c r="K15" s="251"/>
       <c r="L15" s="233">
         <f>K15*0.1</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="85.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="408" t="s">
+      <c r="A16" s="416" t="s">
         <v>142</v>
       </c>
-      <c r="B16" s="427" t="s">
+      <c r="B16" s="435" t="s">
         <v>183</v>
       </c>
-      <c r="C16" s="428"/>
-      <c r="D16" s="428"/>
-      <c r="E16" s="428"/>
-      <c r="F16" s="428"/>
-      <c r="G16" s="428"/>
-      <c r="H16" s="428"/>
-      <c r="I16" s="429"/>
+      <c r="C16" s="436"/>
+      <c r="D16" s="436"/>
+      <c r="E16" s="436"/>
+      <c r="F16" s="436"/>
+      <c r="G16" s="436"/>
+      <c r="H16" s="436"/>
+      <c r="I16" s="437"/>
       <c r="J16" s="18" t="s">
         <v>201</v>
       </c>
-      <c r="K16" s="252">
-        <v>0</v>
-      </c>
+      <c r="K16" s="252"/>
       <c r="L16" s="145">
         <f>K16*0.3</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="409"/>
-      <c r="B17" s="421" t="s">
+      <c r="A17" s="417"/>
+      <c r="B17" s="429" t="s">
         <v>199</v>
       </c>
-      <c r="C17" s="422"/>
-      <c r="D17" s="422"/>
-      <c r="E17" s="422"/>
-      <c r="F17" s="422"/>
-      <c r="G17" s="422"/>
-      <c r="H17" s="422"/>
-      <c r="I17" s="423"/>
+      <c r="C17" s="430"/>
+      <c r="D17" s="430"/>
+      <c r="E17" s="430"/>
+      <c r="F17" s="430"/>
+      <c r="G17" s="430"/>
+      <c r="H17" s="430"/>
+      <c r="I17" s="431"/>
       <c r="J17" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="K17" s="253">
-        <v>0</v>
-      </c>
+      <c r="K17" s="253"/>
       <c r="L17" s="143">
         <f>K17*0.3</f>
         <v>0</v>
@@ -7556,7 +7546,7 @@
       <c r="J18" s="21"/>
       <c r="K18" s="21"/>
       <c r="L18" s="53">
-        <f>SUM(L14:L17)</f>
+        <f>SUM(L13:L17)</f>
         <v>0</v>
       </c>
       <c r="M18" s="21"/>
@@ -7642,6 +7632,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C10:F10"/>
     <mergeCell ref="B13:I13"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="B14:I14"/>
@@ -7649,12 +7644,13 @@
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="B16:I16"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="C10:F10"/>
   </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Du kan endast mata in siffror mellan 0 och 10. Var noga med punkt eller komma beroende på språk" sqref="K13 K14 K15 K16 K17 L20" xr:uid="{D6E2C8F8-7AAD-4E82-B818-AA02695B4DF9}">
+      <formula1>1</formula1>
+      <formula2>10</formula2>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
@@ -7738,10 +7734,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="11"/>
-      <c r="C5" s="394"/>
-      <c r="D5" s="394"/>
-      <c r="E5" s="394"/>
-      <c r="F5" s="394"/>
+      <c r="C5" s="396"/>
+      <c r="D5" s="396"/>
+      <c r="E5" s="396"/>
+      <c r="F5" s="396"/>
       <c r="H5" s="13"/>
       <c r="I5" s="14" t="s">
         <v>11</v>
@@ -7755,10 +7751,10 @@
         <v>8</v>
       </c>
       <c r="B6" s="11"/>
-      <c r="C6" s="394"/>
-      <c r="D6" s="394"/>
-      <c r="E6" s="394"/>
-      <c r="F6" s="394"/>
+      <c r="C6" s="396"/>
+      <c r="D6" s="396"/>
+      <c r="E6" s="396"/>
+      <c r="F6" s="396"/>
       <c r="K6" s="30"/>
     </row>
     <row r="7" spans="1:12" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -7781,30 +7777,30 @@
         <v>0</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="395"/>
-      <c r="D8" s="395"/>
-      <c r="E8" s="395"/>
-      <c r="F8" s="395"/>
+      <c r="C8" s="397"/>
+      <c r="D8" s="397"/>
+      <c r="E8" s="397"/>
+      <c r="F8" s="397"/>
     </row>
     <row r="9" spans="1:12" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="11"/>
-      <c r="C9" s="394"/>
-      <c r="D9" s="394"/>
-      <c r="E9" s="394"/>
-      <c r="F9" s="394"/>
+      <c r="C9" s="396"/>
+      <c r="D9" s="396"/>
+      <c r="E9" s="396"/>
+      <c r="F9" s="396"/>
     </row>
     <row r="10" spans="1:12" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="11"/>
-      <c r="C10" s="394"/>
-      <c r="D10" s="394"/>
-      <c r="E10" s="394"/>
-      <c r="F10" s="394"/>
+      <c r="C10" s="396"/>
+      <c r="D10" s="396"/>
+      <c r="E10" s="396"/>
+      <c r="F10" s="396"/>
     </row>
     <row r="11" spans="1:12" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:12" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -7830,14 +7826,14 @@
       </c>
     </row>
     <row r="15" spans="1:12" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="432" t="s">
+      <c r="A15" s="440" t="s">
         <v>164</v>
       </c>
-      <c r="B15" s="433"/>
-      <c r="C15" s="433"/>
-      <c r="D15" s="433"/>
-      <c r="E15" s="433"/>
-      <c r="F15" s="434"/>
+      <c r="B15" s="441"/>
+      <c r="C15" s="441"/>
+      <c r="D15" s="441"/>
+      <c r="E15" s="441"/>
+      <c r="F15" s="442"/>
       <c r="G15" s="33"/>
       <c r="H15" s="33"/>
       <c r="I15" s="11"/>
@@ -7846,14 +7842,14 @@
       <c r="L15" s="245"/>
     </row>
     <row r="16" spans="1:12" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="435" t="s">
+      <c r="A16" s="443" t="s">
         <v>158</v>
       </c>
-      <c r="B16" s="436"/>
-      <c r="C16" s="436"/>
-      <c r="D16" s="436"/>
-      <c r="E16" s="436"/>
-      <c r="F16" s="437"/>
+      <c r="B16" s="444"/>
+      <c r="C16" s="444"/>
+      <c r="D16" s="444"/>
+      <c r="E16" s="444"/>
+      <c r="F16" s="445"/>
       <c r="G16" s="33"/>
       <c r="H16" s="33"/>
       <c r="I16" s="11"/>
@@ -7914,27 +7910,27 @@
       <c r="L20" s="138"/>
     </row>
     <row r="21" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="441" t="s">
+      <c r="A21" s="449" t="s">
         <v>65</v>
       </c>
-      <c r="B21" s="442"/>
-      <c r="C21" s="442"/>
-      <c r="D21" s="442"/>
-      <c r="E21" s="442"/>
-      <c r="F21" s="442"/>
-      <c r="G21" s="442"/>
-      <c r="H21" s="442"/>
-      <c r="I21" s="442"/>
+      <c r="B21" s="450"/>
+      <c r="C21" s="450"/>
+      <c r="D21" s="450"/>
+      <c r="E21" s="450"/>
+      <c r="F21" s="450"/>
+      <c r="G21" s="450"/>
+      <c r="H21" s="450"/>
+      <c r="I21" s="450"/>
       <c r="J21" s="137"/>
       <c r="K21" s="136"/>
       <c r="L21" s="8"/>
       <c r="R21" s="131"/>
     </row>
     <row r="22" spans="1:18" ht="66" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="449" t="s">
+      <c r="A22" s="457" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="450"/>
+      <c r="B22" s="458"/>
       <c r="C22" s="135"/>
       <c r="D22" s="135"/>
       <c r="E22" s="135"/>
@@ -7948,15 +7944,15 @@
       <c r="R22" s="131"/>
     </row>
     <row r="23" spans="1:18" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="445" t="s">
+      <c r="A23" s="453" t="s">
         <v>54</v>
       </c>
-      <c r="B23" s="446"/>
+      <c r="B23" s="454"/>
       <c r="C23" s="254"/>
-      <c r="D23" s="443" t="s">
+      <c r="D23" s="451" t="s">
         <v>47</v>
       </c>
-      <c r="E23" s="444"/>
+      <c r="E23" s="452"/>
       <c r="F23" s="255"/>
       <c r="G23" s="214" t="s">
         <v>64</v>
@@ -7979,11 +7975,11 @@
       <c r="R23" s="131"/>
     </row>
     <row r="24" spans="1:18" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="447" t="s">
+      <c r="A24" s="455" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="448"/>
-      <c r="C24" s="448"/>
+      <c r="B24" s="456"/>
+      <c r="C24" s="456"/>
       <c r="D24" s="218"/>
       <c r="E24" s="218"/>
       <c r="F24" s="218"/>
@@ -7995,19 +7991,19 @@
       <c r="R24" s="131"/>
     </row>
     <row r="25" spans="1:18" ht="16.350000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="438" t="s">
+      <c r="A25" s="446" t="s">
         <v>56</v>
       </c>
-      <c r="B25" s="439"/>
-      <c r="C25" s="439"/>
-      <c r="D25" s="439"/>
-      <c r="E25" s="439"/>
-      <c r="F25" s="439"/>
-      <c r="G25" s="439"/>
-      <c r="H25" s="439"/>
-      <c r="I25" s="439"/>
-      <c r="J25" s="439"/>
-      <c r="K25" s="440"/>
+      <c r="B25" s="447"/>
+      <c r="C25" s="447"/>
+      <c r="D25" s="447"/>
+      <c r="E25" s="447"/>
+      <c r="F25" s="447"/>
+      <c r="G25" s="447"/>
+      <c r="H25" s="447"/>
+      <c r="I25" s="447"/>
+      <c r="J25" s="447"/>
+      <c r="K25" s="448"/>
       <c r="L25" s="9">
         <f>IFERROR(K23-K24,0)</f>
         <v>0</v>
@@ -8139,6 +8135,16 @@
     <mergeCell ref="C9:F9"/>
     <mergeCell ref="C10:F10"/>
   </mergeCells>
+  <dataValidations count="2">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Du kan endast mata in siffror mellan 0 och 10. Var noga med punkt eller komma beroende på språk" sqref="L15:L19" xr:uid="{924DC316-F573-4895-AFCD-D14BE73F69A0}">
+      <formula1>1</formula1>
+      <formula2>10</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Du kan endast mata in siffror. Var noga med punkt eller komma beroende på språk" sqref="C23 F23 K24" xr:uid="{AC54A561-64AF-48D6-AEDB-6E880CE3EDA4}">
+      <formula1>0</formula1>
+      <formula2>100000</formula2>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" scale="99" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
@@ -8221,10 +8227,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="11"/>
-      <c r="C5" s="394"/>
-      <c r="D5" s="394"/>
-      <c r="E5" s="394"/>
-      <c r="F5" s="394"/>
+      <c r="C5" s="396"/>
+      <c r="D5" s="396"/>
+      <c r="E5" s="396"/>
+      <c r="F5" s="396"/>
       <c r="H5" s="13"/>
       <c r="I5" s="14" t="s">
         <v>11</v>
@@ -8238,10 +8244,10 @@
         <v>8</v>
       </c>
       <c r="B6" s="11"/>
-      <c r="C6" s="394"/>
-      <c r="D6" s="394"/>
-      <c r="E6" s="394"/>
-      <c r="F6" s="394"/>
+      <c r="C6" s="396"/>
+      <c r="D6" s="396"/>
+      <c r="E6" s="396"/>
+      <c r="F6" s="396"/>
       <c r="K6" s="30"/>
     </row>
     <row r="7" spans="1:12" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -8264,30 +8270,30 @@
         <v>0</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="395"/>
-      <c r="D8" s="395"/>
-      <c r="E8" s="395"/>
-      <c r="F8" s="395"/>
+      <c r="C8" s="397"/>
+      <c r="D8" s="397"/>
+      <c r="E8" s="397"/>
+      <c r="F8" s="397"/>
     </row>
     <row r="9" spans="1:12" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="11"/>
-      <c r="C9" s="394"/>
-      <c r="D9" s="394"/>
-      <c r="E9" s="394"/>
-      <c r="F9" s="394"/>
+      <c r="C9" s="396"/>
+      <c r="D9" s="396"/>
+      <c r="E9" s="396"/>
+      <c r="F9" s="396"/>
     </row>
     <row r="10" spans="1:12" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="11"/>
-      <c r="C10" s="394"/>
-      <c r="D10" s="394"/>
-      <c r="E10" s="394"/>
-      <c r="F10" s="394"/>
+      <c r="C10" s="396"/>
+      <c r="D10" s="396"/>
+      <c r="E10" s="396"/>
+      <c r="F10" s="396"/>
     </row>
     <row r="11" spans="1:12" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:12" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -8313,14 +8319,14 @@
       </c>
     </row>
     <row r="15" spans="1:12" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="432" t="s">
+      <c r="A15" s="440" t="s">
         <v>164</v>
       </c>
-      <c r="B15" s="433"/>
-      <c r="C15" s="433"/>
-      <c r="D15" s="433"/>
-      <c r="E15" s="433"/>
-      <c r="F15" s="434"/>
+      <c r="B15" s="441"/>
+      <c r="C15" s="441"/>
+      <c r="D15" s="441"/>
+      <c r="E15" s="441"/>
+      <c r="F15" s="442"/>
       <c r="G15" s="33"/>
       <c r="H15" s="33"/>
       <c r="I15" s="11"/>
@@ -8329,14 +8335,14 @@
       <c r="L15" s="245"/>
     </row>
     <row r="16" spans="1:12" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="435" t="s">
+      <c r="A16" s="443" t="s">
         <v>158</v>
       </c>
-      <c r="B16" s="436"/>
-      <c r="C16" s="436"/>
-      <c r="D16" s="436"/>
-      <c r="E16" s="436"/>
-      <c r="F16" s="437"/>
+      <c r="B16" s="444"/>
+      <c r="C16" s="444"/>
+      <c r="D16" s="444"/>
+      <c r="E16" s="444"/>
+      <c r="F16" s="445"/>
       <c r="G16" s="33"/>
       <c r="H16" s="33"/>
       <c r="I16" s="11"/>
@@ -8397,27 +8403,27 @@
       <c r="L20" s="138"/>
     </row>
     <row r="21" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="441" t="s">
+      <c r="A21" s="449" t="s">
         <v>65</v>
       </c>
-      <c r="B21" s="442"/>
-      <c r="C21" s="442"/>
-      <c r="D21" s="442"/>
-      <c r="E21" s="442"/>
-      <c r="F21" s="442"/>
-      <c r="G21" s="442"/>
-      <c r="H21" s="442"/>
-      <c r="I21" s="442"/>
+      <c r="B21" s="450"/>
+      <c r="C21" s="450"/>
+      <c r="D21" s="450"/>
+      <c r="E21" s="450"/>
+      <c r="F21" s="450"/>
+      <c r="G21" s="450"/>
+      <c r="H21" s="450"/>
+      <c r="I21" s="450"/>
       <c r="J21" s="137"/>
       <c r="K21" s="136"/>
       <c r="L21" s="8"/>
       <c r="R21" s="131"/>
     </row>
     <row r="22" spans="1:18" ht="66" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="449" t="s">
+      <c r="A22" s="457" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="450"/>
+      <c r="B22" s="458"/>
       <c r="C22" s="135"/>
       <c r="D22" s="135"/>
       <c r="E22" s="135"/>
@@ -8431,15 +8437,15 @@
       <c r="R22" s="131"/>
     </row>
     <row r="23" spans="1:18" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="445" t="s">
+      <c r="A23" s="453" t="s">
         <v>54</v>
       </c>
-      <c r="B23" s="446"/>
+      <c r="B23" s="454"/>
       <c r="C23" s="254"/>
-      <c r="D23" s="443" t="s">
+      <c r="D23" s="451" t="s">
         <v>47</v>
       </c>
-      <c r="E23" s="444"/>
+      <c r="E23" s="452"/>
       <c r="F23" s="255"/>
       <c r="G23" s="214" t="s">
         <v>64</v>
@@ -8462,11 +8468,11 @@
       <c r="R23" s="131"/>
     </row>
     <row r="24" spans="1:18" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="447" t="s">
+      <c r="A24" s="455" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="448"/>
-      <c r="C24" s="448"/>
+      <c r="B24" s="456"/>
+      <c r="C24" s="456"/>
       <c r="D24" s="218"/>
       <c r="E24" s="218"/>
       <c r="F24" s="218"/>
@@ -8478,19 +8484,19 @@
       <c r="R24" s="131"/>
     </row>
     <row r="25" spans="1:18" ht="16.350000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="438" t="s">
+      <c r="A25" s="446" t="s">
         <v>56</v>
       </c>
-      <c r="B25" s="439"/>
-      <c r="C25" s="439"/>
-      <c r="D25" s="439"/>
-      <c r="E25" s="439"/>
-      <c r="F25" s="439"/>
-      <c r="G25" s="439"/>
-      <c r="H25" s="439"/>
-      <c r="I25" s="439"/>
-      <c r="J25" s="439"/>
-      <c r="K25" s="440"/>
+      <c r="B25" s="447"/>
+      <c r="C25" s="447"/>
+      <c r="D25" s="447"/>
+      <c r="E25" s="447"/>
+      <c r="F25" s="447"/>
+      <c r="G25" s="447"/>
+      <c r="H25" s="447"/>
+      <c r="I25" s="447"/>
+      <c r="J25" s="447"/>
+      <c r="K25" s="448"/>
       <c r="L25" s="9">
         <f>IFERROR(K23-K24,0)</f>
         <v>0</v>
@@ -8608,12 +8614,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A15:F15"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C10:F10"/>
     <mergeCell ref="A25:K25"/>
     <mergeCell ref="A16:F16"/>
     <mergeCell ref="A21:I21"/>
@@ -8621,7 +8621,23 @@
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="D23:E23"/>
     <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A15:F15"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C10:F10"/>
   </mergeCells>
+  <dataValidations count="2">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Du kan endast mata in siffror mellan 0 och 10. Var noga med punkt eller komma beroende på språk" sqref="L15:L19" xr:uid="{A69A740B-83B6-42AF-8E6A-DFC2DE5E21F4}">
+      <formula1>1</formula1>
+      <formula2>10</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Du kan endast mata in siffror. Var noga med punkt eller komma beroende på språk" sqref="C23 F23 K24" xr:uid="{FFAA6551-97BA-4962-93F4-8BCF71A28866}">
+      <formula1>0</formula1>
+      <formula2>100000</formula2>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" scale="99" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
@@ -8640,7 +8656,7 @@
   <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView showZeros="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="L22" activeCellId="3" sqref="B14:H14 K18 K19 L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
@@ -9230,17 +9246,17 @@
   <sheetData>
     <row r="1" spans="1:12" s="111" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="455" t="s">
+      <c r="A2" s="467" t="s">
         <v>165</v>
       </c>
-      <c r="B2" s="455"/>
-      <c r="C2" s="455"/>
-      <c r="D2" s="455"/>
-      <c r="E2" s="455"/>
-      <c r="F2" s="455"/>
-      <c r="G2" s="455"/>
-      <c r="H2" s="455"/>
-      <c r="I2" s="455"/>
+      <c r="B2" s="467"/>
+      <c r="C2" s="467"/>
+      <c r="D2" s="467"/>
+      <c r="E2" s="467"/>
+      <c r="F2" s="467"/>
+      <c r="G2" s="467"/>
+      <c r="H2" s="467"/>
+      <c r="I2" s="467"/>
       <c r="J2" s="141"/>
       <c r="K2" s="141"/>
       <c r="L2" s="141"/>
@@ -9285,10 +9301,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="11"/>
-      <c r="C5" s="394"/>
-      <c r="D5" s="394"/>
-      <c r="E5" s="394"/>
-      <c r="F5" s="394"/>
+      <c r="C5" s="396"/>
+      <c r="D5" s="396"/>
+      <c r="E5" s="396"/>
+      <c r="F5" s="396"/>
       <c r="G5" s="140"/>
       <c r="H5" s="13"/>
       <c r="I5" s="14" t="s">
@@ -9303,10 +9319,10 @@
         <v>8</v>
       </c>
       <c r="B6" s="11"/>
-      <c r="C6" s="394"/>
-      <c r="D6" s="394"/>
-      <c r="E6" s="394"/>
-      <c r="F6" s="394"/>
+      <c r="C6" s="396"/>
+      <c r="D6" s="396"/>
+      <c r="E6" s="396"/>
+      <c r="F6" s="396"/>
       <c r="G6" s="139"/>
       <c r="H6" s="13"/>
       <c r="I6" s="14" t="s">
@@ -9337,10 +9353,10 @@
         <v>0</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="395"/>
-      <c r="D8" s="395"/>
-      <c r="E8" s="395"/>
-      <c r="F8" s="395"/>
+      <c r="C8" s="397"/>
+      <c r="D8" s="397"/>
+      <c r="E8" s="397"/>
+      <c r="F8" s="397"/>
       <c r="G8" s="149"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -9355,10 +9371,10 @@
         <v>6</v>
       </c>
       <c r="B9" s="11"/>
-      <c r="C9" s="394"/>
-      <c r="D9" s="394"/>
-      <c r="E9" s="394"/>
-      <c r="F9" s="394"/>
+      <c r="C9" s="396"/>
+      <c r="D9" s="396"/>
+      <c r="E9" s="396"/>
+      <c r="F9" s="396"/>
       <c r="G9" s="149"/>
       <c r="H9" s="139"/>
       <c r="I9" s="139"/>
@@ -9371,15 +9387,15 @@
         <v>7</v>
       </c>
       <c r="B10" s="11"/>
-      <c r="C10" s="394"/>
-      <c r="D10" s="394"/>
-      <c r="E10" s="394"/>
-      <c r="F10" s="394"/>
+      <c r="C10" s="396"/>
+      <c r="D10" s="396"/>
+      <c r="E10" s="396"/>
+      <c r="F10" s="396"/>
       <c r="G10" s="149"/>
       <c r="H10" s="139"/>
       <c r="I10" s="139"/>
-      <c r="J10" s="451"/>
-      <c r="K10" s="451"/>
+      <c r="J10" s="463"/>
+      <c r="K10" s="463"/>
       <c r="L10" s="150"/>
     </row>
     <row r="11" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -9406,10 +9422,10 @@
       <c r="C13" s="237" t="s">
         <v>115</v>
       </c>
-      <c r="D13" s="456" t="s">
+      <c r="D13" s="468" t="s">
         <v>116</v>
       </c>
-      <c r="E13" s="457"/>
+      <c r="E13" s="469"/>
       <c r="F13" s="237" t="s">
         <v>117</v>
       </c>
@@ -9422,17 +9438,17 @@
       <c r="I13" s="239" t="s">
         <v>90</v>
       </c>
-      <c r="J13" s="460" t="s">
+      <c r="J13" s="472" t="s">
         <v>122</v>
       </c>
-      <c r="K13" s="461"/>
+      <c r="K13" s="473"/>
       <c r="L13" s="148"/>
     </row>
     <row r="14" spans="1:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="256"/>
       <c r="C14" s="257"/>
-      <c r="D14" s="458"/>
-      <c r="E14" s="459"/>
+      <c r="D14" s="470"/>
+      <c r="E14" s="471"/>
       <c r="F14" s="257"/>
       <c r="G14" s="257"/>
       <c r="H14" s="258"/>
@@ -9440,11 +9456,11 @@
         <f>SUM(B14:H14)</f>
         <v>0</v>
       </c>
-      <c r="J14" s="462">
+      <c r="J14" s="474">
         <f>I14/6</f>
         <v>0</v>
       </c>
-      <c r="K14" s="463"/>
+      <c r="K14" s="475"/>
       <c r="L14" s="148"/>
     </row>
     <row r="15" spans="1:12" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -9460,16 +9476,16 @@
       <c r="A17" s="232" t="s">
         <v>121</v>
       </c>
-      <c r="B17" s="452" t="s">
+      <c r="B17" s="464" t="s">
         <v>169</v>
       </c>
-      <c r="C17" s="453"/>
-      <c r="D17" s="453"/>
-      <c r="E17" s="453"/>
-      <c r="F17" s="453"/>
-      <c r="G17" s="453"/>
-      <c r="H17" s="453"/>
-      <c r="I17" s="454"/>
+      <c r="C17" s="465"/>
+      <c r="D17" s="465"/>
+      <c r="E17" s="465"/>
+      <c r="F17" s="465"/>
+      <c r="G17" s="465"/>
+      <c r="H17" s="465"/>
+      <c r="I17" s="466"/>
       <c r="J17" s="146" t="s">
         <v>120</v>
       </c>
@@ -9483,19 +9499,19 @@
       </c>
     </row>
     <row r="18" spans="1:12" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="337" t="s">
+      <c r="A18" s="313" t="s">
         <v>144</v>
       </c>
-      <c r="B18" s="464" t="s">
+      <c r="B18" s="459" t="s">
         <v>170</v>
       </c>
-      <c r="C18" s="465"/>
-      <c r="D18" s="465"/>
-      <c r="E18" s="465"/>
-      <c r="F18" s="465"/>
-      <c r="G18" s="465"/>
-      <c r="H18" s="465"/>
-      <c r="I18" s="465"/>
+      <c r="C18" s="460"/>
+      <c r="D18" s="460"/>
+      <c r="E18" s="460"/>
+      <c r="F18" s="460"/>
+      <c r="G18" s="460"/>
+      <c r="H18" s="460"/>
+      <c r="I18" s="460"/>
       <c r="J18" s="146" t="s">
         <v>124</v>
       </c>
@@ -9506,17 +9522,17 @@
       </c>
     </row>
     <row r="19" spans="1:12" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="338"/>
-      <c r="B19" s="466" t="s">
+      <c r="A19" s="314"/>
+      <c r="B19" s="461" t="s">
         <v>171</v>
       </c>
-      <c r="C19" s="467"/>
-      <c r="D19" s="467"/>
-      <c r="E19" s="467"/>
-      <c r="F19" s="467"/>
-      <c r="G19" s="467"/>
-      <c r="H19" s="467"/>
-      <c r="I19" s="467"/>
+      <c r="C19" s="462"/>
+      <c r="D19" s="462"/>
+      <c r="E19" s="462"/>
+      <c r="F19" s="462"/>
+      <c r="G19" s="462"/>
+      <c r="H19" s="462"/>
+      <c r="I19" s="462"/>
       <c r="J19" s="144" t="s">
         <v>125</v>
       </c>
@@ -9638,12 +9654,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:I18"/>
-    <mergeCell ref="B19:I19"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C10:F10"/>
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="B17:I17"/>
     <mergeCell ref="A2:I2"/>
@@ -9653,7 +9663,19 @@
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="J13:K13"/>
     <mergeCell ref="J14:K14"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:I18"/>
+    <mergeCell ref="B19:I19"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C10:F10"/>
   </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Du kan endast mata in siffror mellan 0 och 10. Var noga med punkt eller komma beroende på språk" sqref="B14:H14 K18 K19 L22" xr:uid="{5C12642A-ECB8-442A-97E3-CEC6FE13045F}">
+      <formula1>0</formula1>
+      <formula2>10</formula2>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" scale="99" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
@@ -10262,17 +10284,17 @@
   <sheetData>
     <row r="1" spans="1:12" s="111" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="455" t="s">
+      <c r="A2" s="467" t="s">
         <v>167</v>
       </c>
-      <c r="B2" s="455"/>
-      <c r="C2" s="455"/>
-      <c r="D2" s="455"/>
-      <c r="E2" s="455"/>
-      <c r="F2" s="455"/>
-      <c r="G2" s="455"/>
-      <c r="H2" s="455"/>
-      <c r="I2" s="455"/>
+      <c r="B2" s="467"/>
+      <c r="C2" s="467"/>
+      <c r="D2" s="467"/>
+      <c r="E2" s="467"/>
+      <c r="F2" s="467"/>
+      <c r="G2" s="467"/>
+      <c r="H2" s="467"/>
+      <c r="I2" s="467"/>
       <c r="J2" s="141"/>
       <c r="K2" s="141"/>
       <c r="L2" s="141"/>
@@ -10317,10 +10339,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="11"/>
-      <c r="C5" s="394"/>
-      <c r="D5" s="394"/>
-      <c r="E5" s="394"/>
-      <c r="F5" s="394"/>
+      <c r="C5" s="396"/>
+      <c r="D5" s="396"/>
+      <c r="E5" s="396"/>
+      <c r="F5" s="396"/>
       <c r="G5" s="140"/>
       <c r="H5" s="13"/>
       <c r="I5" s="14" t="s">
@@ -10335,10 +10357,10 @@
         <v>8</v>
       </c>
       <c r="B6" s="11"/>
-      <c r="C6" s="394"/>
-      <c r="D6" s="394"/>
-      <c r="E6" s="394"/>
-      <c r="F6" s="394"/>
+      <c r="C6" s="396"/>
+      <c r="D6" s="396"/>
+      <c r="E6" s="396"/>
+      <c r="F6" s="396"/>
       <c r="G6" s="139"/>
       <c r="H6" s="13"/>
       <c r="I6" s="14" t="s">
@@ -10369,10 +10391,10 @@
         <v>0</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="395"/>
-      <c r="D8" s="395"/>
-      <c r="E8" s="395"/>
-      <c r="F8" s="395"/>
+      <c r="C8" s="397"/>
+      <c r="D8" s="397"/>
+      <c r="E8" s="397"/>
+      <c r="F8" s="397"/>
       <c r="G8" s="149"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -10387,10 +10409,10 @@
         <v>6</v>
       </c>
       <c r="B9" s="11"/>
-      <c r="C9" s="394"/>
-      <c r="D9" s="394"/>
-      <c r="E9" s="394"/>
-      <c r="F9" s="394"/>
+      <c r="C9" s="396"/>
+      <c r="D9" s="396"/>
+      <c r="E9" s="396"/>
+      <c r="F9" s="396"/>
       <c r="G9" s="149"/>
       <c r="H9" s="139"/>
       <c r="I9" s="139"/>
@@ -10403,15 +10425,15 @@
         <v>7</v>
       </c>
       <c r="B10" s="11"/>
-      <c r="C10" s="394"/>
-      <c r="D10" s="394"/>
-      <c r="E10" s="394"/>
-      <c r="F10" s="394"/>
+      <c r="C10" s="396"/>
+      <c r="D10" s="396"/>
+      <c r="E10" s="396"/>
+      <c r="F10" s="396"/>
       <c r="G10" s="149"/>
       <c r="H10" s="139"/>
       <c r="I10" s="139"/>
-      <c r="J10" s="451"/>
-      <c r="K10" s="451"/>
+      <c r="J10" s="463"/>
+      <c r="K10" s="463"/>
       <c r="L10" s="150"/>
     </row>
     <row r="11" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -10438,10 +10460,10 @@
       <c r="C13" s="237" t="s">
         <v>115</v>
       </c>
-      <c r="D13" s="456" t="s">
+      <c r="D13" s="468" t="s">
         <v>116</v>
       </c>
-      <c r="E13" s="457"/>
+      <c r="E13" s="469"/>
       <c r="F13" s="237" t="s">
         <v>117</v>
       </c>
@@ -10450,17 +10472,17 @@
       <c r="I13" s="239" t="s">
         <v>90</v>
       </c>
-      <c r="J13" s="460" t="s">
+      <c r="J13" s="472" t="s">
         <v>122</v>
       </c>
-      <c r="K13" s="461"/>
+      <c r="K13" s="473"/>
       <c r="L13" s="148"/>
     </row>
     <row r="14" spans="1:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="256"/>
       <c r="C14" s="257"/>
-      <c r="D14" s="458"/>
-      <c r="E14" s="459"/>
+      <c r="D14" s="470"/>
+      <c r="E14" s="471"/>
       <c r="F14" s="257"/>
       <c r="G14" s="280"/>
       <c r="H14" s="281"/>
@@ -10468,11 +10490,11 @@
         <f>SUM(B14:F14)</f>
         <v>0</v>
       </c>
-      <c r="J14" s="462">
+      <c r="J14" s="474">
         <f>I14/4</f>
         <v>0</v>
       </c>
-      <c r="K14" s="463"/>
+      <c r="K14" s="475"/>
       <c r="L14" s="148"/>
     </row>
     <row r="15" spans="1:12" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -10488,16 +10510,16 @@
       <c r="A17" s="232" t="s">
         <v>121</v>
       </c>
-      <c r="B17" s="468" t="s">
+      <c r="B17" s="476" t="s">
         <v>172</v>
       </c>
-      <c r="C17" s="469"/>
-      <c r="D17" s="469"/>
-      <c r="E17" s="469"/>
-      <c r="F17" s="469"/>
-      <c r="G17" s="469"/>
-      <c r="H17" s="469"/>
-      <c r="I17" s="470"/>
+      <c r="C17" s="477"/>
+      <c r="D17" s="477"/>
+      <c r="E17" s="477"/>
+      <c r="F17" s="477"/>
+      <c r="G17" s="477"/>
+      <c r="H17" s="477"/>
+      <c r="I17" s="478"/>
       <c r="J17" s="146" t="s">
         <v>120</v>
       </c>
@@ -10511,19 +10533,19 @@
       </c>
     </row>
     <row r="18" spans="1:12" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="337" t="s">
+      <c r="A18" s="313" t="s">
         <v>144</v>
       </c>
-      <c r="B18" s="464" t="s">
+      <c r="B18" s="459" t="s">
         <v>170</v>
       </c>
-      <c r="C18" s="465"/>
-      <c r="D18" s="465"/>
-      <c r="E18" s="465"/>
-      <c r="F18" s="465"/>
-      <c r="G18" s="465"/>
-      <c r="H18" s="465"/>
-      <c r="I18" s="465"/>
+      <c r="C18" s="460"/>
+      <c r="D18" s="460"/>
+      <c r="E18" s="460"/>
+      <c r="F18" s="460"/>
+      <c r="G18" s="460"/>
+      <c r="H18" s="460"/>
+      <c r="I18" s="460"/>
       <c r="J18" s="146" t="s">
         <v>124</v>
       </c>
@@ -10534,17 +10556,17 @@
       </c>
     </row>
     <row r="19" spans="1:12" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="338"/>
-      <c r="B19" s="466" t="s">
+      <c r="A19" s="314"/>
+      <c r="B19" s="461" t="s">
         <v>171</v>
       </c>
-      <c r="C19" s="467"/>
-      <c r="D19" s="467"/>
-      <c r="E19" s="467"/>
-      <c r="F19" s="467"/>
-      <c r="G19" s="467"/>
-      <c r="H19" s="467"/>
-      <c r="I19" s="467"/>
+      <c r="C19" s="462"/>
+      <c r="D19" s="462"/>
+      <c r="E19" s="462"/>
+      <c r="F19" s="462"/>
+      <c r="G19" s="462"/>
+      <c r="H19" s="462"/>
+      <c r="I19" s="462"/>
       <c r="J19" s="144" t="s">
         <v>125</v>
       </c>
@@ -10666,11 +10688,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C9:F9"/>
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="B18:I18"/>
     <mergeCell ref="B19:I19"/>
@@ -10681,7 +10698,18 @@
     <mergeCell ref="J14:K14"/>
     <mergeCell ref="B17:I17"/>
     <mergeCell ref="C10:F10"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C9:F9"/>
   </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Du kan endast mata in siffror mellan 0 och 10. Var noga med punkt eller komma beroende på språk" sqref="B14:F14 K18 K19 L22" xr:uid="{F4EB1C43-753F-4EC3-B376-2665BC2F486C}">
+      <formula1>0</formula1>
+      <formula2>10</formula2>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" scale="99" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
@@ -10700,7 +10728,7 @@
   <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView showZeros="0" showRuler="0" topLeftCell="A8" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B23" sqref="B23:C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
@@ -10751,8 +10779,8 @@
         <v>4</v>
       </c>
       <c r="B3" s="158"/>
-      <c r="C3" s="363"/>
-      <c r="D3" s="363"/>
+      <c r="C3" s="307"/>
+      <c r="D3" s="307"/>
       <c r="E3" s="265"/>
       <c r="F3" s="265"/>
       <c r="H3" s="153"/>
@@ -10768,10 +10796,10 @@
         <v>5</v>
       </c>
       <c r="B4" s="134"/>
-      <c r="C4" s="362"/>
-      <c r="D4" s="362"/>
-      <c r="E4" s="362"/>
-      <c r="F4" s="362"/>
+      <c r="C4" s="306"/>
+      <c r="D4" s="306"/>
+      <c r="E4" s="306"/>
+      <c r="F4" s="306"/>
       <c r="H4" s="153"/>
       <c r="I4" s="154" t="s">
         <v>11</v>
@@ -10785,10 +10813,10 @@
         <v>8</v>
       </c>
       <c r="B5" s="134"/>
-      <c r="C5" s="362"/>
-      <c r="D5" s="362"/>
-      <c r="E5" s="362"/>
-      <c r="F5" s="362"/>
+      <c r="C5" s="306"/>
+      <c r="D5" s="306"/>
+      <c r="E5" s="306"/>
+      <c r="F5" s="306"/>
       <c r="K5" s="30"/>
     </row>
     <row r="6" spans="1:12" s="111" customFormat="1" ht="17.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -10811,10 +10839,10 @@
         <v>0</v>
       </c>
       <c r="B7" s="158"/>
-      <c r="C7" s="362"/>
-      <c r="D7" s="362"/>
-      <c r="E7" s="362"/>
-      <c r="F7" s="362"/>
+      <c r="C7" s="306"/>
+      <c r="D7" s="306"/>
+      <c r="E7" s="306"/>
+      <c r="F7" s="306"/>
       <c r="K7" s="30"/>
     </row>
     <row r="8" spans="1:12" s="111" customFormat="1" ht="17.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -10822,10 +10850,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="134"/>
-      <c r="C8" s="362"/>
-      <c r="D8" s="362"/>
-      <c r="E8" s="362"/>
-      <c r="F8" s="362"/>
+      <c r="C8" s="306"/>
+      <c r="D8" s="306"/>
+      <c r="E8" s="306"/>
+      <c r="F8" s="306"/>
       <c r="K8" s="30"/>
     </row>
     <row r="9" spans="1:12" s="111" customFormat="1" ht="17.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -10833,10 +10861,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="134"/>
-      <c r="C9" s="362"/>
-      <c r="D9" s="362"/>
-      <c r="E9" s="362"/>
-      <c r="F9" s="362"/>
+      <c r="C9" s="306"/>
+      <c r="D9" s="306"/>
+      <c r="E9" s="306"/>
+      <c r="F9" s="306"/>
       <c r="K9" s="30"/>
     </row>
     <row r="10" spans="1:12" s="111" customFormat="1" ht="17.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -10851,86 +10879,86 @@
       <c r="D11" s="268"/>
       <c r="E11" s="268"/>
       <c r="F11" s="268"/>
-      <c r="H11" s="332" t="s">
+      <c r="H11" s="308" t="s">
         <v>15</v>
       </c>
-      <c r="I11" s="333"/>
-      <c r="J11" s="334" t="s">
+      <c r="I11" s="309"/>
+      <c r="J11" s="310" t="s">
         <v>16</v>
       </c>
-      <c r="K11" s="335"/>
-      <c r="L11" s="336"/>
+      <c r="K11" s="311"/>
+      <c r="L11" s="312"/>
     </row>
     <row r="12" spans="1:12" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="337" t="s">
+      <c r="A12" s="313" t="s">
         <v>145</v>
       </c>
-      <c r="B12" s="341" t="s">
+      <c r="B12" s="317" t="s">
         <v>146</v>
       </c>
-      <c r="C12" s="342"/>
-      <c r="D12" s="342"/>
-      <c r="E12" s="342"/>
-      <c r="F12" s="342"/>
-      <c r="G12" s="343"/>
-      <c r="H12" s="350"/>
-      <c r="I12" s="351"/>
-      <c r="J12" s="356" t="s">
+      <c r="C12" s="318"/>
+      <c r="D12" s="318"/>
+      <c r="E12" s="318"/>
+      <c r="F12" s="318"/>
+      <c r="G12" s="319"/>
+      <c r="H12" s="326"/>
+      <c r="I12" s="327"/>
+      <c r="J12" s="332" t="s">
         <v>147</v>
       </c>
-      <c r="K12" s="358">
+      <c r="K12" s="335">
         <f>SUM(B17:G17)/6</f>
         <v>0</v>
       </c>
-      <c r="L12" s="360">
+      <c r="L12" s="337">
         <f>ROUND(K12*0.6,3)</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="338"/>
-      <c r="B13" s="344"/>
-      <c r="C13" s="345"/>
-      <c r="D13" s="345"/>
-      <c r="E13" s="345"/>
-      <c r="F13" s="345"/>
-      <c r="G13" s="346"/>
-      <c r="H13" s="352"/>
-      <c r="I13" s="353"/>
-      <c r="J13" s="321"/>
-      <c r="K13" s="359"/>
-      <c r="L13" s="323"/>
+      <c r="A13" s="314"/>
+      <c r="B13" s="320"/>
+      <c r="C13" s="321"/>
+      <c r="D13" s="321"/>
+      <c r="E13" s="321"/>
+      <c r="F13" s="321"/>
+      <c r="G13" s="322"/>
+      <c r="H13" s="328"/>
+      <c r="I13" s="329"/>
+      <c r="J13" s="333"/>
+      <c r="K13" s="336"/>
+      <c r="L13" s="338"/>
     </row>
     <row r="14" spans="1:12" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="338"/>
-      <c r="B14" s="344"/>
-      <c r="C14" s="345"/>
-      <c r="D14" s="345"/>
-      <c r="E14" s="345"/>
-      <c r="F14" s="345"/>
-      <c r="G14" s="346"/>
-      <c r="H14" s="352"/>
-      <c r="I14" s="353"/>
-      <c r="J14" s="321"/>
-      <c r="K14" s="359"/>
-      <c r="L14" s="323"/>
+      <c r="A14" s="314"/>
+      <c r="B14" s="320"/>
+      <c r="C14" s="321"/>
+      <c r="D14" s="321"/>
+      <c r="E14" s="321"/>
+      <c r="F14" s="321"/>
+      <c r="G14" s="322"/>
+      <c r="H14" s="328"/>
+      <c r="I14" s="329"/>
+      <c r="J14" s="333"/>
+      <c r="K14" s="336"/>
+      <c r="L14" s="338"/>
     </row>
     <row r="15" spans="1:12" ht="70.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="338"/>
-      <c r="B15" s="347"/>
-      <c r="C15" s="348"/>
-      <c r="D15" s="348"/>
-      <c r="E15" s="348"/>
-      <c r="F15" s="348"/>
-      <c r="G15" s="349"/>
-      <c r="H15" s="352"/>
-      <c r="I15" s="353"/>
-      <c r="J15" s="321"/>
-      <c r="K15" s="359"/>
-      <c r="L15" s="323"/>
+      <c r="A15" s="314"/>
+      <c r="B15" s="323"/>
+      <c r="C15" s="324"/>
+      <c r="D15" s="324"/>
+      <c r="E15" s="324"/>
+      <c r="F15" s="324"/>
+      <c r="G15" s="325"/>
+      <c r="H15" s="328"/>
+      <c r="I15" s="329"/>
+      <c r="J15" s="333"/>
+      <c r="K15" s="336"/>
+      <c r="L15" s="338"/>
     </row>
     <row r="16" spans="1:12" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="339"/>
+      <c r="A16" s="315"/>
       <c r="B16" s="269" t="s">
         <v>148</v>
       </c>
@@ -10949,154 +10977,154 @@
       <c r="G16" s="272" t="s">
         <v>153</v>
       </c>
-      <c r="H16" s="352"/>
-      <c r="I16" s="353"/>
-      <c r="J16" s="321"/>
-      <c r="K16" s="359"/>
-      <c r="L16" s="323"/>
+      <c r="H16" s="328"/>
+      <c r="I16" s="329"/>
+      <c r="J16" s="333"/>
+      <c r="K16" s="336"/>
+      <c r="L16" s="338"/>
     </row>
     <row r="17" spans="1:12" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="340"/>
+      <c r="A17" s="316"/>
       <c r="B17" s="273"/>
       <c r="C17" s="274"/>
       <c r="D17" s="274"/>
       <c r="E17" s="274"/>
       <c r="F17" s="274"/>
       <c r="G17" s="275"/>
-      <c r="H17" s="354"/>
-      <c r="I17" s="355"/>
-      <c r="J17" s="357"/>
-      <c r="K17" s="359"/>
-      <c r="L17" s="361"/>
+      <c r="H17" s="330"/>
+      <c r="I17" s="331"/>
+      <c r="J17" s="334"/>
+      <c r="K17" s="336"/>
+      <c r="L17" s="339"/>
     </row>
     <row r="18" spans="1:12" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="297"/>
-      <c r="B18" s="300" t="s">
+      <c r="A18" s="342"/>
+      <c r="B18" s="345" t="s">
         <v>154</v>
       </c>
-      <c r="C18" s="300"/>
-      <c r="D18" s="300"/>
-      <c r="E18" s="300"/>
-      <c r="F18" s="300"/>
-      <c r="G18" s="300"/>
-      <c r="H18" s="303"/>
-      <c r="I18" s="304"/>
-      <c r="J18" s="309" t="s">
+      <c r="C18" s="345"/>
+      <c r="D18" s="345"/>
+      <c r="E18" s="345"/>
+      <c r="F18" s="345"/>
+      <c r="G18" s="345"/>
+      <c r="H18" s="348"/>
+      <c r="I18" s="349"/>
+      <c r="J18" s="354" t="s">
         <v>1</v>
       </c>
-      <c r="K18" s="364">
+      <c r="K18" s="375">
         <f>SUMPRODUCT(B23:G23,B22:G22)</f>
         <v>0</v>
       </c>
-      <c r="L18" s="312" t="str">
+      <c r="L18" s="357" t="str">
         <f>IF(K18=0,"",MAX(0.0000000001,IF(K25="",ROUND(K18*0.25,3),ROUND((K18-K25)*0.25,3))))</f>
         <v/>
       </c>
     </row>
     <row r="19" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="298"/>
-      <c r="B19" s="301"/>
-      <c r="C19" s="301"/>
-      <c r="D19" s="301"/>
-      <c r="E19" s="301"/>
-      <c r="F19" s="301"/>
-      <c r="G19" s="301"/>
-      <c r="H19" s="305"/>
-      <c r="I19" s="306"/>
-      <c r="J19" s="310"/>
-      <c r="K19" s="365"/>
-      <c r="L19" s="313"/>
+      <c r="A19" s="343"/>
+      <c r="B19" s="346"/>
+      <c r="C19" s="346"/>
+      <c r="D19" s="346"/>
+      <c r="E19" s="346"/>
+      <c r="F19" s="346"/>
+      <c r="G19" s="346"/>
+      <c r="H19" s="350"/>
+      <c r="I19" s="351"/>
+      <c r="J19" s="355"/>
+      <c r="K19" s="376"/>
+      <c r="L19" s="358"/>
     </row>
     <row r="20" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="298"/>
-      <c r="B20" s="302"/>
-      <c r="C20" s="302"/>
-      <c r="D20" s="302"/>
-      <c r="E20" s="302"/>
-      <c r="F20" s="302"/>
-      <c r="G20" s="301"/>
-      <c r="H20" s="305"/>
-      <c r="I20" s="306"/>
-      <c r="J20" s="310"/>
-      <c r="K20" s="365"/>
-      <c r="L20" s="313"/>
+      <c r="A20" s="343"/>
+      <c r="B20" s="347"/>
+      <c r="C20" s="347"/>
+      <c r="D20" s="347"/>
+      <c r="E20" s="347"/>
+      <c r="F20" s="347"/>
+      <c r="G20" s="346"/>
+      <c r="H20" s="350"/>
+      <c r="I20" s="351"/>
+      <c r="J20" s="355"/>
+      <c r="K20" s="376"/>
+      <c r="L20" s="358"/>
     </row>
     <row r="21" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="298"/>
-      <c r="B21" s="324" t="s">
+      <c r="A21" s="343"/>
+      <c r="B21" s="367" t="s">
         <v>202</v>
       </c>
-      <c r="C21" s="325"/>
-      <c r="D21" s="326" t="s">
+      <c r="C21" s="368"/>
+      <c r="D21" s="369" t="s">
         <v>203</v>
       </c>
-      <c r="E21" s="327"/>
-      <c r="F21" s="328" t="s">
+      <c r="E21" s="370"/>
+      <c r="F21" s="371" t="s">
         <v>204</v>
       </c>
-      <c r="G21" s="329"/>
-      <c r="H21" s="305"/>
-      <c r="I21" s="306"/>
-      <c r="J21" s="310"/>
-      <c r="K21" s="365"/>
-      <c r="L21" s="313"/>
+      <c r="G21" s="372"/>
+      <c r="H21" s="350"/>
+      <c r="I21" s="351"/>
+      <c r="J21" s="355"/>
+      <c r="K21" s="376"/>
+      <c r="L21" s="358"/>
     </row>
     <row r="22" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="298"/>
-      <c r="B22" s="330">
+      <c r="A22" s="343"/>
+      <c r="B22" s="373">
         <v>0.5</v>
       </c>
-      <c r="C22" s="331"/>
-      <c r="D22" s="367">
+      <c r="C22" s="374"/>
+      <c r="D22" s="297">
         <v>0.25</v>
       </c>
-      <c r="E22" s="368"/>
-      <c r="F22" s="369">
+      <c r="E22" s="298"/>
+      <c r="F22" s="299">
         <v>0.25</v>
       </c>
-      <c r="G22" s="370"/>
-      <c r="H22" s="305"/>
-      <c r="I22" s="306"/>
-      <c r="J22" s="310"/>
-      <c r="K22" s="365"/>
-      <c r="L22" s="313"/>
+      <c r="G22" s="300"/>
+      <c r="H22" s="350"/>
+      <c r="I22" s="351"/>
+      <c r="J22" s="355"/>
+      <c r="K22" s="376"/>
+      <c r="L22" s="358"/>
     </row>
     <row r="23" spans="1:12" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="298"/>
-      <c r="B23" s="371">
+      <c r="A23" s="343"/>
+      <c r="B23" s="301">
         <v>0</v>
       </c>
-      <c r="C23" s="372"/>
-      <c r="D23" s="373">
+      <c r="C23" s="302"/>
+      <c r="D23" s="303">
         <v>0</v>
       </c>
-      <c r="E23" s="374"/>
-      <c r="F23" s="372">
+      <c r="E23" s="304"/>
+      <c r="F23" s="302">
         <v>0</v>
       </c>
-      <c r="G23" s="375"/>
-      <c r="H23" s="305"/>
-      <c r="I23" s="306"/>
-      <c r="J23" s="310"/>
-      <c r="K23" s="365"/>
-      <c r="L23" s="313"/>
+      <c r="G23" s="305"/>
+      <c r="H23" s="350"/>
+      <c r="I23" s="351"/>
+      <c r="J23" s="355"/>
+      <c r="K23" s="376"/>
+      <c r="L23" s="358"/>
     </row>
     <row r="24" spans="1:12" s="148" customFormat="1" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="298"/>
+      <c r="A24" s="343"/>
       <c r="B24" s="288"/>
       <c r="C24" s="289"/>
       <c r="D24" s="290"/>
       <c r="E24" s="290"/>
       <c r="F24" s="289"/>
       <c r="G24" s="291"/>
-      <c r="H24" s="305"/>
-      <c r="I24" s="306"/>
-      <c r="J24" s="310"/>
-      <c r="K24" s="366"/>
-      <c r="L24" s="313"/>
+      <c r="H24" s="350"/>
+      <c r="I24" s="351"/>
+      <c r="J24" s="355"/>
+      <c r="K24" s="377"/>
+      <c r="L24" s="358"/>
     </row>
     <row r="25" spans="1:12" ht="28.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="299"/>
+      <c r="A25" s="344"/>
       <c r="B25" s="276" t="s">
         <v>155</v>
       </c>
@@ -11107,42 +11135,42 @@
       <c r="E25" s="277"/>
       <c r="F25" s="277"/>
       <c r="G25" s="277"/>
-      <c r="H25" s="307"/>
-      <c r="I25" s="308"/>
-      <c r="J25" s="311"/>
+      <c r="H25" s="352"/>
+      <c r="I25" s="353"/>
+      <c r="J25" s="356"/>
       <c r="K25" s="292" t="str">
         <f>IF(SUM(C25:G25)=0,"",MAX(0.0000000001,SUM(C25:G25)))</f>
         <v/>
       </c>
-      <c r="L25" s="314"/>
+      <c r="L25" s="359"/>
     </row>
     <row r="26" spans="1:12" ht="87.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="297" t="s">
+      <c r="A26" s="342" t="s">
         <v>12</v>
       </c>
-      <c r="B26" s="300" t="s">
+      <c r="B26" s="345" t="s">
         <v>156</v>
       </c>
-      <c r="C26" s="315"/>
-      <c r="D26" s="315"/>
-      <c r="E26" s="315"/>
-      <c r="F26" s="315"/>
-      <c r="G26" s="316"/>
-      <c r="H26" s="317"/>
-      <c r="I26" s="318"/>
-      <c r="J26" s="321" t="s">
+      <c r="C26" s="360"/>
+      <c r="D26" s="360"/>
+      <c r="E26" s="360"/>
+      <c r="F26" s="360"/>
+      <c r="G26" s="361"/>
+      <c r="H26" s="362"/>
+      <c r="I26" s="363"/>
+      <c r="J26" s="333" t="s">
         <v>157</v>
       </c>
       <c r="K26" s="293">
         <v>0</v>
       </c>
-      <c r="L26" s="323">
+      <c r="L26" s="338">
         <f>IF((K26-K27)&gt;=0,(ROUND((K26-K27)*0.15,3)),0.000000001)</f>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="28.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="299"/>
+      <c r="A27" s="344"/>
       <c r="B27" s="278" t="s">
         <v>155</v>
       </c>
@@ -11161,14 +11189,14 @@
       <c r="G27" s="277">
         <v>0</v>
       </c>
-      <c r="H27" s="319"/>
-      <c r="I27" s="320"/>
-      <c r="J27" s="322"/>
+      <c r="H27" s="364"/>
+      <c r="I27" s="365"/>
+      <c r="J27" s="366"/>
       <c r="K27" s="294">
         <f>SUM(C27:G27)</f>
         <v>0</v>
       </c>
-      <c r="L27" s="314"/>
+      <c r="L27" s="359"/>
     </row>
     <row r="28" spans="1:12" ht="13.15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="21"/>
@@ -11185,11 +11213,11 @@
         <v>3</v>
       </c>
       <c r="J29" s="23"/>
-      <c r="K29" s="295">
+      <c r="K29" s="340">
         <f>SUM(L12:L26)</f>
         <v>0</v>
       </c>
-      <c r="L29" s="296"/>
+      <c r="L29" s="341"/>
     </row>
     <row r="30" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="31" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -11212,25 +11240,6 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="A12:A17"/>
-    <mergeCell ref="B12:G15"/>
-    <mergeCell ref="H12:I17"/>
-    <mergeCell ref="J12:J17"/>
-    <mergeCell ref="K12:K17"/>
-    <mergeCell ref="L12:L17"/>
     <mergeCell ref="K29:L29"/>
     <mergeCell ref="A18:A25"/>
     <mergeCell ref="B18:G20"/>
@@ -11247,6 +11256,25 @@
     <mergeCell ref="F21:G21"/>
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="K18:K24"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="A12:A17"/>
+    <mergeCell ref="B12:G15"/>
+    <mergeCell ref="H12:I17"/>
+    <mergeCell ref="J12:J17"/>
+    <mergeCell ref="K12:K17"/>
+    <mergeCell ref="L12:L17"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:G23"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="decimal" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Enbart siffror" error="Ej giltig siffra_x000a_Kan du ha skirvit komma istället för punkt eller tvärt om" sqref="B17:G17 B23:C23 D23:E23 F23:G23 C25 D25 E25 F25 G25 C27 D27 E27 F27 G27 K26" xr:uid="{2F8E46EA-E6B1-42D6-9781-DACEBCFB30BC}">
@@ -11271,7 +11299,7 @@
   <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView showZeros="0" view="pageLayout" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
@@ -11338,10 +11366,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="134"/>
-      <c r="C5" s="376"/>
-      <c r="D5" s="376"/>
-      <c r="E5" s="376"/>
-      <c r="F5" s="376"/>
+      <c r="C5" s="392"/>
+      <c r="D5" s="392"/>
+      <c r="E5" s="392"/>
+      <c r="F5" s="392"/>
       <c r="H5" s="153"/>
       <c r="I5" s="154" t="s">
         <v>11</v>
@@ -11355,10 +11383,10 @@
         <v>8</v>
       </c>
       <c r="B6" s="134"/>
-      <c r="C6" s="376"/>
-      <c r="D6" s="376"/>
-      <c r="E6" s="376"/>
-      <c r="F6" s="376"/>
+      <c r="C6" s="392"/>
+      <c r="D6" s="392"/>
+      <c r="E6" s="392"/>
+      <c r="F6" s="392"/>
       <c r="K6" s="30"/>
     </row>
     <row r="7" spans="1:12" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -11381,30 +11409,30 @@
         <v>0</v>
       </c>
       <c r="B8" s="158"/>
-      <c r="C8" s="376"/>
-      <c r="D8" s="376"/>
-      <c r="E8" s="376"/>
-      <c r="F8" s="376"/>
+      <c r="C8" s="392"/>
+      <c r="D8" s="392"/>
+      <c r="E8" s="392"/>
+      <c r="F8" s="392"/>
     </row>
     <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="134" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="134"/>
-      <c r="C9" s="376"/>
-      <c r="D9" s="376"/>
-      <c r="E9" s="376"/>
-      <c r="F9" s="376"/>
+      <c r="C9" s="392"/>
+      <c r="D9" s="392"/>
+      <c r="E9" s="392"/>
+      <c r="F9" s="392"/>
     </row>
     <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="134" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="134"/>
-      <c r="C10" s="376"/>
-      <c r="D10" s="376"/>
-      <c r="E10" s="376"/>
-      <c r="F10" s="376"/>
+      <c r="C10" s="392"/>
+      <c r="D10" s="392"/>
+      <c r="E10" s="392"/>
+      <c r="F10" s="392"/>
     </row>
     <row r="11" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:12" ht="57.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -11428,115 +11456,115 @@
       </c>
     </row>
     <row r="15" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="377" t="s">
+      <c r="A15" s="378" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="378"/>
-      <c r="C15" s="378"/>
-      <c r="D15" s="379"/>
-      <c r="E15" s="383"/>
-      <c r="F15" s="384"/>
-      <c r="G15" s="384"/>
-      <c r="H15" s="384"/>
-      <c r="I15" s="384"/>
-      <c r="J15" s="384"/>
-      <c r="K15" s="385"/>
+      <c r="B15" s="379"/>
+      <c r="C15" s="379"/>
+      <c r="D15" s="380"/>
+      <c r="E15" s="384"/>
+      <c r="F15" s="385"/>
+      <c r="G15" s="385"/>
+      <c r="H15" s="385"/>
+      <c r="I15" s="385"/>
+      <c r="J15" s="385"/>
+      <c r="K15" s="386"/>
       <c r="L15" s="244"/>
     </row>
     <row r="16" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="377" t="s">
+      <c r="A16" s="378" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="378"/>
-      <c r="C16" s="378"/>
-      <c r="D16" s="379"/>
-      <c r="E16" s="383"/>
-      <c r="F16" s="384"/>
-      <c r="G16" s="384"/>
-      <c r="H16" s="384"/>
-      <c r="I16" s="384"/>
-      <c r="J16" s="384"/>
-      <c r="K16" s="385"/>
+      <c r="B16" s="379"/>
+      <c r="C16" s="379"/>
+      <c r="D16" s="380"/>
+      <c r="E16" s="384"/>
+      <c r="F16" s="385"/>
+      <c r="G16" s="385"/>
+      <c r="H16" s="385"/>
+      <c r="I16" s="385"/>
+      <c r="J16" s="385"/>
+      <c r="K16" s="386"/>
       <c r="L16" s="244"/>
     </row>
     <row r="17" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="380" t="s">
+      <c r="A17" s="381" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="381"/>
-      <c r="C17" s="381"/>
-      <c r="D17" s="382"/>
-      <c r="E17" s="383"/>
-      <c r="F17" s="384"/>
-      <c r="G17" s="384"/>
-      <c r="H17" s="384"/>
-      <c r="I17" s="384"/>
-      <c r="J17" s="384"/>
-      <c r="K17" s="385"/>
+      <c r="B17" s="382"/>
+      <c r="C17" s="382"/>
+      <c r="D17" s="383"/>
+      <c r="E17" s="384"/>
+      <c r="F17" s="385"/>
+      <c r="G17" s="385"/>
+      <c r="H17" s="385"/>
+      <c r="I17" s="385"/>
+      <c r="J17" s="385"/>
+      <c r="K17" s="386"/>
       <c r="L17" s="244"/>
     </row>
     <row r="18" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="377" t="s">
+      <c r="A18" s="378" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="378"/>
-      <c r="C18" s="378"/>
-      <c r="D18" s="379"/>
-      <c r="E18" s="383"/>
-      <c r="F18" s="384"/>
-      <c r="G18" s="384"/>
-      <c r="H18" s="384"/>
-      <c r="I18" s="384"/>
-      <c r="J18" s="384"/>
-      <c r="K18" s="385"/>
+      <c r="B18" s="379"/>
+      <c r="C18" s="379"/>
+      <c r="D18" s="380"/>
+      <c r="E18" s="384"/>
+      <c r="F18" s="385"/>
+      <c r="G18" s="385"/>
+      <c r="H18" s="385"/>
+      <c r="I18" s="385"/>
+      <c r="J18" s="385"/>
+      <c r="K18" s="386"/>
       <c r="L18" s="244"/>
     </row>
     <row r="19" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="377" t="s">
+      <c r="A19" s="378" t="s">
         <v>168</v>
       </c>
-      <c r="B19" s="378"/>
-      <c r="C19" s="378"/>
-      <c r="D19" s="379"/>
-      <c r="E19" s="386"/>
-      <c r="F19" s="386"/>
-      <c r="G19" s="386"/>
-      <c r="H19" s="386"/>
-      <c r="I19" s="386"/>
-      <c r="J19" s="386"/>
-      <c r="K19" s="387"/>
+      <c r="B19" s="379"/>
+      <c r="C19" s="379"/>
+      <c r="D19" s="380"/>
+      <c r="E19" s="387"/>
+      <c r="F19" s="387"/>
+      <c r="G19" s="387"/>
+      <c r="H19" s="387"/>
+      <c r="I19" s="387"/>
+      <c r="J19" s="387"/>
+      <c r="K19" s="388"/>
       <c r="L19" s="244"/>
     </row>
     <row r="20" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="388" t="s">
+      <c r="A20" s="389" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="389"/>
-      <c r="C20" s="389"/>
-      <c r="D20" s="390"/>
-      <c r="E20" s="383"/>
-      <c r="F20" s="384"/>
-      <c r="G20" s="384"/>
-      <c r="H20" s="384"/>
-      <c r="I20" s="384"/>
-      <c r="J20" s="384"/>
-      <c r="K20" s="385"/>
+      <c r="B20" s="390"/>
+      <c r="C20" s="390"/>
+      <c r="D20" s="391"/>
+      <c r="E20" s="384"/>
+      <c r="F20" s="385"/>
+      <c r="G20" s="385"/>
+      <c r="H20" s="385"/>
+      <c r="I20" s="385"/>
+      <c r="J20" s="385"/>
+      <c r="K20" s="386"/>
       <c r="L20" s="244"/>
     </row>
     <row r="21" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="377" t="s">
+      <c r="A21" s="378" t="s">
         <v>188</v>
       </c>
-      <c r="B21" s="378"/>
-      <c r="C21" s="378"/>
-      <c r="D21" s="379"/>
-      <c r="E21" s="377"/>
-      <c r="F21" s="378"/>
-      <c r="G21" s="378"/>
-      <c r="H21" s="378"/>
-      <c r="I21" s="378"/>
-      <c r="J21" s="378"/>
-      <c r="K21" s="379"/>
+      <c r="B21" s="379"/>
+      <c r="C21" s="379"/>
+      <c r="D21" s="380"/>
+      <c r="E21" s="378"/>
+      <c r="F21" s="379"/>
+      <c r="G21" s="379"/>
+      <c r="H21" s="379"/>
+      <c r="I21" s="379"/>
+      <c r="J21" s="379"/>
+      <c r="K21" s="380"/>
       <c r="L21" s="244"/>
     </row>
     <row r="22" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -11645,6 +11673,11 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C10:F10"/>
     <mergeCell ref="E21:K21"/>
     <mergeCell ref="A18:D18"/>
     <mergeCell ref="A17:D17"/>
@@ -11659,12 +11692,13 @@
     <mergeCell ref="A21:D21"/>
     <mergeCell ref="A20:D20"/>
     <mergeCell ref="A19:D19"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C10:F10"/>
   </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Du kan endast mata in siffror mellan 0 och 10. Var noga med punkt eller komma beroende på språk" sqref="L15:L21" xr:uid="{8720CD5A-D7F9-401B-93A9-DA40D5B20AB8}">
+      <formula1>0</formula1>
+      <formula2>10</formula2>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
@@ -11683,7 +11717,7 @@
   <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView showZeros="0" view="pageLayout" topLeftCell="A3" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="L36" sqref="L36"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
@@ -11751,10 +11785,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="11"/>
-      <c r="C5" s="394"/>
-      <c r="D5" s="394"/>
-      <c r="E5" s="394"/>
-      <c r="F5" s="394"/>
+      <c r="C5" s="396"/>
+      <c r="D5" s="396"/>
+      <c r="E5" s="396"/>
+      <c r="F5" s="396"/>
       <c r="H5" s="13"/>
       <c r="I5" s="14" t="s">
         <v>11</v>
@@ -11768,10 +11802,10 @@
         <v>8</v>
       </c>
       <c r="B6" s="11"/>
-      <c r="C6" s="394"/>
-      <c r="D6" s="394"/>
-      <c r="E6" s="394"/>
-      <c r="F6" s="394"/>
+      <c r="C6" s="396"/>
+      <c r="D6" s="396"/>
+      <c r="E6" s="396"/>
+      <c r="F6" s="396"/>
       <c r="K6" s="30"/>
     </row>
     <row r="7" spans="1:12" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -11794,30 +11828,30 @@
         <v>0</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="395"/>
-      <c r="D8" s="395"/>
-      <c r="E8" s="395"/>
-      <c r="F8" s="395"/>
+      <c r="C8" s="397"/>
+      <c r="D8" s="397"/>
+      <c r="E8" s="397"/>
+      <c r="F8" s="397"/>
     </row>
     <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="11"/>
-      <c r="C9" s="394"/>
-      <c r="D9" s="394"/>
-      <c r="E9" s="394"/>
-      <c r="F9" s="394"/>
+      <c r="C9" s="396"/>
+      <c r="D9" s="396"/>
+      <c r="E9" s="396"/>
+      <c r="F9" s="396"/>
     </row>
     <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="11"/>
-      <c r="C10" s="394"/>
-      <c r="D10" s="394"/>
-      <c r="E10" s="394"/>
-      <c r="F10" s="394"/>
+      <c r="C10" s="396"/>
+      <c r="D10" s="396"/>
+      <c r="E10" s="396"/>
+      <c r="F10" s="396"/>
     </row>
     <row r="11" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -11953,13 +11987,13 @@
       <c r="L21" s="245"/>
     </row>
     <row r="22" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="391" t="s">
+      <c r="A22" s="393" t="s">
         <v>177</v>
       </c>
-      <c r="B22" s="392"/>
-      <c r="C22" s="392"/>
-      <c r="D22" s="392"/>
-      <c r="E22" s="393"/>
+      <c r="B22" s="394"/>
+      <c r="C22" s="394"/>
+      <c r="D22" s="394"/>
+      <c r="E22" s="395"/>
       <c r="F22" s="33"/>
       <c r="G22" s="33"/>
       <c r="H22" s="33"/>
@@ -12072,6 +12106,12 @@
     <mergeCell ref="C9:F9"/>
     <mergeCell ref="C10:F10"/>
   </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Du kan endast mata in siffror mellan 0 och 10. Var noga med punkt eller komma beroende på språk" sqref="L15:L22" xr:uid="{C1B275BF-4E20-428B-8A37-03A2CB6C903B}">
+      <formula1>0</formula1>
+      <formula2>10</formula2>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
@@ -12088,7 +12128,7 @@
   <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView showZeros="0" view="pageLayout" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L40" sqref="L40"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
@@ -12155,10 +12195,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="11"/>
-      <c r="C5" s="394"/>
-      <c r="D5" s="394"/>
-      <c r="E5" s="394"/>
-      <c r="F5" s="394"/>
+      <c r="C5" s="396"/>
+      <c r="D5" s="396"/>
+      <c r="E5" s="396"/>
+      <c r="F5" s="396"/>
       <c r="H5" s="13"/>
       <c r="I5" s="14" t="s">
         <v>11</v>
@@ -12172,10 +12212,10 @@
         <v>8</v>
       </c>
       <c r="B6" s="11"/>
-      <c r="C6" s="394"/>
-      <c r="D6" s="394"/>
-      <c r="E6" s="394"/>
-      <c r="F6" s="394"/>
+      <c r="C6" s="396"/>
+      <c r="D6" s="396"/>
+      <c r="E6" s="396"/>
+      <c r="F6" s="396"/>
       <c r="K6" s="30"/>
     </row>
     <row r="7" spans="1:12" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -12198,30 +12238,30 @@
         <v>0</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="395"/>
-      <c r="D8" s="395"/>
-      <c r="E8" s="395"/>
-      <c r="F8" s="395"/>
+      <c r="C8" s="397"/>
+      <c r="D8" s="397"/>
+      <c r="E8" s="397"/>
+      <c r="F8" s="397"/>
     </row>
     <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="11"/>
-      <c r="C9" s="394"/>
-      <c r="D9" s="394"/>
-      <c r="E9" s="394"/>
-      <c r="F9" s="394"/>
+      <c r="C9" s="396"/>
+      <c r="D9" s="396"/>
+      <c r="E9" s="396"/>
+      <c r="F9" s="396"/>
     </row>
     <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="11"/>
-      <c r="C10" s="394"/>
-      <c r="D10" s="394"/>
-      <c r="E10" s="394"/>
-      <c r="F10" s="394"/>
+      <c r="C10" s="396"/>
+      <c r="D10" s="396"/>
+      <c r="E10" s="396"/>
+      <c r="F10" s="396"/>
     </row>
     <row r="11" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -12357,12 +12397,12 @@
       <c r="L21" s="245"/>
     </row>
     <row r="22" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="396" t="s">
+      <c r="A22" s="398" t="s">
         <v>162</v>
       </c>
-      <c r="B22" s="397"/>
-      <c r="C22" s="397"/>
-      <c r="D22" s="398"/>
+      <c r="B22" s="399"/>
+      <c r="C22" s="399"/>
+      <c r="D22" s="400"/>
       <c r="E22" s="33"/>
       <c r="F22" s="33"/>
       <c r="G22" s="33"/>
@@ -12482,6 +12522,12 @@
     <mergeCell ref="C9:F9"/>
     <mergeCell ref="C10:F10"/>
   </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Du kan endast mata in siffror mellan 0 och 10. Var noga med punkt eller komma beroende på språk" sqref="L15:L22" xr:uid="{698590BB-8FFC-45D4-84E2-22CE91EBBCBD}">
+      <formula1>0</formula1>
+      <formula2>10</formula2>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
@@ -12500,7 +12546,7 @@
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView showZeros="0" view="pageLayout" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:L14"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
@@ -12521,14 +12567,14 @@
   <sheetData>
     <row r="1" spans="1:12" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:12" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="399" t="s">
+      <c r="A2" s="407" t="s">
         <v>175</v>
       </c>
-      <c r="B2" s="399"/>
-      <c r="C2" s="399"/>
-      <c r="D2" s="399"/>
-      <c r="E2" s="399"/>
-      <c r="F2" s="399"/>
+      <c r="B2" s="407"/>
+      <c r="C2" s="407"/>
+      <c r="D2" s="407"/>
+      <c r="E2" s="407"/>
+      <c r="F2" s="407"/>
       <c r="H2" s="153"/>
       <c r="I2" s="154" t="s">
         <v>60</v>
@@ -12571,10 +12617,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="134"/>
-      <c r="C5" s="376"/>
-      <c r="D5" s="376"/>
-      <c r="E5" s="376"/>
-      <c r="F5" s="376"/>
+      <c r="C5" s="392"/>
+      <c r="D5" s="392"/>
+      <c r="E5" s="392"/>
+      <c r="F5" s="392"/>
       <c r="H5" s="153"/>
       <c r="I5" s="154" t="s">
         <v>11</v>
@@ -12588,10 +12634,10 @@
         <v>8</v>
       </c>
       <c r="B6" s="134"/>
-      <c r="C6" s="376"/>
-      <c r="D6" s="376"/>
-      <c r="E6" s="376"/>
-      <c r="F6" s="376"/>
+      <c r="C6" s="392"/>
+      <c r="D6" s="392"/>
+      <c r="E6" s="392"/>
+      <c r="F6" s="392"/>
       <c r="K6" s="30"/>
     </row>
     <row r="7" spans="1:12" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -12614,30 +12660,30 @@
         <v>0</v>
       </c>
       <c r="B8" s="158"/>
-      <c r="C8" s="400"/>
-      <c r="D8" s="400"/>
-      <c r="E8" s="400"/>
-      <c r="F8" s="400"/>
+      <c r="C8" s="408"/>
+      <c r="D8" s="408"/>
+      <c r="E8" s="408"/>
+      <c r="F8" s="408"/>
     </row>
     <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="134" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="134"/>
-      <c r="C9" s="376"/>
-      <c r="D9" s="376"/>
-      <c r="E9" s="376"/>
-      <c r="F9" s="376"/>
+      <c r="C9" s="392"/>
+      <c r="D9" s="392"/>
+      <c r="E9" s="392"/>
+      <c r="F9" s="392"/>
     </row>
     <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="134" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="134"/>
-      <c r="C10" s="376"/>
-      <c r="D10" s="376"/>
-      <c r="E10" s="376"/>
-      <c r="F10" s="376"/>
+      <c r="C10" s="392"/>
+      <c r="D10" s="392"/>
+      <c r="E10" s="392"/>
+      <c r="F10" s="392"/>
     </row>
     <row r="11" spans="1:12" ht="33.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -12658,38 +12704,38 @@
 (LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$13,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""))-LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$13,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""),"1","")))*1+(LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$13,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""))-LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$13,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""),"2","")))*2+(LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$13,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""))-LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$13,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""),"3","")))*3+(LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$13,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""))-LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$13,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""),"4","")))*4+(LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$13,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""))-LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$13,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""),"5","")))*5+(LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$13,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""))-LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$13,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""),"6","")))*6+(LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$13,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""))-LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$13,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""),"7","")))*7+(LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$13,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""))-LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$13,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""),"8","")))*8+(LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$13,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""))-LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$13,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""),"9","")))*9</f>
         <v>0</v>
       </c>
-      <c r="L12" s="477">
+      <c r="L12" s="295">
         <f>LEN(A$13)-LEN(SUBSTITUTE(A$13,"R","")) + LEN(A$13)-LEN(SUBSTITUTE(A$13,"D",""))+LEN(A$13)-LEN(SUBSTITUTE(A$13,"S",""))+ LEN(A$13)-LEN(SUBSTITUTE(A$13,"M",""))+LEN(A$13)-LEN(SUBSTITUTE(A$13,"E",""))+LEN(A$13)-LEN(SUBSTITUTE(A$13,"L",""))</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="471"/>
-      <c r="B13" s="472"/>
-      <c r="C13" s="472"/>
-      <c r="D13" s="472"/>
-      <c r="E13" s="472"/>
-      <c r="F13" s="472"/>
-      <c r="G13" s="472"/>
-      <c r="H13" s="472"/>
-      <c r="I13" s="472"/>
-      <c r="J13" s="472"/>
-      <c r="K13" s="472"/>
-      <c r="L13" s="473"/>
+      <c r="A13" s="401"/>
+      <c r="B13" s="402"/>
+      <c r="C13" s="402"/>
+      <c r="D13" s="402"/>
+      <c r="E13" s="402"/>
+      <c r="F13" s="402"/>
+      <c r="G13" s="402"/>
+      <c r="H13" s="402"/>
+      <c r="I13" s="402"/>
+      <c r="J13" s="402"/>
+      <c r="K13" s="402"/>
+      <c r="L13" s="403"/>
     </row>
     <row r="14" spans="1:12" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="474"/>
-      <c r="B14" s="475"/>
-      <c r="C14" s="475"/>
-      <c r="D14" s="475"/>
-      <c r="E14" s="475"/>
-      <c r="F14" s="475"/>
-      <c r="G14" s="475"/>
-      <c r="H14" s="475"/>
-      <c r="I14" s="475"/>
-      <c r="J14" s="475"/>
-      <c r="K14" s="475"/>
-      <c r="L14" s="476"/>
+      <c r="A14" s="404"/>
+      <c r="B14" s="405"/>
+      <c r="C14" s="405"/>
+      <c r="D14" s="405"/>
+      <c r="E14" s="405"/>
+      <c r="F14" s="405"/>
+      <c r="G14" s="405"/>
+      <c r="H14" s="405"/>
+      <c r="I14" s="405"/>
+      <c r="J14" s="405"/>
+      <c r="K14" s="405"/>
+      <c r="L14" s="406"/>
     </row>
     <row r="15" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="166" t="s">
@@ -12877,6 +12923,11 @@
     <mergeCell ref="C9:F9"/>
   </mergeCells>
   <phoneticPr fontId="22" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Du kan endast mata in siffror. Var noga med punkt eller komma beroende på språk" sqref="E15:J15 E26 H26" xr:uid="{7E6B3053-518B-4E89-A0A3-6B2F41762E4D}">
+      <formula1>-1</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
@@ -12894,8 +12945,8 @@
   </sheetPr>
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" view="pageLayout" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:L14"/>
+    <sheetView showZeros="0" view="pageLayout" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
@@ -13547,14 +13598,14 @@
   <sheetData>
     <row r="1" spans="1:12" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:12" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="401" t="s">
+      <c r="A2" s="409" t="s">
         <v>173</v>
       </c>
-      <c r="B2" s="401"/>
-      <c r="C2" s="401"/>
-      <c r="D2" s="401"/>
-      <c r="E2" s="401"/>
-      <c r="F2" s="401"/>
+      <c r="B2" s="409"/>
+      <c r="C2" s="409"/>
+      <c r="D2" s="409"/>
+      <c r="E2" s="409"/>
+      <c r="F2" s="409"/>
       <c r="H2" s="13"/>
       <c r="I2" s="14" t="s">
         <v>60</v>
@@ -13597,10 +13648,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="11"/>
-      <c r="C5" s="394"/>
-      <c r="D5" s="394"/>
-      <c r="E5" s="394"/>
-      <c r="F5" s="394"/>
+      <c r="C5" s="396"/>
+      <c r="D5" s="396"/>
+      <c r="E5" s="396"/>
+      <c r="F5" s="396"/>
       <c r="H5" s="13"/>
       <c r="I5" s="14" t="s">
         <v>11</v>
@@ -13614,10 +13665,10 @@
         <v>8</v>
       </c>
       <c r="B6" s="11"/>
-      <c r="C6" s="394"/>
-      <c r="D6" s="394"/>
-      <c r="E6" s="394"/>
-      <c r="F6" s="394"/>
+      <c r="C6" s="396"/>
+      <c r="D6" s="396"/>
+      <c r="E6" s="396"/>
+      <c r="F6" s="396"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -13646,30 +13697,30 @@
         <v>0</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="395"/>
-      <c r="D8" s="395"/>
-      <c r="E8" s="395"/>
-      <c r="F8" s="395"/>
+      <c r="C8" s="397"/>
+      <c r="D8" s="397"/>
+      <c r="E8" s="397"/>
+      <c r="F8" s="397"/>
     </row>
     <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="11"/>
-      <c r="C9" s="394"/>
-      <c r="D9" s="394"/>
-      <c r="E9" s="394"/>
-      <c r="F9" s="394"/>
+      <c r="C9" s="396"/>
+      <c r="D9" s="396"/>
+      <c r="E9" s="396"/>
+      <c r="F9" s="396"/>
     </row>
     <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="11"/>
-      <c r="C10" s="394"/>
-      <c r="D10" s="394"/>
-      <c r="E10" s="394"/>
-      <c r="F10" s="394"/>
+      <c r="C10" s="396"/>
+      <c r="D10" s="396"/>
+      <c r="E10" s="396"/>
+      <c r="F10" s="396"/>
     </row>
     <row r="11" spans="1:12" ht="51.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -13690,38 +13741,38 @@
 (LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$13,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""))-LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$13,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""),"1","")))*1+(LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$13,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""))-LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$13,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""),"2","")))*2+(LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$13,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""))-LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$13,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""),"3","")))*3+(LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$13,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""))-LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$13,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""),"4","")))*4+(LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$13,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""))-LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$13,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""),"5","")))*5+(LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$13,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""))-LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$13,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""),"6","")))*6+(LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$13,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""))-LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$13,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""),"7","")))*7+(LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$13,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""))-LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$13,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""),"8","")))*8+(LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$13,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""))-LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$13,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""),"9","")))*9</f>
         <v>0</v>
       </c>
-      <c r="L12" s="478">
+      <c r="L12" s="296">
         <f>E22</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="402"/>
-      <c r="B13" s="403"/>
-      <c r="C13" s="403"/>
-      <c r="D13" s="403"/>
-      <c r="E13" s="403"/>
-      <c r="F13" s="403"/>
-      <c r="G13" s="403"/>
-      <c r="H13" s="403"/>
-      <c r="I13" s="403"/>
-      <c r="J13" s="403"/>
-      <c r="K13" s="403"/>
-      <c r="L13" s="404"/>
+      <c r="A13" s="410"/>
+      <c r="B13" s="411"/>
+      <c r="C13" s="411"/>
+      <c r="D13" s="411"/>
+      <c r="E13" s="411"/>
+      <c r="F13" s="411"/>
+      <c r="G13" s="411"/>
+      <c r="H13" s="411"/>
+      <c r="I13" s="411"/>
+      <c r="J13" s="411"/>
+      <c r="K13" s="411"/>
+      <c r="L13" s="412"/>
     </row>
     <row r="14" spans="1:12" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="405"/>
-      <c r="B14" s="406"/>
-      <c r="C14" s="406"/>
-      <c r="D14" s="406"/>
-      <c r="E14" s="406"/>
-      <c r="F14" s="406"/>
-      <c r="G14" s="406"/>
-      <c r="H14" s="406"/>
-      <c r="I14" s="406"/>
-      <c r="J14" s="406"/>
-      <c r="K14" s="406"/>
-      <c r="L14" s="407"/>
+      <c r="A14" s="413"/>
+      <c r="B14" s="414"/>
+      <c r="C14" s="414"/>
+      <c r="D14" s="414"/>
+      <c r="E14" s="414"/>
+      <c r="F14" s="414"/>
+      <c r="G14" s="414"/>
+      <c r="H14" s="414"/>
+      <c r="I14" s="414"/>
+      <c r="J14" s="414"/>
+      <c r="K14" s="414"/>
+      <c r="L14" s="415"/>
     </row>
     <row r="15" spans="1:12" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="32" t="s">
@@ -14019,6 +14070,11 @@
     <mergeCell ref="C9:F9"/>
     <mergeCell ref="C10:F10"/>
   </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Du kan endast mata in siffror. Var noga med punkt eller komma beroende på språk" sqref="E15:J15" xr:uid="{FFCCD7C7-5955-4673-A6B1-C6949F115A08}">
+      <formula1>-1</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
@@ -14037,7 +14093,7 @@
   <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView showZeros="0" view="pageLayout" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:L14"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.4" x14ac:dyDescent="0.3"/>
@@ -14734,10 +14790,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="11"/>
-      <c r="C5" s="394"/>
-      <c r="D5" s="394"/>
-      <c r="E5" s="394"/>
-      <c r="F5" s="394"/>
+      <c r="C5" s="396"/>
+      <c r="D5" s="396"/>
+      <c r="E5" s="396"/>
+      <c r="F5" s="396"/>
       <c r="H5" s="13"/>
       <c r="I5" s="14" t="s">
         <v>11</v>
@@ -14751,10 +14807,10 @@
         <v>8</v>
       </c>
       <c r="B6" s="11"/>
-      <c r="C6" s="394"/>
-      <c r="D6" s="394"/>
-      <c r="E6" s="394"/>
-      <c r="F6" s="394"/>
+      <c r="C6" s="396"/>
+      <c r="D6" s="396"/>
+      <c r="E6" s="396"/>
+      <c r="F6" s="396"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -14783,30 +14839,30 @@
         <v>0</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="395"/>
-      <c r="D8" s="395"/>
-      <c r="E8" s="395"/>
-      <c r="F8" s="395"/>
+      <c r="C8" s="397"/>
+      <c r="D8" s="397"/>
+      <c r="E8" s="397"/>
+      <c r="F8" s="397"/>
     </row>
     <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="11"/>
-      <c r="C9" s="394"/>
-      <c r="D9" s="394"/>
-      <c r="E9" s="394"/>
-      <c r="F9" s="394"/>
+      <c r="C9" s="396"/>
+      <c r="D9" s="396"/>
+      <c r="E9" s="396"/>
+      <c r="F9" s="396"/>
     </row>
     <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="11"/>
-      <c r="C10" s="394"/>
-      <c r="D10" s="394"/>
-      <c r="E10" s="394"/>
-      <c r="F10" s="394"/>
+      <c r="C10" s="396"/>
+      <c r="D10" s="396"/>
+      <c r="E10" s="396"/>
+      <c r="F10" s="396"/>
     </row>
     <row r="11" spans="1:12" ht="51.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -14827,38 +14883,38 @@
 (LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$13,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""))-LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$13,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""),"1","")))*1+(LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$13,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""))-LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$13,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""),"2","")))*2+(LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$13,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""))-LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$13,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""),"3","")))*3+(LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$13,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""))-LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$13,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""),"4","")))*4+(LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$13,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""))-LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$13,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""),"5","")))*5+(LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$13,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""))-LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$13,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""),"6","")))*6+(LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$13,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""))-LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$13,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""),"7","")))*7+(LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$13,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""))-LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$13,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""),"8","")))*8+(LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$13,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""))-LEN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE($A$13,"M",""),"D",""),"E",""),"L",""),"S",""),"R",""),"9","")))*9</f>
         <v>0</v>
       </c>
-      <c r="L12" s="478">
+      <c r="L12" s="296">
         <f>E22</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="402"/>
-      <c r="B13" s="403"/>
-      <c r="C13" s="403"/>
-      <c r="D13" s="403"/>
-      <c r="E13" s="403"/>
-      <c r="F13" s="403"/>
-      <c r="G13" s="403"/>
-      <c r="H13" s="403"/>
-      <c r="I13" s="403"/>
-      <c r="J13" s="403"/>
-      <c r="K13" s="403"/>
-      <c r="L13" s="404"/>
+      <c r="A13" s="410"/>
+      <c r="B13" s="411"/>
+      <c r="C13" s="411"/>
+      <c r="D13" s="411"/>
+      <c r="E13" s="411"/>
+      <c r="F13" s="411"/>
+      <c r="G13" s="411"/>
+      <c r="H13" s="411"/>
+      <c r="I13" s="411"/>
+      <c r="J13" s="411"/>
+      <c r="K13" s="411"/>
+      <c r="L13" s="412"/>
     </row>
     <row r="14" spans="1:12" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="405"/>
-      <c r="B14" s="406"/>
-      <c r="C14" s="406"/>
-      <c r="D14" s="406"/>
-      <c r="E14" s="406"/>
-      <c r="F14" s="406"/>
-      <c r="G14" s="406"/>
-      <c r="H14" s="406"/>
-      <c r="I14" s="406"/>
-      <c r="J14" s="406"/>
-      <c r="K14" s="406"/>
-      <c r="L14" s="407"/>
+      <c r="A14" s="413"/>
+      <c r="B14" s="414"/>
+      <c r="C14" s="414"/>
+      <c r="D14" s="414"/>
+      <c r="E14" s="414"/>
+      <c r="F14" s="414"/>
+      <c r="G14" s="414"/>
+      <c r="H14" s="414"/>
+      <c r="I14" s="414"/>
+      <c r="J14" s="414"/>
+      <c r="K14" s="414"/>
+      <c r="L14" s="415"/>
     </row>
     <row r="15" spans="1:12" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="32" t="s">
@@ -15157,6 +15213,11 @@
     <mergeCell ref="C9:F9"/>
     <mergeCell ref="C6:F6"/>
   </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Du kan endast mata in siffror. Var noga med punkt eller komma beroende på språk" sqref="E15:J15" xr:uid="{FEE4ED4E-A30B-482B-9DB0-D83A270597B2}">
+      <formula1>-1</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
@@ -15174,7 +15235,7 @@
   </sheetPr>
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView showZeros="0" view="pageLayout" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showZeros="0" tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
@@ -15764,14 +15825,14 @@
   <sheetData>
     <row r="1" spans="1:12" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="401" t="s">
+      <c r="A2" s="409" t="s">
         <v>175</v>
       </c>
-      <c r="B2" s="401"/>
-      <c r="C2" s="401"/>
-      <c r="D2" s="401"/>
-      <c r="E2" s="401"/>
-      <c r="F2" s="401"/>
+      <c r="B2" s="409"/>
+      <c r="C2" s="409"/>
+      <c r="D2" s="409"/>
+      <c r="E2" s="409"/>
+      <c r="F2" s="409"/>
       <c r="H2" s="13"/>
       <c r="I2" s="14" t="s">
         <v>60</v>
@@ -15814,10 +15875,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="11"/>
-      <c r="C5" s="394"/>
-      <c r="D5" s="394"/>
-      <c r="E5" s="394"/>
-      <c r="F5" s="394"/>
+      <c r="C5" s="396"/>
+      <c r="D5" s="396"/>
+      <c r="E5" s="396"/>
+      <c r="F5" s="396"/>
       <c r="H5" s="13"/>
       <c r="I5" s="14" t="s">
         <v>11</v>
@@ -15831,10 +15892,10 @@
         <v>8</v>
       </c>
       <c r="B6" s="11"/>
-      <c r="C6" s="394"/>
-      <c r="D6" s="394"/>
-      <c r="E6" s="394"/>
-      <c r="F6" s="394"/>
+      <c r="C6" s="396"/>
+      <c r="D6" s="396"/>
+      <c r="E6" s="396"/>
+      <c r="F6" s="396"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -15863,30 +15924,30 @@
         <v>0</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="395"/>
-      <c r="D8" s="395"/>
-      <c r="E8" s="395"/>
-      <c r="F8" s="395"/>
+      <c r="C8" s="397"/>
+      <c r="D8" s="397"/>
+      <c r="E8" s="397"/>
+      <c r="F8" s="397"/>
     </row>
     <row r="9" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="11"/>
-      <c r="C9" s="394"/>
-      <c r="D9" s="394"/>
-      <c r="E9" s="394"/>
-      <c r="F9" s="394"/>
+      <c r="C9" s="396"/>
+      <c r="D9" s="396"/>
+      <c r="E9" s="396"/>
+      <c r="F9" s="396"/>
     </row>
     <row r="10" spans="1:12" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="11"/>
-      <c r="C10" s="394"/>
-      <c r="D10" s="394"/>
-      <c r="E10" s="394"/>
-      <c r="F10" s="394"/>
+      <c r="C10" s="396"/>
+      <c r="D10" s="396"/>
+      <c r="E10" s="396"/>
+      <c r="F10" s="396"/>
     </row>
     <row r="11" spans="1:12" ht="10.15" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:12" ht="22.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -15900,16 +15961,16 @@
       <c r="A13" s="283" t="s">
         <v>178</v>
       </c>
-      <c r="B13" s="424" t="s">
+      <c r="B13" s="432" t="s">
         <v>179</v>
       </c>
-      <c r="C13" s="425"/>
-      <c r="D13" s="425"/>
-      <c r="E13" s="425"/>
-      <c r="F13" s="425"/>
-      <c r="G13" s="425"/>
-      <c r="H13" s="425"/>
-      <c r="I13" s="426"/>
+      <c r="C13" s="433"/>
+      <c r="D13" s="433"/>
+      <c r="E13" s="433"/>
+      <c r="F13" s="433"/>
+      <c r="G13" s="433"/>
+      <c r="H13" s="433"/>
+      <c r="I13" s="434"/>
       <c r="J13" s="18" t="s">
         <v>180</v>
       </c>
@@ -15920,19 +15981,19 @@
       </c>
     </row>
     <row r="14" spans="1:12" ht="93.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="408" t="s">
+      <c r="A14" s="416" t="s">
         <v>139</v>
       </c>
-      <c r="B14" s="410" t="s">
+      <c r="B14" s="418" t="s">
         <v>181</v>
       </c>
-      <c r="C14" s="411"/>
-      <c r="D14" s="411"/>
-      <c r="E14" s="411"/>
-      <c r="F14" s="411"/>
-      <c r="G14" s="411"/>
-      <c r="H14" s="411"/>
-      <c r="I14" s="412"/>
+      <c r="C14" s="419"/>
+      <c r="D14" s="419"/>
+      <c r="E14" s="419"/>
+      <c r="F14" s="419"/>
+      <c r="G14" s="419"/>
+      <c r="H14" s="419"/>
+      <c r="I14" s="420"/>
       <c r="J14" s="18" t="s">
         <v>192</v>
       </c>
@@ -15943,17 +16004,17 @@
       </c>
     </row>
     <row r="15" spans="1:12" ht="108" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="409"/>
-      <c r="B15" s="413" t="s">
+      <c r="A15" s="417"/>
+      <c r="B15" s="421" t="s">
         <v>189</v>
       </c>
-      <c r="C15" s="414"/>
-      <c r="D15" s="414"/>
-      <c r="E15" s="414"/>
-      <c r="F15" s="414"/>
-      <c r="G15" s="414"/>
-      <c r="H15" s="414"/>
-      <c r="I15" s="415"/>
+      <c r="C15" s="422"/>
+      <c r="D15" s="422"/>
+      <c r="E15" s="422"/>
+      <c r="F15" s="422"/>
+      <c r="G15" s="422"/>
+      <c r="H15" s="422"/>
+      <c r="I15" s="423"/>
       <c r="J15" s="20" t="s">
         <v>193</v>
       </c>
@@ -15964,19 +16025,19 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="416" t="s">
+      <c r="A16" s="424" t="s">
         <v>140</v>
       </c>
-      <c r="B16" s="418" t="s">
+      <c r="B16" s="426" t="s">
         <v>190</v>
       </c>
-      <c r="C16" s="419"/>
-      <c r="D16" s="419"/>
-      <c r="E16" s="419"/>
-      <c r="F16" s="419"/>
-      <c r="G16" s="419"/>
-      <c r="H16" s="419"/>
-      <c r="I16" s="420"/>
+      <c r="C16" s="427"/>
+      <c r="D16" s="427"/>
+      <c r="E16" s="427"/>
+      <c r="F16" s="427"/>
+      <c r="G16" s="427"/>
+      <c r="H16" s="427"/>
+      <c r="I16" s="428"/>
       <c r="J16" s="18" t="s">
         <v>194</v>
       </c>
@@ -15987,17 +16048,17 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="80.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="417"/>
-      <c r="B17" s="421" t="s">
+      <c r="A17" s="425"/>
+      <c r="B17" s="429" t="s">
         <v>191</v>
       </c>
-      <c r="C17" s="422"/>
-      <c r="D17" s="422"/>
-      <c r="E17" s="422"/>
-      <c r="F17" s="422"/>
-      <c r="G17" s="422"/>
-      <c r="H17" s="422"/>
-      <c r="I17" s="423"/>
+      <c r="C17" s="430"/>
+      <c r="D17" s="430"/>
+      <c r="E17" s="430"/>
+      <c r="F17" s="430"/>
+      <c r="G17" s="430"/>
+      <c r="H17" s="430"/>
+      <c r="I17" s="431"/>
       <c r="J17" s="19" t="s">
         <v>195</v>
       </c>
@@ -16020,7 +16081,7 @@
       <c r="J18" s="21"/>
       <c r="K18" s="21"/>
       <c r="L18" s="53">
-        <f>SUM(L14:L17)</f>
+        <f>SUM(L13:L17)</f>
         <v>0</v>
       </c>
       <c r="M18" s="21"/>
@@ -16122,6 +16183,12 @@
     <mergeCell ref="C10:F10"/>
     <mergeCell ref="B13:I13"/>
   </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Endast siffror" error="Du kan endast mata in siffror mellan 0 och 10. Var noga med punkt eller komma beroende på språk" sqref="K13:K17 L20" xr:uid="{7EDD2186-42C8-450A-990E-80224E63AD55}">
+      <formula1>0</formula1>
+      <formula2>10</formula2>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.78740157480314965" right="0.15748031496062992" top="0.98425196850393704" bottom="0.39370078740157483" header="0.43307086614173229" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" scale="97" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
@@ -16143,6 +16210,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100570C130F412EDB4EBF3E80DF6A9149FD" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cfaa3b10b9be17ef9f56bd19dc71004c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ddb0c952b897a810c8a4e377cff6bff8" ns1:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -16208,15 +16284,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF64F18F-372D-43EC-AE22-C51BFB121B01}">
   <ds:schemaRefs>
@@ -16233,6 +16300,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28A807C1-6DB8-4C6A-8DCB-8B5F61EFE299}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A00BD0D-8423-4FFE-92A4-D273D2078383}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -16247,12 +16322,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28A807C1-6DB8-4C6A-8DCB-8B5F61EFE299}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>